<commit_message>
More data points added
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,16 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="133" documentId="8_{5B780008-BDE6-4C40-9CC4-E10D1565D9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{178157E5-2905-4CEC-91A3-2ED6A9B23EC4}"/>
+  <xr:revisionPtr revIDLastSave="290" documentId="8_{5B780008-BDE6-4C40-9CC4-E10D1565D9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70CF6C2B-5AEF-4941-8514-2D1FCF6854EF}"/>
   <bookViews>
     <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
+    <sheet name="Propane-Use" sheetId="1" r:id="rId1"/>
   </sheets>
   <definedNames>
-    <definedName name="_nInt">Sheet1!$H$9</definedName>
-    <definedName name="_nSlope">Sheet1!$G$9</definedName>
+    <definedName name="_nInt">'Propane-Use'!$H$8</definedName>
+    <definedName name="_nSlope">'Propane-Use'!$G$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -37,8 +37,42 @@
 </workbook>
 </file>
 
+<file path=xl/comments1.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mark Biegert</author>
+  </authors>
+  <commentList>
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{EF058726-1A43-4D59-8681-6DCF8A807CA2}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mark Biegert:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I measured the difference between full and empty tanks after filling the tank at my local propane filling station. The amount of propane fill varies by station.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -60,7 +94,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="29" uniqueCount="28">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
   <si>
     <t>FROM:</t>
   </si>
@@ -92,21 +126,12 @@
     <t>Cht Ttl</t>
   </si>
   <si>
-    <t>Propane Use (Lbs) Per Hour</t>
-  </si>
-  <si>
     <t>Xaxis</t>
   </si>
   <si>
-    <t>Time (Hours)</t>
-  </si>
-  <si>
     <t>Yaxis</t>
   </si>
   <si>
-    <t>Tank Weight (Lbs)</t>
-  </si>
-  <si>
     <t>Slope</t>
   </si>
   <si>
@@ -116,9 +141,6 @@
     <t>Empirical Data</t>
   </si>
   <si>
-    <t>Projection</t>
-  </si>
-  <si>
     <t>Graphical Analysis</t>
   </si>
   <si>
@@ -143,7 +165,28 @@
     <t>lbs/day</t>
   </si>
   <si>
-    <t>"20 lb" Propane tank contents</t>
+    <t>Linear Projection</t>
+  </si>
+  <si>
+    <t>Units</t>
+  </si>
+  <si>
+    <t>Tank Weight (lbs)</t>
+  </si>
+  <si>
+    <t>Propane Use Rate (lbs per hour)</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that I started my test with only 5 lbs of propane in </t>
+  </si>
+  <si>
+    <t>the tank. I am assuming the rate of fuel use is independent</t>
+  </si>
+  <si>
+    <t>of the fill level of the tank.</t>
+  </si>
+  <si>
+    <t>Nominal "20 lbs" Propane tank contents</t>
   </si>
 </sst>
 </file>
@@ -151,11 +194,11 @@
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
   <numFmts count="3">
-    <numFmt numFmtId="167" formatCode="0.00;\-0.00;0.00;@"/>
-    <numFmt numFmtId="168" formatCode="0.0;\-0.0;0.0;@"/>
-    <numFmt numFmtId="169" formatCode="0.000;\-0.000;0.000;@"/>
+    <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
+    <numFmt numFmtId="165" formatCode="0.0;\-0.0;0.0;@"/>
+    <numFmt numFmtId="166" formatCode="0.000;\-0.000;0.000;@"/>
   </numFmts>
-  <fonts count="13" x14ac:knownFonts="1">
+  <fonts count="17" x14ac:knownFonts="1">
     <font>
       <sz val="10"/>
       <color theme="1"/>
@@ -255,8 +298,36 @@
       <family val="2"/>
       <scheme val="minor"/>
     </font>
+    <font>
+      <i/>
+      <sz val="10"/>
+      <color rgb="FF7F7F7F"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="10"/>
+      <color rgb="FF3F3F76"/>
+      <name val="Consolas"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
+    <font>
+      <b/>
+      <sz val="9"/>
+      <color indexed="81"/>
+      <name val="Tahoma"/>
+      <family val="2"/>
+    </font>
   </fonts>
-  <fills count="6">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -283,11 +354,23 @@
     </fill>
     <fill>
       <patternFill patternType="solid">
-        <fgColor rgb="FFF2F2F2"/>
+        <fgColor theme="8" tint="0.79995117038483843"/>
+        <bgColor theme="0"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FF99FF99"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
   </fills>
-  <borders count="4">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -314,22 +397,84 @@
       <diagonal/>
     </border>
     <border>
+      <left/>
+      <right style="thin">
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
       <left style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
       </left>
       <right style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color auto="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color auto="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </left>
+      <right style="thin">
+        <color theme="1"/>
       </right>
       <top style="thin">
-        <color rgb="FF3F3F3F"/>
+        <color theme="0" tint="-0.14996795556505021"/>
       </top>
-      <bottom style="thin">
-        <color rgb="FF3F3F3F"/>
+      <bottom style="double">
+        <color auto="1"/>
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </right>
+      <top style="thin">
+        <color theme="0" tint="-0.14996795556505021"/>
+      </top>
+      <bottom style="double">
+        <color auto="1"/>
+      </bottom>
+      <diagonal/>
+    </border>
+    <border>
+      <left/>
+      <right style="thin">
+        <color theme="1"/>
+      </right>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
+    <border>
+      <left style="thin">
+        <color theme="1"/>
+      </left>
+      <right/>
+      <top/>
+      <bottom/>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="15">
+  <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
@@ -344,23 +489,54 @@
     <xf numFmtId="0" fontId="6" fillId="0" borderId="0"/>
     <xf numFmtId="0" fontId="9" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
-    <xf numFmtId="0" fontId="12" fillId="5" borderId="3" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="11">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="167" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="3" fillId="2" borderId="0" xfId="2"/>
     <xf numFmtId="0" fontId="11" fillId="0" borderId="0" xfId="0" applyFont="1"/>
-    <xf numFmtId="168" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="168" fontId="12" fillId="5" borderId="3" xfId="14" applyNumberFormat="1"/>
-    <xf numFmtId="169" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="165" fontId="12" fillId="6" borderId="0" xfId="14" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="3" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="4" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="4" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="6" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="5" fillId="5" borderId="7" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="8" xfId="0" applyBorder="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="12" fillId="6" borderId="0" xfId="14"/>
+    <xf numFmtId="166" fontId="14" fillId="7" borderId="0" xfId="15" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyAlignment="1">
+      <alignment horizontal="center"/>
+    </xf>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
+    <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="16"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
-  <cellStyles count="15">
+  <cellStyles count="17">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
+    <cellStyle name="Explanatory Text" xfId="16" builtinId="53" customBuiltin="1"/>
     <cellStyle name="Followed Hyperlink" xfId="11" builtinId="9" hidden="1"/>
     <cellStyle name="Followed Hyperlink" xfId="13" builtinId="9" customBuiltin="1"/>
     <cellStyle name="Heading 1" xfId="2" builtinId="16" customBuiltin="1"/>
@@ -368,6 +544,7 @@
     <cellStyle name="Heading 3" xfId="4" builtinId="18" hidden="1"/>
     <cellStyle name="Heading 4" xfId="5" builtinId="19" hidden="1"/>
     <cellStyle name="Hyperlink" xfId="12" builtinId="8" customBuiltin="1"/>
+    <cellStyle name="Input" xfId="15" builtinId="20" customBuiltin="1"/>
     <cellStyle name="Intro_Hd" xfId="7" xr:uid="{84D0D410-758D-4384-B224-A500BAF57428}"/>
     <cellStyle name="Intro_Value" xfId="8" xr:uid="{15DF3F31-B3CA-47B9-81DE-6CDBDA24C6D7}"/>
     <cellStyle name="Linked Cell" xfId="10" builtinId="24" customBuiltin="1"/>
@@ -376,12 +553,91 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="9">
+  <dxfs count="14">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
     <dxf>
       <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -476,15 +732,22 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="8"/>
-      <tableStyleElement type="headerRow" dxfId="7"/>
-      <tableStyleElement type="totalRow" dxfId="6"/>
-      <tableStyleElement type="firstColumn" dxfId="5"/>
-      <tableStyleElement type="lastColumn" dxfId="4"/>
-      <tableStyleElement type="firstRowStripe" dxfId="3"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="2"/>
+      <tableStyleElement type="wholeTable" dxfId="13"/>
+      <tableStyleElement type="headerRow" dxfId="12"/>
+      <tableStyleElement type="totalRow" dxfId="11"/>
+      <tableStyleElement type="firstColumn" dxfId="10"/>
+      <tableStyleElement type="lastColumn" dxfId="9"/>
+      <tableStyleElement type="firstRowStripe" dxfId="8"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
     </tableStyle>
   </tableStyles>
+  <colors>
+    <mruColors>
+      <color rgb="FF99FF99"/>
+      <color rgb="FFFDF5E9"/>
+      <color rgb="FFFFFFCC"/>
+    </mruColors>
+  </colors>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
       <x14:slicerStyles defaultSlicerStyle="SlicerStyleLight1"/>
@@ -513,11 +776,11 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>Sheet1!$C$19</c:f>
+          <c:f>'Propane-Use'!$C$27</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Propane Use (Lbs) Per Hour</c:v>
+              <c:v>Propane Use Rate (lbs per hour)</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -597,42 +860,102 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$D$9:$D$12</c:f>
+              <c:f>'Propane-Use'!$C$8:$C$21</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>11.516666666662786</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>13.083333333372138</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>13.933333333348855</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>14.53333333338378</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>14.950000000011642</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>15.733333333453629</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>16.166666666627862</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>16.883333333360497</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>17.383333333418705</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>18.033333333441988</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>18.550000000046566</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>19.766666666662786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$E$9:$E$12</c:f>
+              <c:f>'Propane-Use'!$D$8:$D$21</c:f>
               <c:numCache>
-                <c:formatCode>General</c:formatCode>
-                <c:ptCount val="4"/>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>28.11</c:v>
                 </c:pt>
                 <c:pt idx="1">
+                  <c:v>28.31</c:v>
+                </c:pt>
+                <c:pt idx="2">
                   <c:v>27.95</c:v>
                 </c:pt>
-                <c:pt idx="2">
+                <c:pt idx="3">
                   <c:v>27.82</c:v>
                 </c:pt>
-                <c:pt idx="3">
+                <c:pt idx="4">
                   <c:v>27.64</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>27.7</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>27.68</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>27.8</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>27.69</c:v>
+                </c:pt>
+                <c:pt idx="9" formatCode="General">
+                  <c:v>27.61</c:v>
+                </c:pt>
+                <c:pt idx="10" formatCode="General">
+                  <c:v>27.69</c:v>
+                </c:pt>
+                <c:pt idx="11" formatCode="General">
+                  <c:v>27.68</c:v>
+                </c:pt>
+                <c:pt idx="12" formatCode="General">
+                  <c:v>27.51</c:v>
+                </c:pt>
+                <c:pt idx="13" formatCode="General">
+                  <c:v>27.67</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -649,7 +972,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$L$8</c:f>
+              <c:f>'Propane-Use'!$L$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -672,10 +995,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>Sheet1!$K$9:$K$32</c:f>
+              <c:f>'Propane-Use'!$K$8:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -747,87 +1070,93 @@
                 </c:pt>
                 <c:pt idx="23">
                   <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>Sheet1!$L$9:$L$32</c:f>
+              <c:f>'Propane-Use'!$L$8:$L$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="24"/>
+                <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>28.132562890945234</c:v>
+                  <c:v>28.211433734837208</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.106345289809084</c:v>
+                  <c:v>28.179417960059183</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.080127688672935</c:v>
+                  <c:v>28.147402185281159</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.053910087536785</c:v>
+                  <c:v>28.115386410503135</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.027692486400639</c:v>
+                  <c:v>28.08337063572511</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.001474885264489</c:v>
+                  <c:v>28.051354860947086</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>27.97525728412834</c:v>
+                  <c:v>28.019339086169062</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.94903968299219</c:v>
+                  <c:v>27.987323311391037</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.92282208185604</c:v>
+                  <c:v>27.955307536613013</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.896604480719891</c:v>
+                  <c:v>27.923291761834989</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.870386879583741</c:v>
+                  <c:v>27.891275987056964</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.844169278447591</c:v>
+                  <c:v>27.85926021227894</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.817951677311445</c:v>
+                  <c:v>27.827244437500916</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.791734076175295</c:v>
+                  <c:v>27.795228662722891</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.765516475039146</c:v>
+                  <c:v>27.763212887944867</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.739298873902996</c:v>
+                  <c:v>27.731197113166843</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.713081272766846</c:v>
+                  <c:v>27.699181338388819</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.686863671630697</c:v>
+                  <c:v>27.667165563610794</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>27.660646070494547</c:v>
+                  <c:v>27.63514978883277</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.634428469358401</c:v>
+                  <c:v>27.603134014054742</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27.608210868222251</c:v>
+                  <c:v>27.571118239276718</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27.581993267086101</c:v>
+                  <c:v>27.539102464498693</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27.555775665949952</c:v>
+                  <c:v>27.507086689720669</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>27.529558064813802</c:v>
+                  <c:v>27.475070914942645</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>27.443055140164621</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -854,6 +1183,8 @@
         <c:axId val="1689859120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
+          <c:max val="24"/>
+          <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
         <c:axPos val="b"/>
@@ -874,11 +1205,11 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$20</c:f>
+              <c:f>'Propane-Use'!$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Time (Hours)</c:v>
+                  <c:v>Time (hours)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -917,7 +1248,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="1"/>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -954,6 +1285,8 @@
         <c:crossAx val="1689860784"/>
         <c:crosses val="autoZero"/>
         <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="1"/>
       </c:valAx>
       <c:valAx>
         <c:axId val="1689860784"/>
@@ -980,11 +1313,11 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>Sheet1!$C$21</c:f>
+              <c:f>'Propane-Use'!$C$29</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
-                  <c:v>Tank Weight (Lbs)</c:v>
+                  <c:v>Tank Weight (lbs)</c:v>
                 </c:pt>
               </c:strCache>
             </c:strRef>
@@ -1023,7 +1356,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="0.00" sourceLinked="0"/>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -1674,13 +2007,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>23</xdr:row>
+      <xdr:row>31</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>39</xdr:row>
+      <xdr:row>47</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:graphicFrame macro="">
@@ -1710,14 +2043,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="C8:E12" totalsRowShown="0">
-  <autoFilter ref="C8:E12" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D21" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+  <autoFilter ref="B7:D21" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="1"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="0">
-      <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($C$9,1,1))*24</calculatedColumnFormula>
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="4"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="3">
+      <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="2"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -1909,18 +2242,20 @@
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{FB114D2F-F620-446A-92CE-0CB3C9FD0F74}">
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="R6" sqref="R6"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
+      <selection activeCell="I35" sqref="I35"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
     <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
     <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
     <row r="1" spans="1:12" x14ac:dyDescent="0.2">
@@ -1931,17 +2266,23 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
-      <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
       <c r="B2" s="2" t="s">
-        <v>20</v>
+        <v>16</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="D2" s="2"/>
+      <c r="E2" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
     </row>
     <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
@@ -1952,370 +2293,523 @@
         <v>12-Jul-2023</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="D3" s="2"/>
-    </row>
-    <row r="5" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="H5">
+      <c r="E3" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E4" s="25" t="s">
+        <v>29</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="10">
+        <v>45118.80972222222</v>
+      </c>
+      <c r="C8" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="19">
+        <v>28.11</v>
+      </c>
+      <c r="G8" s="17" cm="1">
+        <f t="array" ref="G8:H8">LINEST(_tTankWeight[Weight (lbs)],_tTankWeight[Time (hours)])</f>
+        <v>-3.2015774778024406E-2</v>
+      </c>
+      <c r="H8" s="17">
+        <v>28.211433734837208</v>
+      </c>
+      <c r="K8" s="14" cm="1">
+        <f t="array" ref="K8:K32">_xlfn.SEQUENCE(25,1,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="15">
+        <f t="shared" ref="L8:L32" si="0">_nInt+_nSlope*K8</f>
+        <v>28.211433734837208</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="10">
+        <v>45118.810416666667</v>
+      </c>
+      <c r="C9" s="11">
+        <v>0</v>
+      </c>
+      <c r="D9" s="19">
         <v>28.31</v>
       </c>
-    </row>
-    <row r="6" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A6" s="6" t="s">
+      <c r="F9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15">
+        <f t="shared" si="0"/>
+        <v>28.179417960059183</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="10">
+        <v>45119.289583333331</v>
+      </c>
+      <c r="C10" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>11.516666666662786</v>
+      </c>
+      <c r="D10" s="19">
+        <v>27.95</v>
+      </c>
+      <c r="K10" s="14">
+        <v>2</v>
+      </c>
+      <c r="L10" s="15">
+        <f t="shared" si="0"/>
+        <v>28.147402185281159</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="10">
+        <v>45119.354861111111</v>
+      </c>
+      <c r="C11" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>13.083333333372138</v>
+      </c>
+      <c r="D11" s="19">
+        <v>27.82</v>
+      </c>
+      <c r="G11" s="4" t="s">
         <v>17</v>
       </c>
-      <c r="J6" s="6" t="s">
+      <c r="K11" s="14">
+        <v>3</v>
+      </c>
+      <c r="L11" s="15">
+        <f t="shared" si="0"/>
+        <v>28.115386410503135</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>45119.390277777777</v>
+      </c>
+      <c r="C12" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>13.933333333348855</v>
+      </c>
+      <c r="D12" s="19">
+        <v>27.64</v>
+      </c>
+      <c r="G12" s="23">
+        <f>ABS(24*_nSlope)</f>
+        <v>0.76837859467258574</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(G12)</f>
+        <v>=ABS(24*_nSlope)</v>
+      </c>
+      <c r="K12" s="14">
+        <v>4</v>
+      </c>
+      <c r="L12" s="15">
+        <f t="shared" si="0"/>
+        <v>28.08337063572511</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="10">
+        <v>45119.415277777778</v>
+      </c>
+      <c r="C13" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>14.53333333338378</v>
+      </c>
+      <c r="D13" s="19">
+        <v>27.7</v>
+      </c>
+      <c r="K13" s="14">
+        <v>5</v>
+      </c>
+      <c r="L13" s="15">
+        <f t="shared" si="0"/>
+        <v>28.051354860947086</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B14" s="10">
+        <v>45119.432638888888</v>
+      </c>
+      <c r="C14" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>14.950000000011642</v>
+      </c>
+      <c r="D14" s="19">
+        <v>27.68</v>
+      </c>
+      <c r="K14" s="14">
+        <v>6</v>
+      </c>
+      <c r="L14" s="15">
+        <f t="shared" si="0"/>
+        <v>28.019339086169062</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B15" s="10">
+        <v>45119.465277777781</v>
+      </c>
+      <c r="C15" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>15.733333333453629</v>
+      </c>
+      <c r="D15" s="19">
+        <v>27.8</v>
+      </c>
+      <c r="F15" s="22">
+        <v>45119.452777777777</v>
+      </c>
+      <c r="K15" s="14">
+        <v>7</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" si="0"/>
+        <v>27.987323311391037</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B16" s="10">
+        <v>45119.48333333333</v>
+      </c>
+      <c r="C16" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>16.166666666627862</v>
+      </c>
+      <c r="D16" s="19">
+        <v>27.69</v>
+      </c>
+      <c r="K16" s="14">
+        <v>8</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="0"/>
+        <v>27.955307536613013</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B17" s="10">
+        <v>45119.513194444444</v>
+      </c>
+      <c r="C17" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>16.883333333360497</v>
+      </c>
+      <c r="D17" s="24">
+        <v>27.61</v>
+      </c>
+      <c r="K17" s="14">
+        <v>9</v>
+      </c>
+      <c r="L17" s="15">
+        <f t="shared" si="0"/>
+        <v>27.923291761834989</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B18" s="10">
+        <v>45119.53402777778</v>
+      </c>
+      <c r="C18" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>17.383333333418705</v>
+      </c>
+      <c r="D18" s="24">
+        <v>27.69</v>
+      </c>
+      <c r="K18" s="14">
+        <v>10</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="0"/>
+        <v>27.891275987056964</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B19" s="10">
+        <v>45119.561111111114</v>
+      </c>
+      <c r="C19" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>18.033333333441988</v>
+      </c>
+      <c r="D19" s="24">
+        <v>27.68</v>
+      </c>
+      <c r="K19" s="14">
+        <v>11</v>
+      </c>
+      <c r="L19" s="15">
+        <f t="shared" si="0"/>
+        <v>27.85926021227894</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B20" s="10">
+        <v>45119.582638888889</v>
+      </c>
+      <c r="C20" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>18.550000000046566</v>
+      </c>
+      <c r="D20" s="24">
+        <v>27.51</v>
+      </c>
+      <c r="K20" s="14">
+        <v>12</v>
+      </c>
+      <c r="L20" s="15">
+        <f t="shared" si="0"/>
+        <v>27.827244437500916</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="10">
+        <v>45119.633333333331</v>
+      </c>
+      <c r="C21" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>19.766666666662786</v>
+      </c>
+      <c r="D21" s="24">
+        <v>27.67</v>
+      </c>
+      <c r="K21" s="14">
+        <v>13</v>
+      </c>
+      <c r="L21" s="15">
+        <f t="shared" si="0"/>
+        <v>27.795228662722891</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="20"/>
+      <c r="C22" s="21"/>
+      <c r="D22" s="26"/>
+      <c r="K22" s="14">
+        <v>14</v>
+      </c>
+      <c r="L22" s="15">
+        <f t="shared" si="0"/>
+        <v>27.763212887944867</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="20"/>
+      <c r="C23" s="21"/>
+      <c r="D23" s="26"/>
+      <c r="K23" s="14">
+        <v>15</v>
+      </c>
+      <c r="L23" s="15">
+        <f t="shared" si="0"/>
+        <v>27.731197113166843</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B24" s="20"/>
+      <c r="C24" s="21"/>
+      <c r="D24" s="26"/>
+      <c r="K24" s="14">
+        <v>16</v>
+      </c>
+      <c r="L24" s="15">
+        <f t="shared" si="0"/>
+        <v>27.699181338388819</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K25" s="14">
+        <v>17</v>
+      </c>
+      <c r="L25" s="15">
+        <f t="shared" si="0"/>
+        <v>27.667165563610794</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="3" t="s">
         <v>18</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C8" t="s">
-        <v>4</v>
-      </c>
-      <c r="D8" t="s">
+      <c r="K26" s="14">
+        <v>18</v>
+      </c>
+      <c r="L26" s="15">
+        <f t="shared" si="0"/>
+        <v>27.63514978883277</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B27" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C27" t="s">
+        <v>26</v>
+      </c>
+      <c r="K27" s="14">
+        <v>19</v>
+      </c>
+      <c r="L27" s="15">
+        <f t="shared" si="0"/>
+        <v>27.603134014054742</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B28" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C28" t="s">
         <v>6</v>
       </c>
-      <c r="E8" t="s">
-        <v>7</v>
-      </c>
-      <c r="G8" s="7" t="s">
-        <v>15</v>
-      </c>
-      <c r="H8" s="7" t="s">
-        <v>16</v>
-      </c>
-      <c r="K8" t="s">
-        <v>4</v>
-      </c>
-      <c r="L8" t="s">
-        <v>5</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C9" s="3">
-        <v>45118.80972222222</v>
-      </c>
-      <c r="D9" s="4">
-        <f>(_tTankWeight[[#This Row],[X]]-INDEX($C$9,1,1))*24</f>
-        <v>0</v>
-      </c>
-      <c r="E9">
-        <v>28.11</v>
-      </c>
-      <c r="G9" s="10" cm="1">
-        <f t="array" ref="G9:H9">LINEST(_tTankWeight[Weight (lbs)],_tTankWeight[Time (hours)])</f>
-        <v>-2.6217601136149207E-2</v>
-      </c>
-      <c r="H9" s="10">
-        <v>28.132562890945234</v>
-      </c>
-      <c r="I9" t="s">
-        <v>8</v>
-      </c>
-      <c r="K9" cm="1">
-        <f t="array" ref="K9:K32">_xlfn.SEQUENCE(24,1,0,1)</f>
-        <v>0</v>
-      </c>
-      <c r="L9" s="5">
-        <f>_nInt+_nSlope*K9</f>
-        <v>28.132562890945234</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C10" s="3">
-        <v>45119.289583333331</v>
-      </c>
-      <c r="D10" s="4">
-        <f>(_tTankWeight[[#This Row],[X]]-INDEX($C$9,1,1))*24</f>
-        <v>11.516666666662786</v>
-      </c>
-      <c r="E10">
-        <v>27.95</v>
-      </c>
-      <c r="K10">
-        <v>1</v>
-      </c>
-      <c r="L10" s="5">
-        <f>_nInt+_nSlope*K10</f>
-        <v>28.106345289809084</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C11" s="3">
-        <v>45119.354861111111</v>
-      </c>
-      <c r="D11" s="4">
-        <f>(_tTankWeight[[#This Row],[X]]-INDEX($C$9,1,1))*24</f>
-        <v>13.083333333372138</v>
-      </c>
-      <c r="E11">
-        <v>27.82</v>
-      </c>
-      <c r="G11" t="s">
+      <c r="E28" t="s">
+        <v>30</v>
+      </c>
+      <c r="H28" s="5">
+        <v>18</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="14">
+        <v>20</v>
+      </c>
+      <c r="L28" s="15">
+        <f t="shared" si="0"/>
+        <v>27.571118239276718</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B29" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C29" t="s">
+        <v>25</v>
+      </c>
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="6">
+        <f>H28/ABS(G12)</f>
+        <v>23.425951900273837</v>
+      </c>
+      <c r="I29" s="16" t="s">
         <v>21</v>
       </c>
-      <c r="K11">
-        <v>2</v>
-      </c>
-      <c r="L11" s="5">
-        <f>_nInt+_nSlope*K11</f>
-        <v>28.080127688672935</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="C12" s="3">
-        <v>45119.390277777777</v>
-      </c>
-      <c r="D12" s="4">
-        <f>(_tTankWeight[[#This Row],[X]]-INDEX($C$9,1,1))*24</f>
-        <v>13.933333333348855</v>
-      </c>
-      <c r="E12">
-        <v>27.64</v>
-      </c>
-      <c r="H12" s="10">
-        <f>24*G9</f>
-        <v>-0.62922242726758093</v>
-      </c>
-      <c r="I12" t="s">
-        <v>26</v>
-      </c>
-      <c r="K12">
-        <v>3</v>
-      </c>
-      <c r="L12" s="5">
-        <f>_nInt+_nSlope*K12</f>
-        <v>28.053910087536785</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K13">
-        <v>4</v>
-      </c>
-      <c r="L13" s="5">
-        <f>_nInt+_nSlope*K13</f>
-        <v>28.027692486400639</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K14">
-        <v>5</v>
-      </c>
-      <c r="L14" s="5">
-        <f>_nInt+_nSlope*K14</f>
-        <v>28.001474885264489</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K15">
-        <v>6</v>
-      </c>
-      <c r="L15" s="5">
-        <f>_nInt+_nSlope*K15</f>
-        <v>27.97525728412834</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K16">
-        <v>7</v>
-      </c>
-      <c r="L16" s="5">
-        <f>_nInt+_nSlope*K16</f>
-        <v>27.94903968299219</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" ht="15" x14ac:dyDescent="0.25">
-      <c r="A17" s="6" t="s">
-        <v>19</v>
-      </c>
-      <c r="E17" s="6" t="s">
+      <c r="K29" s="14">
+        <v>21</v>
+      </c>
+      <c r="L29" s="15">
+        <f t="shared" si="0"/>
+        <v>27.539102464498693</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K30" s="14">
         <v>22</v>
       </c>
-      <c r="K17">
-        <v>8</v>
-      </c>
-      <c r="L17" s="5">
-        <f>_nInt+_nSlope*K17</f>
-        <v>27.92282208185604</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K18">
-        <v>9</v>
-      </c>
-      <c r="L18" s="5">
-        <f>_nInt+_nSlope*K18</f>
-        <v>27.896604480719891</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B19" s="7" t="s">
-        <v>9</v>
-      </c>
-      <c r="C19" t="s">
-        <v>10</v>
-      </c>
-      <c r="E19" t="s">
-        <v>27</v>
-      </c>
-      <c r="H19" s="8">
-        <v>18</v>
-      </c>
-      <c r="I19" t="s">
+      <c r="L30" s="15">
+        <f t="shared" si="0"/>
+        <v>27.507086689720669</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K31" s="14">
         <v>23</v>
       </c>
-      <c r="K19">
-        <v>10</v>
-      </c>
-      <c r="L19" s="5">
-        <f>_nInt+_nSlope*K19</f>
-        <v>27.870386879583741</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B20" s="7" t="s">
-        <v>11</v>
-      </c>
-      <c r="C20" t="s">
-        <v>12</v>
-      </c>
-      <c r="E20" t="s">
+      <c r="L31" s="15">
+        <f t="shared" si="0"/>
+        <v>27.475070914942645</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K32" s="14">
         <v>24</v>
       </c>
-      <c r="H20" s="9">
-        <f>H19/ABS(H12)</f>
-        <v>28.606736219123007</v>
-      </c>
-      <c r="I20" t="s">
-        <v>25</v>
-      </c>
-      <c r="K20">
-        <v>11</v>
-      </c>
-      <c r="L20" s="5">
-        <f>_nInt+_nSlope*K20</f>
-        <v>27.844169278447591</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B21" s="7" t="s">
-        <v>13</v>
-      </c>
-      <c r="C21" t="s">
-        <v>14</v>
-      </c>
-      <c r="K21">
-        <v>12</v>
-      </c>
-      <c r="L21" s="5">
-        <f>_nInt+_nSlope*K21</f>
-        <v>27.817951677311445</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K22">
-        <v>13</v>
-      </c>
-      <c r="L22" s="5">
-        <f>_nInt+_nSlope*K22</f>
-        <v>27.791734076175295</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K23">
-        <v>14</v>
-      </c>
-      <c r="L23" s="5">
-        <f>_nInt+_nSlope*K23</f>
-        <v>27.765516475039146</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K24">
-        <v>15</v>
-      </c>
-      <c r="L24" s="5">
-        <f>_nInt+_nSlope*K24</f>
-        <v>27.739298873902996</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K25">
-        <v>16</v>
-      </c>
-      <c r="L25" s="5">
-        <f>_nInt+_nSlope*K25</f>
-        <v>27.713081272766846</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K26">
-        <v>17</v>
-      </c>
-      <c r="L26" s="5">
-        <f>_nInt+_nSlope*K26</f>
-        <v>27.686863671630697</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K27">
-        <v>18</v>
-      </c>
-      <c r="L27" s="5">
-        <f>_nInt+_nSlope*K27</f>
-        <v>27.660646070494547</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K28">
-        <v>19</v>
-      </c>
-      <c r="L28" s="5">
-        <f>_nInt+_nSlope*K28</f>
-        <v>27.634428469358401</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K29">
-        <v>20</v>
-      </c>
-      <c r="L29" s="5">
-        <f>_nInt+_nSlope*K29</f>
-        <v>27.608210868222251</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K30">
-        <v>21</v>
-      </c>
-      <c r="L30" s="5">
-        <f>_nInt+_nSlope*K30</f>
-        <v>27.581993267086101</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K31">
-        <v>22</v>
-      </c>
-      <c r="L31" s="5">
-        <f>_nInt+_nSlope*K31</f>
-        <v>27.555775665949952</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="K32">
-        <v>23</v>
-      </c>
-      <c r="L32" s="5">
-        <f>_nInt+_nSlope*K32</f>
-        <v>27.529558064813802</v>
+      <c r="L32" s="15">
+        <f t="shared" si="0"/>
+        <v>27.443055140164621</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="K8:L30">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31:L32">
+    <cfRule type="expression" dxfId="0" priority="1">
+      <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
   <pageSetup orientation="portrait" r:id="rId1"/>
   <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
   <tableParts count="1">
-    <tablePart r:id="rId3"/>
+    <tablePart r:id="rId4"/>
   </tableParts>
 </worksheet>
 </file>
</xml_diff>

<commit_message>
Forgot to add one data point.
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -5,12 +5,12 @@
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey Hearing Technologies\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="290" documentId="8_{5B780008-BDE6-4C40-9CC4-E10D1565D9A2}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{70CF6C2B-5AEF-4941-8514-2D1FCF6854EF}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB84CE0-42CF-4908-8C05-04475F6E78F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="2565" yWindow="2565" windowWidth="21600" windowHeight="11205" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use" sheetId="1" r:id="rId1"/>
@@ -555,20 +555,6 @@
   </cellStyles>
   <dxfs count="14">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -638,6 +624,20 @@
         </vertical>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -860,10 +860,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use'!$C$8:$C$21</c:f>
+              <c:f>'Propane-Use'!$C$8:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -905,16 +905,19 @@
                 </c:pt>
                 <c:pt idx="13">
                   <c:v>19.766666666662786</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>20.516666666662786</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use'!$D$8:$D$21</c:f>
+              <c:f>'Propane-Use'!$D$8:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="14"/>
+                <c:ptCount val="15"/>
                 <c:pt idx="0">
                   <c:v>28.11</c:v>
                 </c:pt>
@@ -956,6 +959,9 @@
                 </c:pt>
                 <c:pt idx="13" formatCode="General">
                   <c:v>27.67</c:v>
+                </c:pt>
+                <c:pt idx="14" formatCode="General">
+                  <c:v>27.57</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1084,79 +1090,79 @@
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>28.211433734837208</c:v>
+                  <c:v>28.209872610430022</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>28.179417960059183</c:v>
+                  <c:v>28.178040868395264</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>28.147402185281159</c:v>
+                  <c:v>28.146209126360503</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>28.115386410503135</c:v>
+                  <c:v>28.114377384325746</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>28.08337063572511</c:v>
+                  <c:v>28.082545642290984</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>28.051354860947086</c:v>
+                  <c:v>28.050713900256227</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>28.019339086169062</c:v>
+                  <c:v>28.018882158221469</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>27.987323311391037</c:v>
+                  <c:v>27.987050416186708</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>27.955307536613013</c:v>
+                  <c:v>27.955218674151951</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>27.923291761834989</c:v>
+                  <c:v>27.923386932117193</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>27.891275987056964</c:v>
+                  <c:v>27.891555190082432</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>27.85926021227894</c:v>
+                  <c:v>27.859723448047674</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>27.827244437500916</c:v>
+                  <c:v>27.827891706012913</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>27.795228662722891</c:v>
+                  <c:v>27.796059963978156</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>27.763212887944867</c:v>
+                  <c:v>27.764228221943398</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>27.731197113166843</c:v>
+                  <c:v>27.732396479908637</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>27.699181338388819</c:v>
+                  <c:v>27.700564737873879</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>27.667165563610794</c:v>
+                  <c:v>27.668732995839122</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>27.63514978883277</c:v>
+                  <c:v>27.636901253804361</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>27.603134014054742</c:v>
+                  <c:v>27.605069511769603</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>27.571118239276718</c:v>
+                  <c:v>27.573237769734842</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>27.539102464498693</c:v>
+                  <c:v>27.541406027700084</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>27.507086689720669</c:v>
+                  <c:v>27.509574285665327</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>27.475070914942645</c:v>
+                  <c:v>27.477742543630566</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>27.443055140164621</c:v>
+                  <c:v>27.445910801595808</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2043,14 +2049,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D21" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
-  <autoFilter ref="B7:D21" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="1">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2246,8 +2252,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="I35" sqref="I35"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="H38" activeCellId="1" sqref="I40 H38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2356,10 +2362,10 @@
       </c>
       <c r="G8" s="17" cm="1">
         <f t="array" ref="G8:H8">LINEST(_tTankWeight[Weight (lbs)],_tTankWeight[Time (hours)])</f>
-        <v>-3.2015774778024406E-2</v>
+        <v>-3.1831742034758935E-2</v>
       </c>
       <c r="H8" s="17">
-        <v>28.211433734837208</v>
+        <v>28.209872610430022</v>
       </c>
       <c r="K8" s="14" cm="1">
         <f t="array" ref="K8:K32">_xlfn.SEQUENCE(25,1,0,1)</f>
@@ -2367,7 +2373,7 @@
       </c>
       <c r="L8" s="15">
         <f t="shared" ref="L8:L32" si="0">_nInt+_nSlope*K8</f>
-        <v>28.211433734837208</v>
+        <v>28.209872610430022</v>
       </c>
     </row>
     <row r="9" spans="1:12" x14ac:dyDescent="0.2">
@@ -2394,7 +2400,7 @@
       </c>
       <c r="L9" s="15">
         <f t="shared" si="0"/>
-        <v>28.179417960059183</v>
+        <v>28.178040868395264</v>
       </c>
     </row>
     <row r="10" spans="1:12" x14ac:dyDescent="0.2">
@@ -2413,7 +2419,7 @@
       </c>
       <c r="L10" s="15">
         <f t="shared" si="0"/>
-        <v>28.147402185281159</v>
+        <v>28.146209126360503</v>
       </c>
     </row>
     <row r="11" spans="1:12" x14ac:dyDescent="0.2">
@@ -2435,7 +2441,7 @@
       </c>
       <c r="L11" s="15">
         <f t="shared" si="0"/>
-        <v>28.115386410503135</v>
+        <v>28.114377384325746</v>
       </c>
     </row>
     <row r="12" spans="1:12" x14ac:dyDescent="0.2">
@@ -2451,7 +2457,7 @@
       </c>
       <c r="G12" s="23">
         <f>ABS(24*_nSlope)</f>
-        <v>0.76837859467258574</v>
+        <v>0.76396180883421438</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -2465,7 +2471,7 @@
       </c>
       <c r="L12" s="15">
         <f t="shared" si="0"/>
-        <v>28.08337063572511</v>
+        <v>28.082545642290984</v>
       </c>
     </row>
     <row r="13" spans="1:12" x14ac:dyDescent="0.2">
@@ -2484,7 +2490,7 @@
       </c>
       <c r="L13" s="15">
         <f t="shared" si="0"/>
-        <v>28.051354860947086</v>
+        <v>28.050713900256227</v>
       </c>
     </row>
     <row r="14" spans="1:12" x14ac:dyDescent="0.2">
@@ -2503,7 +2509,7 @@
       </c>
       <c r="L14" s="15">
         <f t="shared" si="0"/>
-        <v>28.019339086169062</v>
+        <v>28.018882158221469</v>
       </c>
     </row>
     <row r="15" spans="1:12" x14ac:dyDescent="0.2">
@@ -2525,7 +2531,7 @@
       </c>
       <c r="L15" s="15">
         <f t="shared" si="0"/>
-        <v>27.987323311391037</v>
+        <v>27.987050416186708</v>
       </c>
     </row>
     <row r="16" spans="1:12" x14ac:dyDescent="0.2">
@@ -2544,7 +2550,7 @@
       </c>
       <c r="L16" s="15">
         <f t="shared" si="0"/>
-        <v>27.955307536613013</v>
+        <v>27.955218674151951</v>
       </c>
     </row>
     <row r="17" spans="1:12" x14ac:dyDescent="0.2">
@@ -2563,7 +2569,7 @@
       </c>
       <c r="L17" s="15">
         <f t="shared" si="0"/>
-        <v>27.923291761834989</v>
+        <v>27.923386932117193</v>
       </c>
     </row>
     <row r="18" spans="1:12" x14ac:dyDescent="0.2">
@@ -2582,7 +2588,7 @@
       </c>
       <c r="L18" s="15">
         <f t="shared" si="0"/>
-        <v>27.891275987056964</v>
+        <v>27.891555190082432</v>
       </c>
     </row>
     <row r="19" spans="1:12" x14ac:dyDescent="0.2">
@@ -2601,7 +2607,7 @@
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>27.85926021227894</v>
+        <v>27.859723448047674</v>
       </c>
     </row>
     <row r="20" spans="1:12" x14ac:dyDescent="0.2">
@@ -2620,7 +2626,7 @@
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>27.827244437500916</v>
+        <v>27.827891706012913</v>
       </c>
     </row>
     <row r="21" spans="1:12" x14ac:dyDescent="0.2">
@@ -2639,19 +2645,26 @@
       </c>
       <c r="L21" s="15">
         <f t="shared" si="0"/>
-        <v>27.795228662722891</v>
+        <v>27.796059963978156</v>
       </c>
     </row>
     <row r="22" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="B22" s="20"/>
-      <c r="C22" s="21"/>
-      <c r="D22" s="26"/>
+      <c r="B22" s="10">
+        <v>45119.664583333331</v>
+      </c>
+      <c r="C22" s="11">
+        <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>20.516666666662786</v>
+      </c>
+      <c r="D22" s="24">
+        <v>27.57</v>
+      </c>
       <c r="K22" s="14">
         <v>14</v>
       </c>
       <c r="L22" s="15">
         <f t="shared" si="0"/>
-        <v>27.763212887944867</v>
+        <v>27.764228221943398</v>
       </c>
     </row>
     <row r="23" spans="1:12" x14ac:dyDescent="0.2">
@@ -2663,7 +2676,7 @@
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>27.731197113166843</v>
+        <v>27.732396479908637</v>
       </c>
     </row>
     <row r="24" spans="1:12" x14ac:dyDescent="0.2">
@@ -2675,7 +2688,7 @@
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>27.699181338388819</v>
+        <v>27.700564737873879</v>
       </c>
     </row>
     <row r="25" spans="1:12" x14ac:dyDescent="0.2">
@@ -2684,7 +2697,7 @@
       </c>
       <c r="L25" s="15">
         <f t="shared" si="0"/>
-        <v>27.667165563610794</v>
+        <v>27.668732995839122</v>
       </c>
     </row>
     <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
@@ -2699,7 +2712,7 @@
       </c>
       <c r="L26" s="15">
         <f t="shared" si="0"/>
-        <v>27.63514978883277</v>
+        <v>27.636901253804361</v>
       </c>
     </row>
     <row r="27" spans="1:12" x14ac:dyDescent="0.2">
@@ -2714,7 +2727,7 @@
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
-        <v>27.603134014054742</v>
+        <v>27.605069511769603</v>
       </c>
     </row>
     <row r="28" spans="1:12" x14ac:dyDescent="0.2">
@@ -2738,7 +2751,7 @@
       </c>
       <c r="L28" s="15">
         <f t="shared" si="0"/>
-        <v>27.571118239276718</v>
+        <v>27.573237769734842</v>
       </c>
     </row>
     <row r="29" spans="1:12" x14ac:dyDescent="0.2">
@@ -2753,7 +2766,7 @@
       </c>
       <c r="H29" s="6">
         <f>H28/ABS(G12)</f>
-        <v>23.425951900273837</v>
+        <v>23.561387221001958</v>
       </c>
       <c r="I29" s="16" t="s">
         <v>21</v>
@@ -2763,7 +2776,7 @@
       </c>
       <c r="L29" s="15">
         <f t="shared" si="0"/>
-        <v>27.539102464498693</v>
+        <v>27.541406027700084</v>
       </c>
     </row>
     <row r="30" spans="1:12" x14ac:dyDescent="0.2">
@@ -2772,7 +2785,7 @@
       </c>
       <c r="L30" s="15">
         <f t="shared" si="0"/>
-        <v>27.507086689720669</v>
+        <v>27.509574285665327</v>
       </c>
     </row>
     <row r="31" spans="1:12" x14ac:dyDescent="0.2">
@@ -2781,7 +2794,7 @@
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
-        <v>27.475070914942645</v>
+        <v>27.477742543630566</v>
       </c>
     </row>
     <row r="32" spans="1:12" x14ac:dyDescent="0.2">
@@ -2790,17 +2803,17 @@
       </c>
       <c r="L32" s="15">
         <f t="shared" si="0"/>
-        <v>27.443055140164621</v>
+        <v>27.445910801595808</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L30">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="6" priority="2">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:L32">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added Day2 Test Data
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,16 +8,19 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey Hearing Technologies\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{FAB84CE0-42CF-4908-8C05-04475F6E78F6}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC32658-FA1B-4044-94B7-430B012FDA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="2565" yWindow="2565" windowWidth="21600" windowHeight="11205" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
-    <sheet name="Propane-Use" sheetId="1" r:id="rId1"/>
+    <sheet name="Propane-Use-Day1" sheetId="1" r:id="rId1"/>
+    <sheet name="Propane-Use-Day2" sheetId="3" r:id="rId2"/>
   </sheets>
   <definedNames>
-    <definedName name="_nInt">'Propane-Use'!$H$8</definedName>
-    <definedName name="_nSlope">'Propane-Use'!$G$8</definedName>
+    <definedName name="_nInt" localSheetId="1">'Propane-Use-Day2'!$H$8</definedName>
+    <definedName name="_nInt">'Propane-Use-Day1'!$H$8</definedName>
+    <definedName name="_nSlope" localSheetId="1">'Propane-Use-Day2'!$G$8</definedName>
+    <definedName name="_nSlope">'Propane-Use-Day1'!$G$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
@@ -71,8 +74,42 @@
 </comments>
 </file>
 
+<file path=xl/comments2.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mark Biegert</author>
+  </authors>
+  <commentList>
+    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{37CA3984-311B-4082-974E-33113DB63516}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mark Biegert:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I measured the difference between full and empty tanks after filling the tank at my local propane filling station. The amount of propane fill varies by station.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -94,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="34" uniqueCount="31">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
   <si>
     <t>FROM:</t>
   </si>
@@ -177,9 +214,6 @@
     <t>Propane Use Rate (lbs per hour)</t>
   </si>
   <si>
-    <t xml:space="preserve">Note that I started my test with only 5 lbs of propane in </t>
-  </si>
-  <si>
     <t>the tank. I am assuming the rate of fuel use is independent</t>
   </si>
   <si>
@@ -187,6 +221,15 @@
   </si>
   <si>
     <t>Nominal "20 lbs" Propane tank contents</t>
+  </si>
+  <si>
+    <t>tare weight</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that I started my test with only 11 lbs of propane in </t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that I started my test with only 7 lbs of propane in </t>
   </si>
 </sst>
 </file>
@@ -553,7 +596,35 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="14">
+  <dxfs count="21">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
@@ -626,18 +697,75 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -732,13 +860,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="13"/>
-      <tableStyleElement type="headerRow" dxfId="12"/>
-      <tableStyleElement type="totalRow" dxfId="11"/>
-      <tableStyleElement type="firstColumn" dxfId="10"/>
-      <tableStyleElement type="lastColumn" dxfId="9"/>
-      <tableStyleElement type="firstRowStripe" dxfId="8"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="7"/>
+      <tableStyleElement type="wholeTable" dxfId="20"/>
+      <tableStyleElement type="headerRow" dxfId="19"/>
+      <tableStyleElement type="totalRow" dxfId="18"/>
+      <tableStyleElement type="firstColumn" dxfId="17"/>
+      <tableStyleElement type="lastColumn" dxfId="16"/>
+      <tableStyleElement type="firstRowStripe" dxfId="15"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="14"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -776,7 +904,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>'Propane-Use'!$C$27</c:f>
+          <c:f>'Propane-Use-Day1'!$C$27</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -860,7 +988,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use'!$C$8:$C$22</c:f>
+              <c:f>'Propane-Use-Day1'!$C$8:$C$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
                 <c:ptCount val="15"/>
@@ -914,7 +1042,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use'!$D$8:$D$22</c:f>
+              <c:f>'Propane-Use-Day1'!$D$8:$D$22</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="15"/>
@@ -978,7 +1106,7 @@
           <c:order val="1"/>
           <c:tx>
             <c:strRef>
-              <c:f>'Propane-Use'!$L$7</c:f>
+              <c:f>'Propane-Use-Day1'!$L$7</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1001,7 +1129,7 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use'!$K$8:$K$32</c:f>
+              <c:f>'Propane-Use-Day1'!$K$8:$K$32</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1085,7 +1213,7 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use'!$L$8:$L$32</c:f>
+              <c:f>'Propane-Use-Day1'!$L$8:$L$32</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="25"/>
@@ -1211,7 +1339,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Propane-Use'!$C$28</c:f>
+              <c:f>'Propane-Use-Day1'!$C$28</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1319,7 +1447,649 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Propane-Use'!$C$29</c:f>
+              <c:f>'Propane-Use-Day1'!$C$29</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tank Weight (lbs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9444444444444445E-2"/>
+              <c:y val="0.25376166520851562"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689859120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart2.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'Propane-Use-Day2'!$C$21</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Propane Use Rate (lbs per hour)</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="6.9347112860892401E-2"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16663888888888889"/>
+          <c:y val="0.16849555263925342"/>
+          <c:w val="0.76843066491688539"/>
+          <c:h val="0.64506926217556138"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Day 2 Rate</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="7030A0"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day2'!$C$8:$C$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.3500000000349246</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0500000000465661</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.6166666667559184</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.683333333407063</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.433333333407063</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day2'!$D$8:$D$13</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="6"/>
+                <c:pt idx="0">
+                  <c:v>24.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.63</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.6</c:v>
+                </c:pt>
+                <c:pt idx="3" formatCode="General">
+                  <c:v>24.58</c:v>
+                </c:pt>
+                <c:pt idx="4" formatCode="General">
+                  <c:v>24.35</c:v>
+                </c:pt>
+                <c:pt idx="5" formatCode="General">
+                  <c:v>24.51</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-3932-45FB-9A3D-27708D390E69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Propane-Use-Day2'!$L$7</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Y</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day2'!$K$8:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day2'!$L$8:$L$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>24.681953470058957</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.638078714008</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.594203957957038</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.550329201906081</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.50645444585512</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.462579689804162</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.418704933753201</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.374830177702243</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.330955421651282</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.287080665600325</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.243205909549363</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.199331153498406</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.155456397447445</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.111581641396487</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.067706885345526</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.023832129294568</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>23.979957373243607</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>23.93608261719265</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>23.892207861141689</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.848333105090731</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.80445834903977</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.760583592988812</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.716708836937855</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.672834080886894</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.628959324835936</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-3932-45FB-9A3D-27708D390E69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1689859120"/>
+        <c:axId val="1689860784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1689859120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="24"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Propane-Use-Day2'!$C$22</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44252077865266842"/>
+              <c:y val="0.90412037037037041"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689860784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1689860784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="25"/>
+          <c:min val="23.5"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Propane-Use-Day2'!$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -1491,7 +2261,563 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -2048,15 +3374,72 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing2.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>31</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>47</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="2" name="Chart 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{6048C808-15CE-4973-83EF-97D9B458B822}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr>
+          <a:graphicFrameLocks/>
+        </xdr:cNvGraphicFramePr>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="10">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="9"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D13" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="B7:D13" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="5">
+      <calculatedColumnFormula>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -2252,8 +3635,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
-      <selection activeCell="H38" activeCellId="1" sqref="I40 H38"/>
+    <sheetView showGridLines="0" workbookViewId="0">
+      <selection activeCell="E8" sqref="E8"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -2272,6 +3655,15 @@
         <v>1</v>
       </c>
       <c r="C1" s="2"/>
+      <c r="E1" t="s">
+        <v>30</v>
+      </c>
+      <c r="F1">
+        <v>17</v>
+      </c>
+      <c r="G1" t="s">
+        <v>19</v>
+      </c>
     </row>
     <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
@@ -2282,7 +3674,7 @@
       </c>
       <c r="C2" s="2"/>
       <c r="E2" s="25" t="s">
-        <v>27</v>
+        <v>31</v>
       </c>
       <c r="F2" s="25"/>
       <c r="G2" s="25"/>
@@ -2300,7 +3692,7 @@
       </c>
       <c r="C3" s="2"/>
       <c r="E3" s="25" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="F3" s="25"/>
       <c r="G3" s="25"/>
@@ -2310,7 +3702,7 @@
     </row>
     <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" s="25" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="F4" s="25"/>
       <c r="G4" s="25"/>
@@ -2738,7 +4130,7 @@
         <v>6</v>
       </c>
       <c r="E28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="H28" s="5">
         <v>18</v>
@@ -2808,12 +4200,494 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L30">
-    <cfRule type="expression" dxfId="6" priority="2">
+    <cfRule type="expression" dxfId="3" priority="2">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:L32">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
+      <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EB25A4-07B8-4BBE-AD53-051224E82545}">
+  <dimension ref="A1:L32"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="E2" s="25" t="s">
+        <v>32</v>
+      </c>
+      <c r="F2" s="25"/>
+      <c r="G2" s="25"/>
+      <c r="H2" s="25"/>
+      <c r="I2" s="25"/>
+      <c r="J2" s="25"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>TEXT(DATE(2023,7,13),"dd-mmm-yyyy")</f>
+        <v>13-Jul-2023</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="E3" s="25" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="25"/>
+      <c r="G3" s="25"/>
+      <c r="H3" s="25"/>
+      <c r="I3" s="25"/>
+      <c r="J3" s="25"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E4" s="25" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="25"/>
+      <c r="G4" s="25"/>
+      <c r="H4" s="25"/>
+      <c r="I4" s="25"/>
+      <c r="J4" s="25"/>
+    </row>
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>5</v>
+      </c>
+    </row>
+    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="10">
+        <v>45120.291666666664</v>
+      </c>
+      <c r="C8" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="19">
+        <v>24.67</v>
+      </c>
+      <c r="G8" s="17" cm="1">
+        <f t="array" ref="G8:H8">LINEST(_tTankWeight2[Weight (lbs)],_tTankWeight2[Time (hours)])</f>
+        <v>-4.3874756050959279E-2</v>
+      </c>
+      <c r="H8" s="17">
+        <v>24.681953470058957</v>
+      </c>
+      <c r="K8" s="14" cm="1">
+        <f t="array" ref="K8:K32">_xlfn.SEQUENCE(25,1,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="15">
+        <f t="shared" ref="L8:L32" si="0">_nInt+_nSlope*K8</f>
+        <v>24.681953470058957</v>
+      </c>
+    </row>
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B9" s="10">
+        <v>45120.347916666666</v>
+      </c>
+      <c r="C9" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>1.3500000000349246</v>
+      </c>
+      <c r="D9" s="19">
+        <v>24.63</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15">
+        <f t="shared" si="0"/>
+        <v>24.638078714008</v>
+      </c>
+    </row>
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B10" s="10">
+        <v>45120.377083333333</v>
+      </c>
+      <c r="C10" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>2.0500000000465661</v>
+      </c>
+      <c r="D10" s="19">
+        <v>24.6</v>
+      </c>
+      <c r="K10" s="14">
+        <v>2</v>
+      </c>
+      <c r="L10" s="15">
+        <f t="shared" si="0"/>
+        <v>24.594203957957038</v>
+      </c>
+    </row>
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B11" s="10">
+        <v>45120.442361111112</v>
+      </c>
+      <c r="C11" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>3.6166666667559184</v>
+      </c>
+      <c r="D11" s="24">
+        <v>24.58</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="14">
+        <v>3</v>
+      </c>
+      <c r="L11" s="15">
+        <f t="shared" si="0"/>
+        <v>24.550329201906081</v>
+      </c>
+    </row>
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>45120.486805555556</v>
+      </c>
+      <c r="C12" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>4.683333333407063</v>
+      </c>
+      <c r="D12" s="24">
+        <v>24.35</v>
+      </c>
+      <c r="G12" s="23">
+        <f>ABS(24*_nSlope)</f>
+        <v>1.0529941452230227</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(G12)</f>
+        <v>=ABS(24*_nSlope)</v>
+      </c>
+      <c r="K12" s="14">
+        <v>4</v>
+      </c>
+      <c r="L12" s="15">
+        <f t="shared" si="0"/>
+        <v>24.50645444585512</v>
+      </c>
+    </row>
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B13" s="10">
+        <v>45120.518055555556</v>
+      </c>
+      <c r="C13" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>5.433333333407063</v>
+      </c>
+      <c r="D13" s="24">
+        <v>24.51</v>
+      </c>
+      <c r="K13" s="14">
+        <v>5</v>
+      </c>
+      <c r="L13" s="15">
+        <f t="shared" si="0"/>
+        <v>24.462579689804162</v>
+      </c>
+    </row>
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K14" s="14">
+        <v>6</v>
+      </c>
+      <c r="L14" s="15">
+        <f t="shared" si="0"/>
+        <v>24.418704933753201</v>
+      </c>
+    </row>
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K15" s="14">
+        <v>7</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" si="0"/>
+        <v>24.374830177702243</v>
+      </c>
+    </row>
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K16" s="14">
+        <v>8</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="0"/>
+        <v>24.330955421651282</v>
+      </c>
+    </row>
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K17" s="14">
+        <v>9</v>
+      </c>
+      <c r="L17" s="15">
+        <f t="shared" si="0"/>
+        <v>24.287080665600325</v>
+      </c>
+    </row>
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K18" s="14">
+        <v>10</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="0"/>
+        <v>24.243205909549363</v>
+      </c>
+    </row>
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K19" s="14">
+        <v>11</v>
+      </c>
+      <c r="L19" s="15">
+        <f t="shared" si="0"/>
+        <v>24.199331153498406</v>
+      </c>
+    </row>
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K20" s="14">
+        <v>12</v>
+      </c>
+      <c r="L20" s="15">
+        <f t="shared" si="0"/>
+        <v>24.155456397447445</v>
+      </c>
+    </row>
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B21" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C21" t="s">
+        <v>26</v>
+      </c>
+      <c r="K21" s="14">
+        <v>13</v>
+      </c>
+      <c r="L21" s="15">
+        <f t="shared" si="0"/>
+        <v>24.111581641396487</v>
+      </c>
+    </row>
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B22" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C22" t="s">
+        <v>6</v>
+      </c>
+      <c r="K22" s="14">
+        <v>14</v>
+      </c>
+      <c r="L22" s="15">
+        <f t="shared" si="0"/>
+        <v>24.067706885345526</v>
+      </c>
+    </row>
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
+      <c r="F23" s="22"/>
+      <c r="K23" s="14">
+        <v>15</v>
+      </c>
+      <c r="L23" s="15">
+        <f t="shared" si="0"/>
+        <v>24.023832129294568</v>
+      </c>
+    </row>
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K24" s="14">
+        <v>16</v>
+      </c>
+      <c r="L24" s="15">
+        <f t="shared" si="0"/>
+        <v>23.979957373243607</v>
+      </c>
+    </row>
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K25" s="14">
+        <v>17</v>
+      </c>
+      <c r="L25" s="15">
+        <f t="shared" si="0"/>
+        <v>23.93608261719265</v>
+      </c>
+    </row>
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="A26" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E26" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K26" s="14">
+        <v>18</v>
+      </c>
+      <c r="L26" s="15">
+        <f t="shared" si="0"/>
+        <v>23.892207861141689</v>
+      </c>
+    </row>
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K27" s="14">
+        <v>19</v>
+      </c>
+      <c r="L27" s="15">
+        <f t="shared" si="0"/>
+        <v>23.848333105090731</v>
+      </c>
+    </row>
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E28" t="s">
+        <v>29</v>
+      </c>
+      <c r="H28" s="5">
+        <v>18</v>
+      </c>
+      <c r="I28" t="s">
+        <v>19</v>
+      </c>
+      <c r="K28" s="14">
+        <v>20</v>
+      </c>
+      <c r="L28" s="15">
+        <f t="shared" si="0"/>
+        <v>23.80445834903977</v>
+      </c>
+    </row>
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="E29" t="s">
+        <v>20</v>
+      </c>
+      <c r="H29" s="6">
+        <f>H28/ABS(G12)</f>
+        <v>17.094112138854889</v>
+      </c>
+      <c r="I29" s="16" t="s">
+        <v>21</v>
+      </c>
+      <c r="K29" s="14">
+        <v>21</v>
+      </c>
+      <c r="L29" s="15">
+        <f t="shared" si="0"/>
+        <v>23.760583592988812</v>
+      </c>
+    </row>
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K30" s="14">
+        <v>22</v>
+      </c>
+      <c r="L30" s="15">
+        <f t="shared" si="0"/>
+        <v>23.716708836937855</v>
+      </c>
+    </row>
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K31" s="14">
+        <v>23</v>
+      </c>
+      <c r="L31" s="15">
+        <f t="shared" si="0"/>
+        <v>23.672834080886894</v>
+      </c>
+    </row>
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="K32" s="14">
+        <v>24</v>
+      </c>
+      <c r="L32" s="15">
+        <f t="shared" si="0"/>
+        <v>23.628959324835936</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K8:L30">
+    <cfRule type="expression" dxfId="1" priority="2">
+      <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31:L32">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Added another data point
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\biegertm\OneDrive - Starkey Hearing Technologies\Downloads\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5CC32658-FA1B-4044-94B7-430B012FDA9F}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A89EF07A-0062-4B00-9C61-6FA25FF7B53A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="70" uniqueCount="33">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
   <si>
     <t>FROM:</t>
   </si>
@@ -230,6 +230,15 @@
   </si>
   <si>
     <t xml:space="preserve">Note that I started my test with only 7 lbs of propane in </t>
+  </si>
+  <si>
+    <t>Yexpected</t>
+  </si>
+  <si>
+    <t>Expected Use</t>
+  </si>
+  <si>
+    <t>Propane Rate of Use (lbs per hour)</t>
   </si>
 </sst>
 </file>
@@ -596,13 +605,77 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="21">
+  <dxfs count="22">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -697,75 +770,18 @@
       </border>
     </dxf>
     <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right/>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
-      <numFmt numFmtId="2" formatCode="0.00"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
-    </dxf>
-    <dxf>
-      <border diagonalUp="0" diagonalDown="0">
-        <left/>
-        <right/>
-        <top/>
-        <bottom/>
-      </border>
-    </dxf>
-    <dxf>
-      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
-      <border diagonalUp="0" diagonalDown="0">
-        <left style="thin">
-          <color auto="1"/>
-        </left>
-        <right style="thin">
-          <color auto="1"/>
-        </right>
-        <top/>
-        <bottom/>
-        <vertical style="thin">
-          <color auto="1"/>
-        </vertical>
-        <horizontal/>
-      </border>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -860,13 +876,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="20"/>
-      <tableStyleElement type="headerRow" dxfId="19"/>
-      <tableStyleElement type="totalRow" dxfId="18"/>
-      <tableStyleElement type="firstColumn" dxfId="17"/>
-      <tableStyleElement type="lastColumn" dxfId="16"/>
-      <tableStyleElement type="firstRowStripe" dxfId="15"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="14"/>
+      <tableStyleElement type="wholeTable" dxfId="21"/>
+      <tableStyleElement type="headerRow" dxfId="20"/>
+      <tableStyleElement type="totalRow" dxfId="19"/>
+      <tableStyleElement type="firstColumn" dxfId="18"/>
+      <tableStyleElement type="lastColumn" dxfId="17"/>
+      <tableStyleElement type="firstRowStripe" dxfId="16"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="15"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1600,7 +1616,7 @@
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
-              <c:v>Propane Use Rate (lbs per hour)</c:v>
+              <c:v>Propane Rate of Use (lbs per hour)</c:v>
             </c:pt>
           </c:strCache>
         </c:strRef>
@@ -1659,7 +1675,7 @@
           <c:idx val="0"/>
           <c:order val="0"/>
           <c:tx>
-            <c:v>Day 2 Rate</c:v>
+            <c:v>Measurements</c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="28575" cap="rnd">
@@ -1673,7 +1689,7 @@
             <c:size val="10"/>
             <c:spPr>
               <a:solidFill>
-                <a:srgbClr val="7030A0"/>
+                <a:srgbClr val="FF0000"/>
               </a:solidFill>
               <a:ln w="9525">
                 <a:noFill/>
@@ -1683,10 +1699,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$C$8:$C$13</c:f>
+              <c:f>'Propane-Use-Day2'!$C$8:$C$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1704,16 +1720,22 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>5.433333333407063</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>5.9833333334536292</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7.7666666666627862</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$D$8:$D$13</c:f>
+              <c:f>'Propane-Use-Day2'!$D$8:$D$15</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>24.67</c:v>
                 </c:pt>
@@ -1731,6 +1753,12 @@
                 </c:pt>
                 <c:pt idx="5" formatCode="General">
                   <c:v>24.51</c:v>
+                </c:pt>
+                <c:pt idx="6" formatCode="General">
+                  <c:v>24.55</c:v>
+                </c:pt>
+                <c:pt idx="7" formatCode="General">
+                  <c:v>24.42</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1746,15 +1774,7 @@
           <c:idx val="1"/>
           <c:order val="1"/>
           <c:tx>
-            <c:strRef>
-              <c:f>'Propane-Use-Day2'!$L$7</c:f>
-              <c:strCache>
-                <c:ptCount val="1"/>
-                <c:pt idx="0">
-                  <c:v>Y</c:v>
-                </c:pt>
-              </c:strCache>
-            </c:strRef>
+            <c:v>Curve Fit </c:v>
           </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
@@ -1859,79 +1879,79 @@
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="25"/>
                 <c:pt idx="0">
-                  <c:v>24.681953470058957</c:v>
+                  <c:v>24.660538200123117</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>24.638078714008</c:v>
+                  <c:v>24.628990258375534</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>24.594203957957038</c:v>
+                  <c:v>24.597442316627948</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>24.550329201906081</c:v>
+                  <c:v>24.565894374880365</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24.50645444585512</c:v>
+                  <c:v>24.534346433132782</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>24.462579689804162</c:v>
+                  <c:v>24.502798491385196</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>24.418704933753201</c:v>
+                  <c:v>24.471250549637613</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>24.374830177702243</c:v>
+                  <c:v>24.43970260789003</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>24.330955421651282</c:v>
+                  <c:v>24.408154666142444</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>24.287080665600325</c:v>
+                  <c:v>24.376606724394861</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>24.243205909549363</c:v>
+                  <c:v>24.345058782647278</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>24.199331153498406</c:v>
+                  <c:v>24.313510840899692</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>24.155456397447445</c:v>
+                  <c:v>24.281962899152109</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>24.111581641396487</c:v>
+                  <c:v>24.250414957404526</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>24.067706885345526</c:v>
+                  <c:v>24.21886701565694</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>24.023832129294568</c:v>
+                  <c:v>24.187319073909357</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>23.979957373243607</c:v>
+                  <c:v>24.155771132161775</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>23.93608261719265</c:v>
+                  <c:v>24.124223190414188</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>23.892207861141689</c:v>
+                  <c:v>24.092675248666605</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>23.848333105090731</c:v>
+                  <c:v>24.061127306919023</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>23.80445834903977</c:v>
+                  <c:v>24.029579365171436</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>23.760583592988812</c:v>
+                  <c:v>23.998031423423853</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>23.716708836937855</c:v>
+                  <c:v>23.966483481676271</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23.672834080886894</c:v>
+                  <c:v>23.934935539928684</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>23.628959324835936</c:v>
+                  <c:v>23.903387598181101</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -1940,6 +1960,199 @@
           <c:extLst>
             <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
               <c16:uniqueId val="{00000001-3932-45FB-9A3D-27708D390E69}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Specification</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day2'!$K$8:$K$32</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>24</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day2'!$M$8:$M$32</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="25"/>
+                <c:pt idx="0">
+                  <c:v>24.67</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>24.634285714285717</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>24.598571428571429</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>24.562857142857144</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>24.527142857142859</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>24.491428571428575</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>24.455714285714286</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>24.42</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>24.384285714285717</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>24.348571428571429</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>24.312857142857144</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>24.277142857142859</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>24.241428571428575</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>24.205714285714286</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>24.17</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>24.134285714285717</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>24.098571428571429</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>24.062857142857144</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>24.027142857142859</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>23.991428571428575</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>23.955714285714286</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>23.92</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>23.884285714285717</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23.848571428571429</c:v>
+                </c:pt>
+                <c:pt idx="24">
+                  <c:v>23.812857142857144</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-A096-47BF-82E9-C2C867EAAF4B}"/>
             </c:ext>
           </c:extLst>
         </c:ser>
@@ -2067,7 +2280,7 @@
         <c:axId val="1689860784"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="25"/>
+          <c:max val="25.1"/>
           <c:min val="23.5"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -2178,6 +2391,46 @@
         <a:effectLst/>
       </c:spPr>
     </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.67814879906268299"/>
+          <c:y val="0.23169291338582676"/>
+          <c:w val="0.2210896309314587"/>
+          <c:h val="0.22825787401574804"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
     <c:plotVisOnly val="1"/>
     <c:dispBlanksAs val="gap"/>
     <c:extLst>
@@ -3418,28 +3671,28 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="12" tableBorderDxfId="11">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="11"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="10">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="10"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="9">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="9"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="8"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D13" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
-  <autoFilter ref="B7:D13" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D15" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B7:D15" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="6"/>
-    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="5">
+    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="1">
       <calculatedColumnFormula>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="4"/>
+    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -3635,8 +3888,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="E8" sqref="E8"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="H39" sqref="H39"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4200,12 +4453,12 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L30">
-    <cfRule type="expression" dxfId="3" priority="2">
+    <cfRule type="expression" dxfId="14" priority="2">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:L32">
-    <cfRule type="expression" dxfId="2" priority="1">
+    <cfRule type="expression" dxfId="13" priority="1">
       <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4221,10 +4474,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EB25A4-07B8-4BBE-AD53-051224E82545}">
-  <dimension ref="A1:L32"/>
+  <dimension ref="A1:M32"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
-      <selection activeCell="P18" sqref="P18"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="C8" sqref="C8:C15"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -4235,7 +4488,7 @@
     <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4244,7 +4497,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4261,7 +4514,7 @@
       <c r="I2" s="25"/>
       <c r="J2" s="25"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4279,7 +4532,7 @@
       <c r="I3" s="25"/>
       <c r="J3" s="25"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E4" s="25" t="s">
         <v>28</v>
       </c>
@@ -4289,7 +4542,7 @@
       <c r="I4" s="25"/>
       <c r="J4" s="25"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4297,7 +4550,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -4319,8 +4572,11 @@
       <c r="L7" s="13" t="s">
         <v>5</v>
       </c>
-    </row>
-    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="M7" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B8" s="10">
         <v>45120.291666666664</v>
       </c>
@@ -4333,10 +4589,10 @@
       </c>
       <c r="G8" s="17" cm="1">
         <f t="array" ref="G8:H8">LINEST(_tTankWeight2[Weight (lbs)],_tTankWeight2[Time (hours)])</f>
-        <v>-4.3874756050959279E-2</v>
+        <v>-3.1547941747583984E-2</v>
       </c>
       <c r="H8" s="17">
-        <v>24.681953470058957</v>
+        <v>24.660538200123117</v>
       </c>
       <c r="K8" s="14" cm="1">
         <f t="array" ref="K8:K32">_xlfn.SEQUENCE(25,1,0,1)</f>
@@ -4344,10 +4600,14 @@
       </c>
       <c r="L8" s="15">
         <f t="shared" ref="L8:L32" si="0">_nInt+_nSlope*K8</f>
-        <v>24.681953470058957</v>
-      </c>
-    </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.660538200123117</v>
+      </c>
+      <c r="M8" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K8</f>
+        <v>24.67</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="10">
         <v>45120.347916666666</v>
       </c>
@@ -4372,10 +4632,14 @@
       </c>
       <c r="L9" s="15">
         <f t="shared" si="0"/>
-        <v>24.638078714008</v>
-      </c>
-    </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.628990258375534</v>
+      </c>
+      <c r="M9" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K9</f>
+        <v>24.634285714285717</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="10">
         <v>45120.377083333333</v>
       </c>
@@ -4391,10 +4655,14 @@
       </c>
       <c r="L10" s="15">
         <f t="shared" si="0"/>
-        <v>24.594203957957038</v>
-      </c>
-    </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.597442316627948</v>
+      </c>
+      <c r="M10" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K10</f>
+        <v>24.598571428571429</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>45120.442361111112</v>
       </c>
@@ -4413,10 +4681,14 @@
       </c>
       <c r="L11" s="15">
         <f t="shared" si="0"/>
-        <v>24.550329201906081</v>
-      </c>
-    </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.565894374880365</v>
+      </c>
+      <c r="M11" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K11</f>
+        <v>24.562857142857144</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="10">
         <v>45120.486805555556</v>
       </c>
@@ -4429,7 +4701,7 @@
       </c>
       <c r="G12" s="23">
         <f>ABS(24*_nSlope)</f>
-        <v>1.0529941452230227</v>
+        <v>0.75715060194201556</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -4443,10 +4715,14 @@
       </c>
       <c r="L12" s="15">
         <f t="shared" si="0"/>
-        <v>24.50645444585512</v>
-      </c>
-    </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.534346433132782</v>
+      </c>
+      <c r="M12" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K12</f>
+        <v>24.527142857142859</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="10">
         <v>45120.518055555556</v>
       </c>
@@ -4462,88 +4738,155 @@
       </c>
       <c r="L13" s="15">
         <f t="shared" si="0"/>
-        <v>24.462579689804162</v>
-      </c>
-    </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.502798491385196</v>
+      </c>
+      <c r="M13" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K13</f>
+        <v>24.491428571428575</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="10">
+        <v>45120.540972222225</v>
+      </c>
+      <c r="C14" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>5.9833333334536292</v>
+      </c>
+      <c r="D14" s="24">
+        <v>24.55</v>
+      </c>
       <c r="K14" s="14">
         <v>6</v>
       </c>
       <c r="L14" s="15">
         <f t="shared" si="0"/>
-        <v>24.418704933753201</v>
-      </c>
-    </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.471250549637613</v>
+      </c>
+      <c r="M14" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K14</f>
+        <v>24.455714285714286</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B15" s="10">
+        <v>45120.615277777775</v>
+      </c>
+      <c r="C15" s="11">
+        <f>(_tTankWeight2[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
+        <v>7.7666666666627862</v>
+      </c>
+      <c r="D15" s="24">
+        <v>24.42</v>
+      </c>
+      <c r="G15" s="4" t="s">
+        <v>34</v>
+      </c>
       <c r="K15" s="14">
         <v>7</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" si="0"/>
-        <v>24.374830177702243</v>
-      </c>
-    </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.43970260789003</v>
+      </c>
+      <c r="M15" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K15</f>
+        <v>24.42</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G16" s="23">
+        <f>H28/21</f>
+        <v>0.8571428571428571</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
       <c r="K16" s="14">
         <v>8</v>
       </c>
       <c r="L16" s="15">
         <f t="shared" si="0"/>
-        <v>24.330955421651282</v>
-      </c>
-    </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.408154666142444</v>
+      </c>
+      <c r="M16" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K16</f>
+        <v>24.384285714285717</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G17" s="23"/>
       <c r="K17" s="14">
         <v>9</v>
       </c>
       <c r="L17" s="15">
         <f t="shared" si="0"/>
-        <v>24.287080665600325</v>
-      </c>
-    </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.376606724394861</v>
+      </c>
+      <c r="M17" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K17</f>
+        <v>24.348571428571429</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K18" s="14">
         <v>10</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="0"/>
-        <v>24.243205909549363</v>
-      </c>
-    </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.345058782647278</v>
+      </c>
+      <c r="M18" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K18</f>
+        <v>24.312857142857144</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K19" s="14">
         <v>11</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>24.199331153498406</v>
-      </c>
-    </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.313510840899692</v>
+      </c>
+      <c r="M19" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K19</f>
+        <v>24.277142857142859</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K20" s="14">
         <v>12</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>24.155456397447445</v>
-      </c>
-    </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.281962899152109</v>
+      </c>
+      <c r="M20" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K20</f>
+        <v>24.241428571428575</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>26</v>
+        <v>35</v>
       </c>
       <c r="K21" s="14">
         <v>13</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="0"/>
-        <v>24.111581641396487</v>
-      </c>
-    </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.250414957404526</v>
+      </c>
+      <c r="M21" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K21</f>
+        <v>24.205714285714286</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
@@ -4555,10 +4898,14 @@
       </c>
       <c r="L22" s="15">
         <f t="shared" si="0"/>
-        <v>24.067706885345526</v>
-      </c>
-    </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.21886701565694</v>
+      </c>
+      <c r="M22" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K22</f>
+        <v>24.17</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
@@ -4571,28 +4918,40 @@
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>24.023832129294568</v>
-      </c>
-    </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.187319073909357</v>
+      </c>
+      <c r="M23" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K23</f>
+        <v>24.134285714285717</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K24" s="14">
         <v>16</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>23.979957373243607</v>
-      </c>
-    </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.155771132161775</v>
+      </c>
+      <c r="M24" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K24</f>
+        <v>24.098571428571429</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K25" s="14">
         <v>17</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="0"/>
-        <v>23.93608261719265</v>
-      </c>
-    </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+        <v>24.124223190414188</v>
+      </c>
+      <c r="M25" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K25</f>
+        <v>24.062857142857144</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -4604,19 +4963,27 @@
       </c>
       <c r="L26" s="15">
         <f t="shared" si="0"/>
-        <v>23.892207861141689</v>
-      </c>
-    </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.092675248666605</v>
+      </c>
+      <c r="M26" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K26</f>
+        <v>24.027142857142859</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K27" s="14">
         <v>19</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
-        <v>23.848333105090731</v>
-      </c>
-    </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.061127306919023</v>
+      </c>
+      <c r="M27" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K27</f>
+        <v>23.991428571428575</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E28" t="s">
         <v>29</v>
       </c>
@@ -4631,16 +4998,20 @@
       </c>
       <c r="L28" s="15">
         <f t="shared" si="0"/>
-        <v>23.80445834903977</v>
-      </c>
-    </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+        <v>24.029579365171436</v>
+      </c>
+      <c r="M28" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K28</f>
+        <v>23.955714285714286</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>20</v>
       </c>
       <c r="H29" s="6">
         <f>H28/ABS(G12)</f>
-        <v>17.094112138854889</v>
+        <v>23.773341728622814</v>
       </c>
       <c r="I29" s="16" t="s">
         <v>21</v>
@@ -4650,45 +5021,66 @@
       </c>
       <c r="L29" s="15">
         <f t="shared" si="0"/>
-        <v>23.760583592988812</v>
-      </c>
-    </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+        <v>23.998031423423853</v>
+      </c>
+      <c r="M29" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K29</f>
+        <v>23.92</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K30" s="14">
         <v>22</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="0"/>
-        <v>23.716708836937855</v>
-      </c>
-    </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+        <v>23.966483481676271</v>
+      </c>
+      <c r="M30" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K30</f>
+        <v>23.884285714285717</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K31" s="14">
         <v>23</v>
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
-        <v>23.672834080886894</v>
-      </c>
-    </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+        <v>23.934935539928684</v>
+      </c>
+      <c r="M31" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K31</f>
+        <v>23.848571428571429</v>
+      </c>
+    </row>
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K32" s="14">
         <v>24</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" si="0"/>
-        <v>23.628959324835936</v>
+        <v>23.903387598181101</v>
+      </c>
+      <c r="M32" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K32</f>
+        <v>23.812857142857144</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L30">
-    <cfRule type="expression" dxfId="1" priority="2">
+    <cfRule type="expression" dxfId="7" priority="4">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <conditionalFormatting sqref="K31:L32">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="6" priority="3">
       <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="M8:M32">
+    <cfRule type="expression" dxfId="5" priority="2">
+      <formula>MOD(ROW(M8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Integrated changes from home and cabin
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="48" documentId="8_{AD3A0508-E467-47A3-A7B9-5A12E75B114D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{4E7C2585-D677-4119-936F-9D2DF5AF6C5E}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF6AE12-FFE9-448A-9796-FABF3514EDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-26970" yWindow="1830" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -545,7 +545,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="25">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -578,13 +578,11 @@
       <alignment horizontal="center"/>
     </xf>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
-    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="16"/>
-    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -605,7 +603,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="24">
+  <dxfs count="19">
     <dxf>
       <fill>
         <patternFill>
@@ -652,7 +650,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -692,27 +690,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -744,7 +721,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -782,20 +759,6 @@
         </vertical>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -890,13 +853,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="23"/>
-      <tableStyleElement type="headerRow" dxfId="22"/>
-      <tableStyleElement type="totalRow" dxfId="21"/>
-      <tableStyleElement type="firstColumn" dxfId="20"/>
-      <tableStyleElement type="lastColumn" dxfId="19"/>
-      <tableStyleElement type="firstRowStripe" dxfId="18"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="17"/>
+      <tableStyleElement type="wholeTable" dxfId="18"/>
+      <tableStyleElement type="headerRow" dxfId="17"/>
+      <tableStyleElement type="totalRow" dxfId="16"/>
+      <tableStyleElement type="firstColumn" dxfId="15"/>
+      <tableStyleElement type="lastColumn" dxfId="14"/>
+      <tableStyleElement type="firstRowStripe" dxfId="13"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1805,9 +1768,6 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
-          <c:tx>
-            <c:v>Curve Fit</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
@@ -1822,10 +1782,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$K$8:$K$37</c:f>
+              <c:f>'Propane-Use-Day2'!$K$8:$K$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1915,16 +1875,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$L$8:$L$37</c:f>
+              <c:f>'Propane-Use-Day2'!$L$8:$L$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>24.675384823451715</c:v>
                 </c:pt>
@@ -2014,6 +1977,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>23.826987410838306</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>23.797732327644738</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -2028,9 +1994,6 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
-          <c:tx>
-            <c:v>Specification</c:v>
-          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
@@ -2045,10 +2008,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$K$8:$K$37</c:f>
+              <c:f>'Propane-Use-Day2'!$K$8:$K$38</c:f>
               <c:numCache>
                 <c:formatCode>General</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -2138,16 +2101,19 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>29</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>30</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$M$8:$M$37</c:f>
+              <c:f>'Propane-Use-Day2'!$M$8:$M$38</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="30"/>
+                <c:ptCount val="31"/>
                 <c:pt idx="0">
                   <c:v>24.67</c:v>
                 </c:pt>
@@ -2237,6 +2203,9 @@
                 </c:pt>
                 <c:pt idx="29">
                   <c:v>23.691825396825397</c:v>
+                </c:pt>
+                <c:pt idx="30">
+                  <c:v>23.658095238095239</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -3747,8 +3716,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="5095875"/>
-          <a:ext cx="5419725" cy="2743200"/>
+          <a:off x="609600" y="5334000"/>
+          <a:ext cx="5558790" cy="2895600"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -3821,7 +3790,7 @@
           <a:lstStyle/>
           <a:p>
             <a:fld id="{A1859F44-2397-49EC-A253-DFB0636E0576}" type="TxLink">
-              <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
                 <a:solidFill>
                   <a:srgbClr val="000000"/>
                 </a:solidFill>
@@ -3830,7 +3799,7 @@
               <a:pPr/>
               <a:t>Measured Propane Burn Rate = 0.70 lbs/day</a:t>
             </a:fld>
-            <a:endParaRPr lang="en-US" sz="1100"/>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
           </a:p>
         </xdr:txBody>
       </xdr:sp>
@@ -3841,14 +3810,14 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="14" tableBorderDxfId="13">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="12"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="11">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="8">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="10"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4058,19 +4027,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" topLeftCell="A10" workbookViewId="0">
+    <sheetView showGridLines="0" workbookViewId="0">
       <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4088,7 +4057,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4096,16 +4065,16 @@
         <v>16</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>31</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4114,26 +4083,26 @@
         <v>12-Jul-2023</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
-      <c r="E4" s="25" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+      <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4141,7 +4110,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -4164,7 +4133,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45118.80972222222</v>
       </c>
@@ -4191,7 +4160,7 @@
         <v>28.209872610430022</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45118.810416666667</v>
       </c>
@@ -4218,7 +4187,7 @@
         <v>28.178040868395264</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45119.289583333331</v>
       </c>
@@ -4237,7 +4206,7 @@
         <v>28.146209126360503</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45119.354861111111</v>
       </c>
@@ -4259,7 +4228,7 @@
         <v>28.114377384325746</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45119.390277777777</v>
       </c>
@@ -4270,7 +4239,7 @@
       <c r="D12" s="19">
         <v>27.64</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <f>ABS(24*_nSlope)</f>
         <v>0.76396180883421438</v>
       </c>
@@ -4289,7 +4258,7 @@
         <v>28.082545642290984</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45119.415277777778</v>
       </c>
@@ -4308,7 +4277,7 @@
         <v>28.050713900256227</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45119.432638888888</v>
       </c>
@@ -4327,7 +4296,7 @@
         <v>28.018882158221469</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45119.465277777781</v>
       </c>
@@ -4338,7 +4307,7 @@
       <c r="D15" s="19">
         <v>27.8</v>
       </c>
-      <c r="F15" s="22">
+      <c r="F15" s="20">
         <v>45119.452777777777</v>
       </c>
       <c r="K15" s="14">
@@ -4349,7 +4318,7 @@
         <v>27.987050416186708</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>45119.48333333333</v>
       </c>
@@ -4368,7 +4337,7 @@
         <v>27.955218674151951</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>45119.513194444444</v>
       </c>
@@ -4376,7 +4345,7 @@
         <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
         <v>16.883333333360497</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <v>27.61</v>
       </c>
       <c r="K17" s="14">
@@ -4387,7 +4356,7 @@
         <v>27.923386932117193</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>45119.53402777778</v>
       </c>
@@ -4395,7 +4364,7 @@
         <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
         <v>17.383333333418705</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="23">
         <v>27.69</v>
       </c>
       <c r="K18" s="14">
@@ -4406,7 +4375,7 @@
         <v>27.891555190082432</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>45119.561111111114</v>
       </c>
@@ -4414,7 +4383,7 @@
         <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
         <v>18.033333333441988</v>
       </c>
-      <c r="D19" s="24">
+      <c r="D19" s="23">
         <v>27.68</v>
       </c>
       <c r="K19" s="14">
@@ -4425,7 +4394,7 @@
         <v>27.859723448047674</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>45119.582638888889</v>
       </c>
@@ -4433,7 +4402,7 @@
         <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
         <v>18.550000000046566</v>
       </c>
-      <c r="D20" s="24">
+      <c r="D20" s="23">
         <v>27.51</v>
       </c>
       <c r="K20" s="14">
@@ -4444,7 +4413,7 @@
         <v>27.827891706012913</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>45119.633333333331</v>
       </c>
@@ -4452,7 +4421,7 @@
         <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
         <v>19.766666666662786</v>
       </c>
-      <c r="D21" s="24">
+      <c r="D21" s="23">
         <v>27.67</v>
       </c>
       <c r="K21" s="14">
@@ -4463,7 +4432,7 @@
         <v>27.796059963978156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>45119.664583333331</v>
       </c>
@@ -4471,7 +4440,7 @@
         <f>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</f>
         <v>20.516666666662786</v>
       </c>
-      <c r="D22" s="24">
+      <c r="D22" s="23">
         <v>27.57</v>
       </c>
       <c r="K22" s="14">
@@ -4482,10 +4451,9 @@
         <v>27.764228221943398</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
-      <c r="D23" s="26"/>
       <c r="K23" s="14">
         <v>15</v>
       </c>
@@ -4494,7 +4462,7 @@
         <v>27.732396479908637</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -4503,7 +4471,7 @@
         <v>27.700564737873879</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -4512,7 +4480,7 @@
         <v>27.668732995839122</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -4533,7 +4501,7 @@
         <v>27.636901253804361</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -4548,7 +4516,7 @@
         <v>27.605069511769603</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
@@ -4572,7 +4540,7 @@
         <v>27.573237769734842</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -4591,7 +4559,7 @@
         <v>27.541406027700084</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -4600,7 +4568,7 @@
         <v>27.509574285665327</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -4609,7 +4577,7 @@
         <v>27.477742543630566</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -4619,14 +4587,9 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K8:L30">
-    <cfRule type="expression" dxfId="16" priority="2">
+  <conditionalFormatting sqref="K8:L32">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31:L32">
-    <cfRule type="expression" dxfId="15" priority="1">
-      <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
@@ -4641,21 +4604,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EB25A4-07B8-4BBE-AD53-051224E82545}">
-  <dimension ref="A1:M37"/>
+  <dimension ref="A1:M38"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A10" workbookViewId="0">
-      <selection activeCell="D19" sqref="D19"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
+      <selection activeCell="N34" sqref="N33:N34"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4664,7 +4627,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4672,16 +4635,16 @@
         <v>16</v>
       </c>
       <c r="C2" s="2"/>
-      <c r="E2" s="25" t="s">
+      <c r="E2" s="24" t="s">
         <v>32</v>
       </c>
-      <c r="F2" s="25"/>
-      <c r="G2" s="25"/>
-      <c r="H2" s="25"/>
-      <c r="I2" s="25"/>
-      <c r="J2" s="25"/>
-    </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4690,26 +4653,26 @@
         <v>13-Jul-2023</v>
       </c>
       <c r="C3" s="2"/>
-      <c r="E3" s="25" t="s">
+      <c r="E3" s="24" t="s">
         <v>27</v>
       </c>
-      <c r="F3" s="25"/>
-      <c r="G3" s="25"/>
-      <c r="H3" s="25"/>
-      <c r="I3" s="25"/>
-      <c r="J3" s="25"/>
-    </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="E4" s="25" t="s">
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
-      <c r="F4" s="25"/>
-      <c r="G4" s="25"/>
-      <c r="H4" s="25"/>
-      <c r="I4" s="25"/>
-      <c r="J4" s="25"/>
-    </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4717,7 +4680,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -4743,7 +4706,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45120.291666666664</v>
       </c>
@@ -4762,7 +4725,7 @@
         <v>24.675384823451715</v>
       </c>
       <c r="K8" s="14" cm="1">
-        <f t="array" ref="K8:K37">_xlfn.SEQUENCE(30,1,0,1)</f>
+        <f t="array" ref="K8:K38">_xlfn.SEQUENCE(31,1,0,1)</f>
         <v>0</v>
       </c>
       <c r="L8" s="15">
@@ -4774,7 +4737,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45120.347916666666</v>
       </c>
@@ -4806,7 +4769,7 @@
         <v>24.636269841269844</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45120.377083333333</v>
       </c>
@@ -4829,7 +4792,7 @@
         <v>24.602539682539685</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45120.442361111112</v>
       </c>
@@ -4837,7 +4800,7 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>3.6166666667559184</v>
       </c>
-      <c r="D11" s="24">
+      <c r="D11" s="23">
         <v>24.58</v>
       </c>
       <c r="G11" s="4" t="s">
@@ -4855,7 +4818,7 @@
         <v>24.568809523809527</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45120.518055555556</v>
       </c>
@@ -4863,10 +4826,10 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>5.433333333407063</v>
       </c>
-      <c r="D12" s="24">
+      <c r="D12" s="23">
         <v>24.51</v>
       </c>
-      <c r="G12" s="23">
+      <c r="G12" s="22">
         <f>ABS(24*_nSlope)</f>
         <v>0.70212199664558106</v>
       </c>
@@ -4889,7 +4852,7 @@
         <v>24.535079365079365</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45120.540972222225</v>
       </c>
@@ -4897,7 +4860,7 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>5.9833333334536292</v>
       </c>
-      <c r="D13" s="24">
+      <c r="D13" s="23">
         <v>24.55</v>
       </c>
       <c r="K13" s="14">
@@ -4912,7 +4875,7 @@
         <v>24.501349206349207</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45120.615277777775</v>
       </c>
@@ -4920,7 +4883,7 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>7.7666666666627862</v>
       </c>
-      <c r="D14" s="24">
+      <c r="D14" s="23">
         <v>24.42</v>
       </c>
       <c r="K14" s="14">
@@ -4935,7 +4898,7 @@
         <v>24.467619047619049</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45121.286111111112</v>
       </c>
@@ -4943,7 +4906,7 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>23.866666666755918</v>
       </c>
-      <c r="D15" s="24">
+      <c r="D15" s="23">
         <v>23.96</v>
       </c>
       <c r="G15" s="4" t="s">
@@ -4961,7 +4924,7 @@
         <v>24.433888888888891</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>45121.354861111111</v>
       </c>
@@ -4969,10 +4932,10 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>25.516666666720994</v>
       </c>
-      <c r="D16" s="24">
+      <c r="D16" s="23">
         <v>23.97</v>
       </c>
-      <c r="G16" s="23">
+      <c r="G16" s="22">
         <f>H28/21</f>
         <v>0.80952380952380953</v>
       </c>
@@ -4991,7 +4954,7 @@
         <v>24.400158730158733</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>45121.421527777777</v>
       </c>
@@ -4999,10 +4962,10 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>27.116666666697711</v>
       </c>
-      <c r="D17" s="24">
+      <c r="D17" s="23">
         <v>23.89</v>
       </c>
-      <c r="G17" s="23"/>
+      <c r="G17" s="22"/>
       <c r="K17" s="14">
         <v>9</v>
       </c>
@@ -5015,7 +4978,7 @@
         <v>24.366428571428575</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>45121.509027777778</v>
       </c>
@@ -5023,7 +4986,7 @@
         <f>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</f>
         <v>29.216666666732635</v>
       </c>
-      <c r="D18" s="24">
+      <c r="D18" s="23">
         <v>23.79</v>
       </c>
       <c r="K18" s="14">
@@ -5038,7 +5001,7 @@
         <v>24.332698412698413</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K19" s="14">
         <v>11</v>
       </c>
@@ -5051,7 +5014,7 @@
         <v>24.298968253968255</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B20" s="4" t="s">
         <v>9</v>
       </c>
@@ -5074,7 +5037,7 @@
         <v>24.265238095238097</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>10</v>
       </c>
@@ -5093,7 +5056,7 @@
         <v>24.231507936507938</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>11</v>
       </c>
@@ -5112,8 +5075,8 @@
         <v>24.19777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="F23" s="22"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="F23" s="20"/>
       <c r="K23" s="14">
         <v>15</v>
       </c>
@@ -5126,7 +5089,7 @@
         <v>24.164047619047622</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -5139,7 +5102,7 @@
         <v>24.13031746031746</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -5152,7 +5115,7 @@
         <v>24.096587301587302</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -5171,7 +5134,7 @@
         <v>24.062857142857144</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27" s="14">
         <v>19</v>
       </c>
@@ -5184,7 +5147,7 @@
         <v>24.029126984126986</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E28" t="s">
         <v>29</v>
       </c>
@@ -5206,7 +5169,7 @@
         <v>23.995396825396828</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -5229,7 +5192,7 @@
         <v>23.96166666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -5242,7 +5205,7 @@
         <v>23.927936507936511</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -5255,7 +5218,7 @@
         <v>23.89420634920635</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -5268,7 +5231,7 @@
         <v>23.860476190476192</v>
       </c>
     </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K33" s="14">
         <v>25</v>
       </c>
@@ -5281,7 +5244,7 @@
         <v>23.826746031746033</v>
       </c>
     </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K34" s="14">
         <v>26</v>
       </c>
@@ -5294,7 +5257,7 @@
         <v>23.793015873015875</v>
       </c>
     </row>
-    <row r="35" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K35" s="14">
         <v>27</v>
       </c>
@@ -5307,7 +5270,7 @@
         <v>23.759285714285717</v>
       </c>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K36" s="14">
         <v>28</v>
       </c>
@@ -5320,7 +5283,7 @@
         <v>23.725555555555559</v>
       </c>
     </row>
-    <row r="37" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K37" s="14">
         <v>29</v>
       </c>
@@ -5333,30 +5296,23 @@
         <v>23.691825396825397</v>
       </c>
     </row>
+    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
+      <c r="K38">
+        <v>30</v>
+      </c>
+      <c r="L38" s="15">
+        <f t="shared" ref="L38" si="2">_nInt+_nSlope*K38</f>
+        <v>23.797732327644738</v>
+      </c>
+      <c r="M38" s="15">
+        <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K38</f>
+        <v>23.658095238095239</v>
+      </c>
+    </row>
   </sheetData>
-  <conditionalFormatting sqref="K8:L30">
-    <cfRule type="expression" dxfId="9" priority="6">
+  <conditionalFormatting sqref="K8:M37 L38:M38">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K31:L32">
-    <cfRule type="expression" dxfId="8" priority="5">
-      <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M8:M32">
-    <cfRule type="expression" dxfId="7" priority="4">
-      <formula>MOD(ROW(M8)-ROW($K$7),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="K33:L37">
-    <cfRule type="expression" dxfId="1" priority="2">
-      <formula>MOD(ROW(K33)-ROW($K$7),2)</formula>
-    </cfRule>
-  </conditionalFormatting>
-  <conditionalFormatting sqref="M33:M37">
-    <cfRule type="expression" dxfId="0" priority="1">
-      <formula>MOD(ROW(M33)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>

<commit_message>
Added list of work to do
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EFF6AE12-FFE9-448A-9796-FABF3514EDBB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFEE024-17E0-45B5-B9D0-4454BE6A1972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-26970" yWindow="1830" windowWidth="21600" windowHeight="11235" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day1" sheetId="1" r:id="rId1"/>
@@ -109,7 +109,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -131,7 +131,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="73" uniqueCount="36">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
   <si>
     <t>FROM:</t>
   </si>
@@ -239,6 +239,15 @@
   </si>
   <si>
     <t>Propane Use</t>
+  </si>
+  <si>
+    <t>Mosquito Magnetic Test Plans</t>
+  </si>
+  <si>
+    <t>Checkout hair dryer to kill remaining mosquitos</t>
+  </si>
+  <si>
+    <t>Attempt to measure number of mosquitos</t>
   </si>
 </sst>
 </file>
@@ -4604,10 +4613,10 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EB25A4-07B8-4BBE-AD53-051224E82545}">
-  <dimension ref="A1:M38"/>
+  <dimension ref="A1:M53"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="N34" sqref="N33:N34"/>
+      <selection activeCell="G55" sqref="G55"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -5307,6 +5316,21 @@
       <c r="M38" s="15">
         <f>INDEX(_tTankWeight2[Weight (lbs)],1,1)-$G$16/24*K38</f>
         <v>23.658095238095239</v>
+      </c>
+    </row>
+    <row r="50" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="A50" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A52" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
+      <c r="A53" t="s">
+        <v>38</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
Add Day 3 of Testing Tab
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -1,25 +1,28 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5DFEE024-17E0-45B5-B9D0-4454BE6A1972}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="85" documentId="8_{7E461252-B442-4B32-8E50-AE06978549AB}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{54C8832A-A22C-4E63-AF0E-A46703DA0E1E}"/>
   <bookViews>
-    <workbookView xWindow="-28920" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="1" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day1" sheetId="1" r:id="rId1"/>
     <sheet name="Propane-Use-Day2" sheetId="3" r:id="rId2"/>
+    <sheet name="Propane-Use-Day3" sheetId="4" r:id="rId3"/>
   </sheets>
   <definedNames>
     <definedName name="_nInt" localSheetId="1">'Propane-Use-Day2'!$H$8</definedName>
+    <definedName name="_nInt" localSheetId="2">'Propane-Use-Day3'!$H$8</definedName>
     <definedName name="_nInt">'Propane-Use-Day1'!$H$8</definedName>
     <definedName name="_nSlope" localSheetId="1">'Propane-Use-Day2'!$G$8</definedName>
+    <definedName name="_nSlope" localSheetId="2">'Propane-Use-Day3'!$G$8</definedName>
     <definedName name="_nSlope">'Propane-Use-Day1'!$G$8</definedName>
   </definedNames>
   <calcPr calcId="191029"/>
@@ -80,7 +83,41 @@
     <author>Mark Biegert</author>
   </authors>
   <commentList>
-    <comment ref="H28" authorId="0" shapeId="0" xr:uid="{37CA3984-311B-4082-974E-33113DB63516}">
+    <comment ref="H29" authorId="0" shapeId="0" xr:uid="{37CA3984-311B-4082-974E-33113DB63516}">
+      <text>
+        <r>
+          <rPr>
+            <b/>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t>Mark Biegert:</t>
+        </r>
+        <r>
+          <rPr>
+            <sz val="9"/>
+            <color indexed="81"/>
+            <rFont val="Tahoma"/>
+            <family val="2"/>
+          </rPr>
+          <t xml:space="preserve">
+I measured the difference between full and empty tanks after filling the tank at my local propane filling station. The amount of propane fill varies by station.</t>
+        </r>
+      </text>
+    </comment>
+  </commentList>
+</comments>
+</file>
+
+<file path=xl/comments3.xml><?xml version="1.0" encoding="utf-8"?>
+<comments xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr">
+  <authors>
+    <author>Mark Biegert</author>
+  </authors>
+  <commentList>
+    <comment ref="H33" authorId="0" shapeId="0" xr:uid="{BD9FAC42-22A4-4FF1-B146-F2C42D0545F9}">
       <text>
         <r>
           <rPr>
@@ -131,7 +168,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="76" uniqueCount="39">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="118" uniqueCount="42">
   <si>
     <t>FROM:</t>
   </si>
@@ -248,6 +285,15 @@
   </si>
   <si>
     <t>Attempt to measure number of mosquitos</t>
+  </si>
+  <si>
+    <t xml:space="preserve">Note that I started my test with only 5 lbs of propane in </t>
+  </si>
+  <si>
+    <t>Rate</t>
+  </si>
+  <si>
+    <t>Fuel</t>
   </si>
 </sst>
 </file>
@@ -554,7 +600,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="25">
+  <cellXfs count="28">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -592,6 +638,9 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="16"/>
+    <xf numFmtId="22" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="2" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -612,13 +661,70 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="19">
+  <dxfs count="25">
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
+      <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="2" formatCode="0.00"/>
+      <border diagonalUp="0" diagonalDown="0" outline="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
+    </dxf>
+    <dxf>
+      <border diagonalUp="0" diagonalDown="0">
+        <left/>
+        <right/>
+        <top/>
+        <bottom/>
+      </border>
+    </dxf>
+    <dxf>
+      <alignment horizontal="center" vertical="bottom" textRotation="0" wrapText="0" indent="0" justifyLastLine="0" shrinkToFit="0" readingOrder="0"/>
+      <border diagonalUp="0" diagonalDown="0">
+        <left style="thin">
+          <color auto="1"/>
+        </left>
+        <right style="thin">
+          <color auto="1"/>
+        </right>
+        <top/>
+        <bottom/>
+        <vertical style="thin">
+          <color auto="1"/>
+        </vertical>
+        <horizontal/>
+      </border>
     </dxf>
     <dxf>
       <fill>
@@ -659,7 +765,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -699,6 +805,13 @@
       </border>
     </dxf>
     <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -730,7 +843,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -768,6 +881,13 @@
         </vertical>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -862,13 +982,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="18"/>
-      <tableStyleElement type="headerRow" dxfId="17"/>
-      <tableStyleElement type="totalRow" dxfId="16"/>
-      <tableStyleElement type="firstColumn" dxfId="15"/>
-      <tableStyleElement type="lastColumn" dxfId="14"/>
-      <tableStyleElement type="firstRowStripe" dxfId="13"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="12"/>
+      <tableStyleElement type="wholeTable" dxfId="24"/>
+      <tableStyleElement type="headerRow" dxfId="23"/>
+      <tableStyleElement type="totalRow" dxfId="22"/>
+      <tableStyleElement type="firstColumn" dxfId="21"/>
+      <tableStyleElement type="lastColumn" dxfId="20"/>
+      <tableStyleElement type="firstRowStripe" dxfId="19"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="18"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -1598,7 +1718,7 @@
     <c:title>
       <c:tx>
         <c:strRef>
-          <c:f>'Propane-Use-Day2'!$C$20</c:f>
+          <c:f>'Propane-Use-Day2'!$C$21</c:f>
           <c:strCache>
             <c:ptCount val="1"/>
             <c:pt idx="0">
@@ -1685,10 +1805,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$C$8:$C$18</c:f>
+              <c:f>'Propane-Use-Day2'!$C$8:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -1727,10 +1847,10 @@
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day2'!$D$8:$D$18</c:f>
+              <c:f>'Propane-Use-Day2'!$D$8:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="12"/>
                 <c:pt idx="0">
                   <c:v>24.67</c:v>
                 </c:pt>
@@ -1777,6 +1897,9 @@
         <c:ser>
           <c:idx val="1"/>
           <c:order val="1"/>
+          <c:tx>
+            <c:v>Curve Fit</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
@@ -2003,6 +2126,9 @@
         <c:ser>
           <c:idx val="2"/>
           <c:order val="2"/>
+          <c:tx>
+            <c:v>Specification</c:v>
+          </c:tx>
           <c:spPr>
             <a:ln w="25400" cap="rnd">
               <a:solidFill>
@@ -2263,7 +2389,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Propane-Use-Day2'!$C$21</c:f>
+              <c:f>'Propane-Use-Day2'!$C$22</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2372,7 +2498,7 @@
         <c:title>
           <c:tx>
             <c:strRef>
-              <c:f>'Propane-Use-Day2'!$C$22</c:f>
+              <c:f>'Propane-Use-Day2'!$C$23</c:f>
               <c:strCache>
                 <c:ptCount val="1"/>
                 <c:pt idx="0">
@@ -2544,6 +2670,1185 @@
 </c:chartSpace>
 </file>
 
+<file path=xl/charts/chart3.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:tx>
+        <c:strRef>
+          <c:f>'Propane-Use-Day3'!$C$33</c:f>
+          <c:strCache>
+            <c:ptCount val="1"/>
+            <c:pt idx="0">
+              <c:v>Propane Use</c:v>
+            </c:pt>
+          </c:strCache>
+        </c:strRef>
+      </c:tx>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="9.7466568875727091E-2"/>
+          <c:y val="2.7777777777777776E-2"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="1" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout>
+        <c:manualLayout>
+          <c:layoutTarget val="inner"/>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.16663888888888889"/>
+          <c:y val="0.16849555263925342"/>
+          <c:w val="0.76843066491688539"/>
+          <c:h val="0.64506926217556138"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:scatterChart>
+        <c:scatterStyle val="lineMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:v>Measurements</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="28575" cap="rnd">
+              <a:noFill/>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="triangle"/>
+            <c:size val="10"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:srgbClr val="FF0000"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:noFill/>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$C$8:$C$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1.0833333333721384</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2.0166666666045785</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3.28333333338378</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4.3000000000465661</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5.3666666666977108</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6.3833333333604969</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$D$8:$D$14</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="7"/>
+                <c:pt idx="0">
+                  <c:v>21.882999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.83</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.736666670000002</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.72</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.79</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.725000000000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.704999999999998</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-D8DA-46B1-A799-581615440ECB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="1"/>
+          <c:order val="1"/>
+          <c:tx>
+            <c:v>Curve Fit</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="92D050"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$K$8:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$L$8:$L$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>21.843256712213481</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.820383146886972</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.797509581560462</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.774636016233952</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.751762450907442</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.728888885580933</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.706015320254423</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.683141754927913</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.660268189601403</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.637394624274894</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.614521058948384</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.591647493621874</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.568773928295364</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.545900362968855</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.523026797642345</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.500153232315835</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.477279666989325</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.454406101662816</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.431532536336306</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.408658971009796</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.385785405683286</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.362911840356777</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21.340038275030267</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.317164709703757</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000001-D8DA-46B1-A799-581615440ECB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:ser>
+          <c:idx val="2"/>
+          <c:order val="2"/>
+          <c:tx>
+            <c:v>Specification</c:v>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="25400" cap="rnd">
+              <a:solidFill>
+                <a:srgbClr val="0070C0"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="none"/>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$K$8:$K$38</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>0</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>1</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>2</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>3</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>4</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>5</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>6</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>7</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>8</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>9</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>10</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>11</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>12</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>13</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>14</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>15</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>16</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>17</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>18</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>19</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>20</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>22</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>23</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$M$8:$M$38</c:f>
+              <c:numCache>
+                <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
+                <c:ptCount val="31"/>
+                <c:pt idx="0">
+                  <c:v>21.882999999999999</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>21.849269841269841</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>21.815539682539683</c:v>
+                </c:pt>
+                <c:pt idx="3">
+                  <c:v>21.781809523809525</c:v>
+                </c:pt>
+                <c:pt idx="4">
+                  <c:v>21.748079365079363</c:v>
+                </c:pt>
+                <c:pt idx="5">
+                  <c:v>21.714349206349205</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>21.680619047619047</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>21.646888888888888</c:v>
+                </c:pt>
+                <c:pt idx="8">
+                  <c:v>21.61315873015873</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>21.579428571428572</c:v>
+                </c:pt>
+                <c:pt idx="10">
+                  <c:v>21.54569841269841</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>21.511968253968252</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>21.478238095238094</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>21.444507936507936</c:v>
+                </c:pt>
+                <c:pt idx="14">
+                  <c:v>21.410777777777778</c:v>
+                </c:pt>
+                <c:pt idx="15">
+                  <c:v>21.37704761904762</c:v>
+                </c:pt>
+                <c:pt idx="16">
+                  <c:v>21.343317460317458</c:v>
+                </c:pt>
+                <c:pt idx="17">
+                  <c:v>21.3095873015873</c:v>
+                </c:pt>
+                <c:pt idx="18">
+                  <c:v>21.275857142857141</c:v>
+                </c:pt>
+                <c:pt idx="19">
+                  <c:v>21.242126984126983</c:v>
+                </c:pt>
+                <c:pt idx="20">
+                  <c:v>21.208396825396825</c:v>
+                </c:pt>
+                <c:pt idx="21">
+                  <c:v>21.174666666666667</c:v>
+                </c:pt>
+                <c:pt idx="22">
+                  <c:v>21.140936507936509</c:v>
+                </c:pt>
+                <c:pt idx="23">
+                  <c:v>21.107206349206347</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="0"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000002-D8DA-46B1-A799-581615440ECB}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1689859120"/>
+        <c:axId val="1689860784"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1689859120"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="24"/>
+          <c:min val="0"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Propane-Use-Day3'!$C$34</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Time (hours)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="0.44252077865266842"/>
+              <c:y val="0.90412037037037041"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689860784"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+        <c:majorUnit val="2"/>
+        <c:minorUnit val="1"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1689860784"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+          <c:max val="22"/>
+          <c:min val="20"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:title>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Propane-Use-Day3'!$C$35</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Tank Weight (lbs)</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:layout>
+            <c:manualLayout>
+              <c:xMode val="edge"/>
+              <c:yMode val="edge"/>
+              <c:x val="1.9444444444444445E-2"/>
+              <c:y val="0.25376166520851562"/>
+            </c:manualLayout>
+          </c:layout>
+          <c:overlay val="0"/>
+          <c:spPr>
+            <a:noFill/>
+            <a:ln>
+              <a:noFill/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:txPr>
+            <a:bodyPr rot="-5400000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+            <a:lstStyle/>
+            <a:p>
+              <a:pPr>
+                <a:defRPr sz="1000" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                  <a:solidFill>
+                    <a:schemeClr val="tx1"/>
+                  </a:solidFill>
+                  <a:latin typeface="+mn-lt"/>
+                  <a:ea typeface="+mn-ea"/>
+                  <a:cs typeface="+mn-cs"/>
+                </a:defRPr>
+              </a:pPr>
+              <a:endParaRPr lang="en-US"/>
+            </a:p>
+          </c:txPr>
+        </c:title>
+        <c:numFmt formatCode="0.0" sourceLinked="0"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1"/>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1689859120"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:legend>
+      <c:legendPos val="r"/>
+      <c:layout>
+        <c:manualLayout>
+          <c:xMode val="edge"/>
+          <c:yMode val="edge"/>
+          <c:x val="0.18605741066198"/>
+          <c:y val="0.41687809857101193"/>
+          <c:w val="0.2210896309314587"/>
+          <c:h val="0.22825787401574804"/>
+        </c:manualLayout>
+      </c:layout>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:solidFill>
+          <a:schemeClr val="bg1"/>
+        </a:solidFill>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="900" b="1" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1"/>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:legend>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:noFill/>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr>
+          <a:solidFill>
+            <a:schemeClr val="tx1"/>
+          </a:solidFill>
+        </a:defRPr>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
+<file path=xl/charts/chart4.xml><?xml version="1.0" encoding="utf-8"?>
+<c:chartSpace xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:c16r2="http://schemas.microsoft.com/office/drawing/2015/06/chart">
+  <c:date1904 val="0"/>
+  <c:lang val="en-US"/>
+  <c:roundedCorners val="0"/>
+  <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
+    <mc:Choice xmlns:c14="http://schemas.microsoft.com/office/drawing/2007/8/2/chart" Requires="c14">
+      <c14:style val="102"/>
+    </mc:Choice>
+    <mc:Fallback>
+      <c:style val="2"/>
+    </mc:Fallback>
+  </mc:AlternateContent>
+  <c:chart>
+    <c:title>
+      <c:overlay val="0"/>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+      <c:txPr>
+        <a:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:pPr>
+            <a:defRPr sz="1400" b="0" i="0" u="none" strike="noStrike" kern="1200" spc="0" baseline="0">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="65000"/>
+                  <a:lumOff val="35000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:latin typeface="+mn-lt"/>
+              <a:ea typeface="+mn-ea"/>
+              <a:cs typeface="+mn-cs"/>
+            </a:defRPr>
+          </a:pPr>
+          <a:endParaRPr lang="en-US"/>
+        </a:p>
+      </c:txPr>
+    </c:title>
+    <c:autoTitleDeleted val="0"/>
+    <c:plotArea>
+      <c:layout/>
+      <c:scatterChart>
+        <c:scatterStyle val="smoothMarker"/>
+        <c:varyColors val="0"/>
+        <c:ser>
+          <c:idx val="0"/>
+          <c:order val="0"/>
+          <c:tx>
+            <c:strRef>
+              <c:f>'Propane-Use-Day3'!$M$45</c:f>
+              <c:strCache>
+                <c:ptCount val="1"/>
+                <c:pt idx="0">
+                  <c:v>Rate</c:v>
+                </c:pt>
+              </c:strCache>
+            </c:strRef>
+          </c:tx>
+          <c:spPr>
+            <a:ln w="19050" cap="rnd">
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+          <c:marker>
+            <c:symbol val="circle"/>
+            <c:size val="5"/>
+            <c:spPr>
+              <a:solidFill>
+                <a:schemeClr val="accent1"/>
+              </a:solidFill>
+              <a:ln w="9525">
+                <a:solidFill>
+                  <a:schemeClr val="accent1"/>
+                </a:solidFill>
+              </a:ln>
+              <a:effectLst/>
+            </c:spPr>
+          </c:marker>
+          <c:xVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$L$46:$L$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>4.5</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>7.5500000000000007</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>10.850000000000001</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:xVal>
+          <c:yVal>
+            <c:numRef>
+              <c:f>'Propane-Use-Day3'!$M$46:$M$48</c:f>
+              <c:numCache>
+                <c:formatCode>General</c:formatCode>
+                <c:ptCount val="3"/>
+                <c:pt idx="0">
+                  <c:v>0.55000000000000004</c:v>
+                </c:pt>
+                <c:pt idx="1">
+                  <c:v>0.7</c:v>
+                </c:pt>
+                <c:pt idx="2">
+                  <c:v>0.76</c:v>
+                </c:pt>
+              </c:numCache>
+            </c:numRef>
+          </c:yVal>
+          <c:smooth val="1"/>
+          <c:extLst>
+            <c:ext xmlns:c16="http://schemas.microsoft.com/office/drawing/2014/chart" uri="{C3380CC4-5D6E-409C-BE32-E72D297353CC}">
+              <c16:uniqueId val="{00000000-9EB4-42BF-B093-D69BBC128A78}"/>
+            </c:ext>
+          </c:extLst>
+        </c:ser>
+        <c:dLbls>
+          <c:showLegendKey val="0"/>
+          <c:showVal val="0"/>
+          <c:showCatName val="0"/>
+          <c:showSerName val="0"/>
+          <c:showPercent val="0"/>
+          <c:showBubbleSize val="0"/>
+        </c:dLbls>
+        <c:axId val="1424605519"/>
+        <c:axId val="1424607183"/>
+      </c:scatterChart>
+      <c:valAx>
+        <c:axId val="1424605519"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="b"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1424607183"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:valAx>
+        <c:axId val="1424607183"/>
+        <c:scaling>
+          <c:orientation val="minMax"/>
+        </c:scaling>
+        <c:delete val="0"/>
+        <c:axPos val="l"/>
+        <c:majorGridlines>
+          <c:spPr>
+            <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+              <a:solidFill>
+                <a:schemeClr val="tx1">
+                  <a:lumMod val="15000"/>
+                  <a:lumOff val="85000"/>
+                </a:schemeClr>
+              </a:solidFill>
+              <a:round/>
+            </a:ln>
+            <a:effectLst/>
+          </c:spPr>
+        </c:majorGridlines>
+        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:majorTickMark val="none"/>
+        <c:minorTickMark val="none"/>
+        <c:tickLblPos val="nextTo"/>
+        <c:spPr>
+          <a:noFill/>
+          <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+            <a:solidFill>
+              <a:schemeClr val="tx1">
+                <a:lumMod val="25000"/>
+                <a:lumOff val="75000"/>
+              </a:schemeClr>
+            </a:solidFill>
+            <a:round/>
+          </a:ln>
+          <a:effectLst/>
+        </c:spPr>
+        <c:txPr>
+          <a:bodyPr rot="-60000000" spcFirstLastPara="1" vertOverflow="ellipsis" vert="horz" wrap="square" anchor="ctr" anchorCtr="1"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:pPr>
+              <a:defRPr sz="900" b="0" i="0" u="none" strike="noStrike" kern="1200" baseline="0">
+                <a:solidFill>
+                  <a:schemeClr val="tx1">
+                    <a:lumMod val="65000"/>
+                    <a:lumOff val="35000"/>
+                  </a:schemeClr>
+                </a:solidFill>
+                <a:latin typeface="+mn-lt"/>
+                <a:ea typeface="+mn-ea"/>
+                <a:cs typeface="+mn-cs"/>
+              </a:defRPr>
+            </a:pPr>
+            <a:endParaRPr lang="en-US"/>
+          </a:p>
+        </c:txPr>
+        <c:crossAx val="1424605519"/>
+        <c:crosses val="autoZero"/>
+        <c:crossBetween val="midCat"/>
+      </c:valAx>
+      <c:spPr>
+        <a:noFill/>
+        <a:ln>
+          <a:noFill/>
+        </a:ln>
+        <a:effectLst/>
+      </c:spPr>
+    </c:plotArea>
+    <c:plotVisOnly val="1"/>
+    <c:dispBlanksAs val="gap"/>
+    <c:extLst>
+      <c:ext xmlns:c16r3="http://schemas.microsoft.com/office/drawing/2017/03/chart" uri="{56B9EC1D-385E-4148-901F-78D8002777C0}">
+        <c16r3:dataDisplayOptions16>
+          <c16r3:dispNaAsBlank val="1"/>
+        </c16r3:dataDisplayOptions16>
+      </c:ext>
+    </c:extLst>
+    <c:showDLblsOverMax val="0"/>
+  </c:chart>
+  <c:spPr>
+    <a:solidFill>
+      <a:schemeClr val="bg1"/>
+    </a:solidFill>
+    <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+      <a:solidFill>
+        <a:schemeClr val="tx1">
+          <a:lumMod val="15000"/>
+          <a:lumOff val="85000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:round/>
+    </a:ln>
+    <a:effectLst/>
+  </c:spPr>
+  <c:txPr>
+    <a:bodyPr/>
+    <a:lstStyle/>
+    <a:p>
+      <a:pPr>
+        <a:defRPr/>
+      </a:pPr>
+      <a:endParaRPr lang="en-US"/>
+    </a:p>
+  </c:txPr>
+  <c:printSettings>
+    <c:headerFooter/>
+    <c:pageMargins b="0.75" l="0.7" r="0.7" t="0.75" header="0.3" footer="0.3"/>
+    <c:pageSetup/>
+  </c:printSettings>
+</c:chartSpace>
+</file>
+
 <file path=xl/charts/colors1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
   <a:schemeClr val="accent1"/>
@@ -2624,6 +3929,86 @@
 </cs:colorStyle>
 </file>
 
+<file path=xl/charts/colors3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
+<file path=xl/charts/colors4.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:colorStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" meth="cycle" id="10">
+  <a:schemeClr val="accent1"/>
+  <a:schemeClr val="accent2"/>
+  <a:schemeClr val="accent3"/>
+  <a:schemeClr val="accent4"/>
+  <a:schemeClr val="accent5"/>
+  <a:schemeClr val="accent6"/>
+  <cs:variation/>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+    <a:lumOff val="20000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="80000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="60000"/>
+    <a:lumOff val="40000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+    <a:lumOff val="30000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="70000"/>
+  </cs:variation>
+  <cs:variation>
+    <a:lumMod val="50000"/>
+    <a:lumOff val="50000"/>
+  </cs:variation>
+</cs:colorStyle>
+</file>
+
 <file path=xl/charts/style1.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
@@ -3141,6 +4526,1038 @@
 </file>
 
 <file path=xl/charts/style2.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style3.xml><?xml version="1.0" encoding="utf-8"?>
+<cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
+  <cs:axisTitle>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:axisTitle>
+  <cs:categoryAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:categoryAxis>
+  <cs:chartArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="bg1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="1000" kern="1200"/>
+  </cs:chartArea>
+  <cs:dataLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="75000"/>
+        <a:lumOff val="25000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataLabel>
+  <cs:dataLabelCallout>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln>
+        <a:solidFill>
+          <a:schemeClr val="dk1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+    <cs:bodyPr rot="0" spcFirstLastPara="1" vertOverflow="clip" horzOverflow="clip" vert="horz" wrap="square" lIns="36576" tIns="18288" rIns="36576" bIns="18288" anchor="ctr" anchorCtr="1">
+      <a:spAutoFit/>
+    </cs:bodyPr>
+  </cs:dataLabelCallout>
+  <cs:dataPoint>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint>
+  <cs:dataPoint3D>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:dataPoint3D>
+  <cs:dataPointLine>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointLine>
+  <cs:dataPointMarker>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="1">
+      <cs:styleClr val="auto"/>
+    </cs:fillRef>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointMarker>
+  <cs:dataPointMarkerLayout symbol="circle" size="5"/>
+  <cs:dataPointWireframe>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="dk1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dataPointWireframe>
+  <cs:dataTable>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:dataTable>
+  <cs:downBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="dk1">
+          <a:lumMod val="75000"/>
+          <a:lumOff val="25000"/>
+        </a:schemeClr>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:downBar>
+  <cs:dropLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:dropLine>
+  <cs:errorBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:errorBar>
+  <cs:floor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:floor>
+  <cs:gridlineMajor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="15000"/>
+            <a:lumOff val="85000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMajor>
+  <cs:gridlineMinor>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="5000"/>
+            <a:lumOff val="95000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:gridlineMinor>
+  <cs:hiLoLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="50000"/>
+            <a:lumOff val="50000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:hiLoLine>
+  <cs:leaderLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:leaderLine>
+  <cs:legend>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:legend>
+  <cs:plotArea mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea>
+  <cs:plotArea3D mods="allowNoFillOverride allowNoLineOverride">
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+  </cs:plotArea3D>
+  <cs:seriesAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:seriesAxis>
+  <cs:seriesLine>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="35000"/>
+            <a:lumOff val="65000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:seriesLine>
+  <cs:title>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="1400" b="0" kern="1200" spc="0" baseline="0"/>
+  </cs:title>
+  <cs:trendline>
+    <cs:lnRef idx="0">
+      <cs:styleClr val="auto"/>
+    </cs:lnRef>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="19050" cap="rnd">
+        <a:solidFill>
+          <a:schemeClr val="phClr"/>
+        </a:solidFill>
+        <a:prstDash val="sysDot"/>
+      </a:ln>
+    </cs:spPr>
+  </cs:trendline>
+  <cs:trendlineLabel>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:trendlineLabel>
+  <cs:upBar>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:solidFill>
+        <a:schemeClr val="lt1"/>
+      </a:solidFill>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="65000"/>
+            <a:lumOff val="35000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+  </cs:upBar>
+  <cs:valueAxis>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1">
+        <a:lumMod val="65000"/>
+        <a:lumOff val="35000"/>
+      </a:schemeClr>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:ln w="9525" cap="flat" cmpd="sng" algn="ctr">
+        <a:solidFill>
+          <a:schemeClr val="tx1">
+            <a:lumMod val="25000"/>
+            <a:lumOff val="75000"/>
+          </a:schemeClr>
+        </a:solidFill>
+        <a:round/>
+      </a:ln>
+    </cs:spPr>
+    <cs:defRPr sz="900" kern="1200"/>
+  </cs:valueAxis>
+  <cs:wall>
+    <cs:lnRef idx="0"/>
+    <cs:fillRef idx="0"/>
+    <cs:effectRef idx="0"/>
+    <cs:fontRef idx="minor">
+      <a:schemeClr val="tx1"/>
+    </cs:fontRef>
+    <cs:spPr>
+      <a:noFill/>
+      <a:ln>
+        <a:noFill/>
+      </a:ln>
+    </cs:spPr>
+  </cs:wall>
+</cs:chartStyle>
+</file>
+
+<file path=xl/charts/style4.xml><?xml version="1.0" encoding="utf-8"?>
 <cs:chartStyle xmlns:cs="http://schemas.microsoft.com/office/drawing/2012/chartStyle" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main" id="240">
   <cs:axisTitle>
     <cs:lnRef idx="0"/>
@@ -3703,13 +6120,13 @@
     <xdr:from>
       <xdr:col>1</xdr:col>
       <xdr:colOff>0</xdr:colOff>
-      <xdr:row>31</xdr:row>
+      <xdr:row>32</xdr:row>
       <xdr:rowOff>0</xdr:rowOff>
     </xdr:from>
     <xdr:to>
       <xdr:col>6</xdr:col>
       <xdr:colOff>285750</xdr:colOff>
-      <xdr:row>47</xdr:row>
+      <xdr:row>48</xdr:row>
       <xdr:rowOff>152400</xdr:rowOff>
     </xdr:to>
     <xdr:grpSp>
@@ -3725,8 +6142,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="5334000"/>
-          <a:ext cx="5558790" cy="2895600"/>
+          <a:off x="609600" y="5257800"/>
+          <a:ext cx="5419725" cy="2743200"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -3754,7 +6171,7 @@
           </a:graphicData>
         </a:graphic>
       </xdr:graphicFrame>
-      <xdr:sp macro="" textlink="$G$20">
+      <xdr:sp macro="" textlink="$G$21">
         <xdr:nvSpPr>
           <xdr:cNvPr id="3" name="TextBox 2">
             <a:extLst>
@@ -3818,29 +6235,200 @@
 </xdr:wsDr>
 </file>
 
+<file path=xl/drawings/drawing3.xml><?xml version="1.0" encoding="utf-8"?>
+<xdr:wsDr xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:a="http://schemas.openxmlformats.org/drawingml/2006/main">
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>1</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>37</xdr:row>
+      <xdr:rowOff>0</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>6</xdr:col>
+      <xdr:colOff>285750</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>152400</xdr:rowOff>
+    </xdr:to>
+    <xdr:grpSp>
+      <xdr:nvGrpSpPr>
+        <xdr:cNvPr id="2" name="Group 1">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ACD62075-FF7F-4476-95E2-D94784952108}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGrpSpPr/>
+      </xdr:nvGrpSpPr>
+      <xdr:grpSpPr>
+        <a:xfrm>
+          <a:off x="609600" y="6067425"/>
+          <a:ext cx="5419725" cy="2743200"/>
+          <a:chOff x="609600" y="5095875"/>
+          <a:chExt cx="5419725" cy="2743200"/>
+        </a:xfrm>
+      </xdr:grpSpPr>
+      <xdr:graphicFrame macro="">
+        <xdr:nvGraphicFramePr>
+          <xdr:cNvPr id="3" name="Chart 2">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{ED4C94F9-EC2E-F48E-87C0-6A250853E20D}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvGraphicFramePr>
+            <a:graphicFrameLocks/>
+          </xdr:cNvGraphicFramePr>
+        </xdr:nvGraphicFramePr>
+        <xdr:xfrm>
+          <a:off x="609600" y="5095875"/>
+          <a:ext cx="5419725" cy="2743200"/>
+        </xdr:xfrm>
+        <a:graphic>
+          <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+            <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId1"/>
+          </a:graphicData>
+        </a:graphic>
+      </xdr:graphicFrame>
+      <xdr:sp macro="" textlink="$G$26">
+        <xdr:nvSpPr>
+          <xdr:cNvPr id="4" name="TextBox 3">
+            <a:extLst>
+              <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+                <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{FB8B34EA-721C-C583-F5ED-17A035D7C2C4}"/>
+              </a:ext>
+            </a:extLst>
+          </xdr:cNvPr>
+          <xdr:cNvSpPr txBox="1"/>
+        </xdr:nvSpPr>
+        <xdr:spPr>
+          <a:xfrm>
+            <a:off x="1562100" y="7000876"/>
+            <a:ext cx="3048000" cy="247650"/>
+          </a:xfrm>
+          <a:prstGeom prst="rect">
+            <a:avLst/>
+          </a:prstGeom>
+          <a:solidFill>
+            <a:schemeClr val="lt1"/>
+          </a:solidFill>
+          <a:ln w="9525" cmpd="sng">
+            <a:noFill/>
+          </a:ln>
+        </xdr:spPr>
+        <xdr:style>
+          <a:lnRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:lnRef>
+          <a:fillRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:fillRef>
+          <a:effectRef idx="0">
+            <a:scrgbClr r="0" g="0" b="0"/>
+          </a:effectRef>
+          <a:fontRef idx="minor">
+            <a:schemeClr val="dk1"/>
+          </a:fontRef>
+        </xdr:style>
+        <xdr:txBody>
+          <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+          <a:lstStyle/>
+          <a:p>
+            <a:fld id="{A1859F44-2397-49EC-A253-DFB0636E0576}" type="TxLink">
+              <a:rPr lang="en-US" sz="1000" b="1" i="0" u="none" strike="noStrike">
+                <a:solidFill>
+                  <a:srgbClr val="000000"/>
+                </a:solidFill>
+                <a:latin typeface="Consolas"/>
+              </a:rPr>
+              <a:pPr/>
+              <a:t>Measured Propane Burn Rate = 0.55 lbs/day</a:t>
+            </a:fld>
+            <a:endParaRPr lang="en-US" sz="1100" b="1"/>
+          </a:p>
+        </xdr:txBody>
+      </xdr:sp>
+    </xdr:grpSp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>13</xdr:col>
+      <xdr:colOff>304800</xdr:colOff>
+      <xdr:row>36</xdr:row>
+      <xdr:rowOff>71437</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>21</xdr:col>
+      <xdr:colOff>0</xdr:colOff>
+      <xdr:row>53</xdr:row>
+      <xdr:rowOff>61912</xdr:rowOff>
+    </xdr:to>
+    <xdr:graphicFrame macro="">
+      <xdr:nvGraphicFramePr>
+        <xdr:cNvPr id="5" name="Chart 4">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{0DBBE5B3-C1BA-7811-8496-BCF7A96B5888}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvGraphicFramePr/>
+      </xdr:nvGraphicFramePr>
+      <xdr:xfrm>
+        <a:off x="0" y="0"/>
+        <a:ext cx="0" cy="0"/>
+      </xdr:xfrm>
+      <a:graphic>
+        <a:graphicData uri="http://schemas.openxmlformats.org/drawingml/2006/chart">
+          <c:chart xmlns:c="http://schemas.openxmlformats.org/drawingml/2006/chart" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" r:id="rId2"/>
+        </a:graphicData>
+      </a:graphic>
+    </xdr:graphicFrame>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
+</xdr:wsDr>
+</file>
+
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="9"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="8">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="14"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="13">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="7"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="12"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="6" tableBorderDxfId="5">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
   <autoFilter ref="B7:D18" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="4"/>
-    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="3">
+    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="8"/>
+    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="7">
       <calculatedColumnFormula>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day2'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="2"/>
+    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="6"/>
+  </tableColumns>
+  <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
+</table>
+</file>
+
+<file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D14" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B7:D14" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+  <tableColumns count="3">
+    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="2"/>
+    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="1">
+      <calculatedColumnFormula>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</calculatedColumnFormula>
+    </tableColumn>
+    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="0"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -4036,19 +6624,19 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:L32"/>
   <sheetViews>
-    <sheetView showGridLines="0" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+    <sheetView showGridLines="0" topLeftCell="A7" workbookViewId="0">
+      <selection activeCell="F22" sqref="F22"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4066,7 +6654,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4083,7 +6671,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4101,7 +6689,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -4111,7 +6699,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4119,7 +6707,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -4142,7 +6730,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B8" s="10">
         <v>45118.80972222222</v>
       </c>
@@ -4169,7 +6757,7 @@
         <v>28.209872610430022</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B9" s="10">
         <v>45118.810416666667</v>
       </c>
@@ -4196,7 +6784,7 @@
         <v>28.178040868395264</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B10" s="10">
         <v>45119.289583333331</v>
       </c>
@@ -4215,7 +6803,7 @@
         <v>28.146209126360503</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>45119.354861111111</v>
       </c>
@@ -4237,7 +6825,7 @@
         <v>28.114377384325746</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B12" s="10">
         <v>45119.390277777777</v>
       </c>
@@ -4267,7 +6855,7 @@
         <v>28.082545642290984</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B13" s="10">
         <v>45119.415277777778</v>
       </c>
@@ -4286,7 +6874,7 @@
         <v>28.050713900256227</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B14" s="10">
         <v>45119.432638888888</v>
       </c>
@@ -4305,7 +6893,7 @@
         <v>28.018882158221469</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B15" s="10">
         <v>45119.465277777781</v>
       </c>
@@ -4316,9 +6904,7 @@
       <c r="D15" s="19">
         <v>27.8</v>
       </c>
-      <c r="F15" s="20">
-        <v>45119.452777777777</v>
-      </c>
+      <c r="F15" s="20"/>
       <c r="K15" s="14">
         <v>7</v>
       </c>
@@ -4327,7 +6913,7 @@
         <v>27.987050416186708</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B16" s="10">
         <v>45119.48333333333</v>
       </c>
@@ -4346,7 +6932,7 @@
         <v>27.955218674151951</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B17" s="10">
         <v>45119.513194444444</v>
       </c>
@@ -4365,7 +6951,7 @@
         <v>27.923386932117193</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B18" s="10">
         <v>45119.53402777778</v>
       </c>
@@ -4384,7 +6970,7 @@
         <v>27.891555190082432</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B19" s="10">
         <v>45119.561111111114</v>
       </c>
@@ -4403,7 +6989,7 @@
         <v>27.859723448047674</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B20" s="10">
         <v>45119.582638888889</v>
       </c>
@@ -4422,7 +7008,7 @@
         <v>27.827891706012913</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B21" s="10">
         <v>45119.633333333331</v>
       </c>
@@ -4441,7 +7027,7 @@
         <v>27.796059963978156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B22" s="10">
         <v>45119.664583333331</v>
       </c>
@@ -4460,7 +7046,7 @@
         <v>27.764228221943398</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
       <c r="K23" s="14">
@@ -4471,7 +7057,7 @@
         <v>27.732396479908637</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -4480,7 +7066,7 @@
         <v>27.700564737873879</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -4489,7 +7075,7 @@
         <v>27.668732995839122</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -4510,7 +7096,7 @@
         <v>27.636901253804361</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -4525,7 +7111,7 @@
         <v>27.605069511769603</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
@@ -4549,7 +7135,7 @@
         <v>27.573237769734842</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -4568,7 +7154,7 @@
         <v>27.541406027700084</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -4577,7 +7163,7 @@
         <v>27.509574285665327</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -4586,7 +7172,7 @@
         <v>27.477742543630566</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -4597,7 +7183,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L32">
-    <cfRule type="expression" dxfId="1" priority="1">
+    <cfRule type="expression" dxfId="17" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -4613,21 +7199,21 @@
 
 <file path=xl/worksheets/sheet2.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{62EB25A4-07B8-4BBE-AD53-051224E82545}">
-  <dimension ref="A1:M53"/>
+  <dimension ref="A1:M54"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A24" workbookViewId="0">
-      <selection activeCell="G55" sqref="G55"/>
+    <sheetView showGridLines="0" topLeftCell="A4" workbookViewId="0">
+      <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
   <cols>
-    <col min="2" max="2" width="15.88671875" customWidth="1"/>
-    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -4636,7 +7222,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -4653,7 +7239,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -4671,7 +7257,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -4681,7 +7267,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -4689,7 +7275,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -4715,7 +7301,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="B8" s="10">
         <v>45120.291666666664</v>
       </c>
@@ -4746,7 +7332,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B9" s="10">
         <v>45120.347916666666</v>
       </c>
@@ -4778,7 +7364,7 @@
         <v>24.636269841269844</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B10" s="10">
         <v>45120.377083333333</v>
       </c>
@@ -4801,7 +7387,7 @@
         <v>24.602539682539685</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B11" s="10">
         <v>45120.442361111112</v>
       </c>
@@ -4827,7 +7413,7 @@
         <v>24.568809523809527</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B12" s="10">
         <v>45120.518055555556</v>
       </c>
@@ -4861,7 +7447,7 @@
         <v>24.535079365079365</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B13" s="10">
         <v>45120.540972222225</v>
       </c>
@@ -4884,7 +7470,7 @@
         <v>24.501349206349207</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B14" s="10">
         <v>45120.615277777775</v>
       </c>
@@ -4907,7 +7493,7 @@
         <v>24.467619047619049</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B15" s="10">
         <v>45121.286111111112</v>
       </c>
@@ -4933,7 +7519,7 @@
         <v>24.433888888888891</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B16" s="10">
         <v>45121.354861111111</v>
       </c>
@@ -4945,7 +7531,7 @@
         <v>23.97</v>
       </c>
       <c r="G16" s="22">
-        <f>H28/21</f>
+        <f>H29/21</f>
         <v>0.80952380952380953</v>
       </c>
       <c r="H16" t="s">
@@ -4963,7 +7549,7 @@
         <v>24.400158730158733</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B17" s="10">
         <v>45121.421527777777</v>
       </c>
@@ -4987,7 +7573,7 @@
         <v>24.366428571428575</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B18" s="10">
         <v>45121.509027777778</v>
       </c>
@@ -5010,7 +7596,10 @@
         <v>24.332698412698413</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="25"/>
+      <c r="C19" s="26"/>
+      <c r="D19" s="27"/>
       <c r="K19" s="14">
         <v>11</v>
       </c>
@@ -5023,17 +7612,7 @@
         <v>24.298968253968255</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="B20" s="4" t="s">
-        <v>9</v>
-      </c>
-      <c r="C20" t="s">
-        <v>35</v>
-      </c>
-      <c r="G20" t="str">
-        <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
-        <v>Measured Propane Burn Rate = 0.70 lbs/day</v>
-      </c>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K20" s="14">
         <v>12</v>
       </c>
@@ -5046,12 +7625,16 @@
         <v>24.265238095238097</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B21" s="4" t="s">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="C21" t="s">
-        <v>6</v>
+        <v>35</v>
+      </c>
+      <c r="G21" t="str">
+        <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
+        <v>Measured Propane Burn Rate = 0.70 lbs/day</v>
       </c>
       <c r="K21" s="14">
         <v>13</v>
@@ -5065,12 +7648,12 @@
         <v>24.231507936507938</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
       <c r="B22" s="4" t="s">
-        <v>11</v>
+        <v>10</v>
       </c>
       <c r="C22" t="s">
-        <v>25</v>
+        <v>6</v>
       </c>
       <c r="K22" s="14">
         <v>14</v>
@@ -5084,8 +7667,13 @@
         <v>24.19777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="F23" s="20"/>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C23" t="s">
+        <v>25</v>
+      </c>
       <c r="K23" s="14">
         <v>15</v>
       </c>
@@ -5098,7 +7686,8 @@
         <v>24.164047619047622</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F24" s="20"/>
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -5111,7 +7700,7 @@
         <v>24.13031746031746</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -5124,13 +7713,7 @@
         <v>24.096587301587302</v>
       </c>
     </row>
-    <row r="26" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A26" s="3" t="s">
-        <v>15</v>
-      </c>
-      <c r="E26" s="3" t="s">
-        <v>18</v>
-      </c>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K26" s="14">
         <v>18</v>
       </c>
@@ -5143,7 +7726,13 @@
         <v>24.062857142857144</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A27" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E27" s="3" t="s">
+        <v>18</v>
+      </c>
       <c r="K27" s="14">
         <v>19</v>
       </c>
@@ -5156,16 +7745,7 @@
         <v>24.029126984126986</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
-      <c r="E28" t="s">
-        <v>29</v>
-      </c>
-      <c r="H28" s="5">
-        <v>17</v>
-      </c>
-      <c r="I28" t="s">
-        <v>19</v>
-      </c>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K28" s="14">
         <v>20</v>
       </c>
@@ -5178,16 +7758,15 @@
         <v>23.995396825396828</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
       <c r="E29" t="s">
-        <v>20</v>
-      </c>
-      <c r="H29" s="6">
-        <f>H28/ABS(G12)</f>
-        <v>24.212316493740765</v>
-      </c>
-      <c r="I29" s="16" t="s">
-        <v>21</v>
+        <v>29</v>
+      </c>
+      <c r="H29" s="5">
+        <v>17</v>
+      </c>
+      <c r="I29" t="s">
+        <v>19</v>
       </c>
       <c r="K29" s="14">
         <v>21</v>
@@ -5201,7 +7780,17 @@
         <v>23.96166666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E30" t="s">
+        <v>20</v>
+      </c>
+      <c r="H30" s="6">
+        <f>H29/ABS(G12)</f>
+        <v>24.212316493740765</v>
+      </c>
+      <c r="I30" s="16" t="s">
+        <v>21</v>
+      </c>
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -5214,7 +7803,7 @@
         <v>23.927936507936511</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -5227,7 +7816,7 @@
         <v>23.89420634920635</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -5240,7 +7829,7 @@
         <v>23.860476190476192</v>
       </c>
     </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K33" s="14">
         <v>25</v>
       </c>
@@ -5253,7 +7842,7 @@
         <v>23.826746031746033</v>
       </c>
     </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="34" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K34" s="14">
         <v>26</v>
       </c>
@@ -5266,7 +7855,7 @@
         <v>23.793015873015875</v>
       </c>
     </row>
-    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="35" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K35" s="14">
         <v>27</v>
       </c>
@@ -5279,7 +7868,7 @@
         <v>23.759285714285717</v>
       </c>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="36" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K36" s="14">
         <v>28</v>
       </c>
@@ -5292,7 +7881,7 @@
         <v>23.725555555555559</v>
       </c>
     </row>
-    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="37" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K37" s="14">
         <v>29</v>
       </c>
@@ -5305,7 +7894,7 @@
         <v>23.691825396825397</v>
       </c>
     </row>
-    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
+    <row r="38" spans="11:13" x14ac:dyDescent="0.2">
       <c r="K38">
         <v>30</v>
       </c>
@@ -5318,24 +7907,694 @@
         <v>23.658095238095239</v>
       </c>
     </row>
-    <row r="50" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
-      <c r="A50" s="3" t="s">
+    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A51" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="52" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A52" t="s">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
-      <c r="A53" t="s">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A54" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M37 L38:M38">
-    <cfRule type="expression" dxfId="0" priority="1">
+    <cfRule type="expression" dxfId="11" priority="1">
+      <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <pageSetup orientation="portrait" r:id="rId1"/>
+  <drawing r:id="rId2"/>
+  <legacyDrawing r:id="rId3"/>
+  <tableParts count="1">
+    <tablePart r:id="rId4"/>
+  </tableParts>
+</worksheet>
+</file>
+
+<file path=xl/worksheets/sheet3.xml><?xml version="1.0" encoding="utf-8"?>
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{B61ACF8F-163F-4FEE-A5DD-653E823CCE8B}">
+  <dimension ref="A1:M59"/>
+  <sheetViews>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="P33" sqref="P33"/>
+    </sheetView>
+  </sheetViews>
+  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <cols>
+    <col min="2" max="2" width="15.85546875" customWidth="1"/>
+    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+  </cols>
+  <sheetData>
+    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A1" s="1" t="s">
+        <v>0</v>
+      </c>
+      <c r="B1" s="2" t="s">
+        <v>1</v>
+      </c>
+      <c r="C1" s="2"/>
+    </row>
+    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A2" s="1" t="s">
+        <v>2</v>
+      </c>
+      <c r="B2" s="2" t="s">
+        <v>16</v>
+      </c>
+      <c r="C2" s="2"/>
+      <c r="E2" s="24" t="s">
+        <v>39</v>
+      </c>
+      <c r="F2" s="24"/>
+      <c r="G2" s="24"/>
+      <c r="H2" s="24"/>
+      <c r="I2" s="24"/>
+      <c r="J2" s="24"/>
+    </row>
+    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="A3" s="1" t="s">
+        <v>3</v>
+      </c>
+      <c r="B3" s="2" t="str">
+        <f>TEXT(DATE(2023,7,13),"dd-mmm-yyyy")</f>
+        <v>13-Jul-2023</v>
+      </c>
+      <c r="C3" s="2"/>
+      <c r="E3" s="24" t="s">
+        <v>27</v>
+      </c>
+      <c r="F3" s="24"/>
+      <c r="G3" s="24"/>
+      <c r="H3" s="24"/>
+      <c r="I3" s="24"/>
+      <c r="J3" s="24"/>
+    </row>
+    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="E4" s="24" t="s">
+        <v>28</v>
+      </c>
+      <c r="F4" s="24"/>
+      <c r="G4" s="24"/>
+      <c r="H4" s="24"/>
+      <c r="I4" s="24"/>
+      <c r="J4" s="24"/>
+    </row>
+    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A5" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="J5" s="3" t="s">
+        <v>23</v>
+      </c>
+    </row>
+    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+      <c r="B7" s="7" t="s">
+        <v>4</v>
+      </c>
+      <c r="C7" s="8" t="s">
+        <v>6</v>
+      </c>
+      <c r="D7" s="9" t="s">
+        <v>7</v>
+      </c>
+      <c r="G7" s="4" t="s">
+        <v>12</v>
+      </c>
+      <c r="H7" s="4" t="s">
+        <v>13</v>
+      </c>
+      <c r="K7" s="12" t="s">
+        <v>4</v>
+      </c>
+      <c r="L7" s="13" t="s">
+        <v>5</v>
+      </c>
+      <c r="M7" s="13" t="s">
+        <v>33</v>
+      </c>
+    </row>
+    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+      <c r="B8" s="10">
+        <v>45124.356944444444</v>
+      </c>
+      <c r="C8" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>0</v>
+      </c>
+      <c r="D8" s="19">
+        <v>21.882999999999999</v>
+      </c>
+      <c r="G8" s="17" cm="1">
+        <f t="array" ref="G8:H8">LINEST(_tTankWeight24[Weight (lbs)],_tTankWeight24[Time (hours)])</f>
+        <v>-2.2873565326509762E-2</v>
+      </c>
+      <c r="H8" s="17">
+        <v>21.843256712213481</v>
+      </c>
+      <c r="K8" s="14" cm="1">
+        <f t="array" ref="K8:K31">_xlfn.SEQUENCE(24,1,0,1)</f>
+        <v>0</v>
+      </c>
+      <c r="L8" s="15">
+        <f>_nInt+_nSlope*K8</f>
+        <v>21.843256712213481</v>
+      </c>
+      <c r="M8" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K8</f>
+        <v>21.882999999999999</v>
+      </c>
+    </row>
+    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B9" s="10">
+        <v>45124.402083333334</v>
+      </c>
+      <c r="C9" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>1.0833333333721384</v>
+      </c>
+      <c r="D9" s="19">
+        <f>21.83</f>
+        <v>21.83</v>
+      </c>
+      <c r="F9" s="18" t="s">
+        <v>24</v>
+      </c>
+      <c r="G9" s="18" t="s">
+        <v>8</v>
+      </c>
+      <c r="H9" s="18" t="s">
+        <v>19</v>
+      </c>
+      <c r="K9" s="14">
+        <v>1</v>
+      </c>
+      <c r="L9" s="15">
+        <f t="shared" ref="L9:L31" si="0">_nInt+_nSlope*K9</f>
+        <v>21.820383146886972</v>
+      </c>
+      <c r="M9" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K9</f>
+        <v>21.849269841269841</v>
+      </c>
+    </row>
+    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B10" s="10">
+        <v>45124.440972222219</v>
+      </c>
+      <c r="C10" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>2.0166666666045785</v>
+      </c>
+      <c r="D10" s="19">
+        <v>21.736666670000002</v>
+      </c>
+      <c r="K10" s="14">
+        <v>2</v>
+      </c>
+      <c r="L10" s="15">
+        <f t="shared" si="0"/>
+        <v>21.797509581560462</v>
+      </c>
+      <c r="M10" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K10</f>
+        <v>21.815539682539683</v>
+      </c>
+    </row>
+    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B11" s="10">
+        <v>45124.493750000001</v>
+      </c>
+      <c r="C11" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>3.28333333338378</v>
+      </c>
+      <c r="D11" s="19">
+        <v>21.72</v>
+      </c>
+      <c r="G11" s="4" t="s">
+        <v>17</v>
+      </c>
+      <c r="K11" s="14">
+        <v>3</v>
+      </c>
+      <c r="L11" s="15">
+        <f t="shared" si="0"/>
+        <v>21.774636016233952</v>
+      </c>
+      <c r="M11" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K11</f>
+        <v>21.781809523809525</v>
+      </c>
+    </row>
+    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B12" s="10">
+        <v>45124.536111111112</v>
+      </c>
+      <c r="C12" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>4.3000000000465661</v>
+      </c>
+      <c r="D12" s="19">
+        <v>21.79</v>
+      </c>
+      <c r="G12" s="22">
+        <f>ABS(24*_nSlope)</f>
+        <v>0.54896556783623429</v>
+      </c>
+      <c r="H12" t="s">
+        <v>22</v>
+      </c>
+      <c r="I12" t="str">
+        <f ca="1">_xlfn.FORMULATEXT(G12)</f>
+        <v>=ABS(24*_nSlope)</v>
+      </c>
+      <c r="K12" s="14">
+        <v>4</v>
+      </c>
+      <c r="L12" s="15">
+        <f t="shared" si="0"/>
+        <v>21.751762450907442</v>
+      </c>
+      <c r="M12" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K12</f>
+        <v>21.748079365079363</v>
+      </c>
+    </row>
+    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B13" s="10">
+        <v>45124.580555555556</v>
+      </c>
+      <c r="C13" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>5.3666666666977108</v>
+      </c>
+      <c r="D13" s="19">
+        <v>21.725000000000001</v>
+      </c>
+      <c r="K13" s="14">
+        <v>5</v>
+      </c>
+      <c r="L13" s="15">
+        <f t="shared" si="0"/>
+        <v>21.728888885580933</v>
+      </c>
+      <c r="M13" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K13</f>
+        <v>21.714349206349205</v>
+      </c>
+    </row>
+    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="B14" s="10">
+        <v>45124.622916666667</v>
+      </c>
+      <c r="C14" s="11">
+        <f>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day3'!$B$8,1,1))*24</f>
+        <v>6.3833333333604969</v>
+      </c>
+      <c r="D14" s="19">
+        <v>21.704999999999998</v>
+      </c>
+      <c r="K14" s="14">
+        <v>6</v>
+      </c>
+      <c r="L14" s="15">
+        <f t="shared" si="0"/>
+        <v>21.706015320254423</v>
+      </c>
+      <c r="M14" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K14</f>
+        <v>21.680619047619047</v>
+      </c>
+    </row>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G15" s="4" t="s">
+        <v>34</v>
+      </c>
+      <c r="K15" s="14">
+        <v>7</v>
+      </c>
+      <c r="L15" s="15">
+        <f t="shared" si="0"/>
+        <v>21.683141754927913</v>
+      </c>
+      <c r="M15" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K15</f>
+        <v>21.646888888888888</v>
+      </c>
+    </row>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G16" s="22">
+        <f>H33/21</f>
+        <v>0.80952380952380953</v>
+      </c>
+      <c r="H16" t="s">
+        <v>22</v>
+      </c>
+      <c r="K16" s="14">
+        <v>8</v>
+      </c>
+      <c r="L16" s="15">
+        <f t="shared" si="0"/>
+        <v>21.660268189601403</v>
+      </c>
+      <c r="M16" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K16</f>
+        <v>21.61315873015873</v>
+      </c>
+    </row>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G17" s="22"/>
+      <c r="K17" s="14">
+        <v>9</v>
+      </c>
+      <c r="L17" s="15">
+        <f t="shared" si="0"/>
+        <v>21.637394624274894</v>
+      </c>
+      <c r="M17" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K17</f>
+        <v>21.579428571428572</v>
+      </c>
+    </row>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K18" s="14">
+        <v>10</v>
+      </c>
+      <c r="L18" s="15">
+        <f t="shared" si="0"/>
+        <v>21.614521058948384</v>
+      </c>
+      <c r="M18" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K18</f>
+        <v>21.54569841269841</v>
+      </c>
+    </row>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K19" s="14">
+        <v>11</v>
+      </c>
+      <c r="L19" s="15">
+        <f t="shared" si="0"/>
+        <v>21.591647493621874</v>
+      </c>
+      <c r="M19" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K19</f>
+        <v>21.511968253968252</v>
+      </c>
+    </row>
+    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C20">
+        <v>21.77</v>
+      </c>
+      <c r="K20" s="14">
+        <v>12</v>
+      </c>
+      <c r="L20" s="15">
+        <f t="shared" si="0"/>
+        <v>21.568773928295364</v>
+      </c>
+      <c r="M20" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K20</f>
+        <v>21.478238095238094</v>
+      </c>
+    </row>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C21">
+        <v>21.63</v>
+      </c>
+      <c r="K21" s="14">
+        <v>13</v>
+      </c>
+      <c r="L21" s="15">
+        <f t="shared" si="0"/>
+        <v>21.545900362968855</v>
+      </c>
+      <c r="M21" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K21</f>
+        <v>21.444507936507936</v>
+      </c>
+    </row>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C22">
+        <v>21.7</v>
+      </c>
+      <c r="K22" s="14">
+        <v>14</v>
+      </c>
+      <c r="L22" s="15">
+        <f t="shared" si="0"/>
+        <v>21.523026797642345</v>
+      </c>
+      <c r="M22" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K22</f>
+        <v>21.410777777777778</v>
+      </c>
+    </row>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="C23">
+        <v>21.72</v>
+      </c>
+      <c r="K23" s="14">
+        <v>15</v>
+      </c>
+      <c r="L23" s="15">
+        <f t="shared" si="0"/>
+        <v>21.500153232315835</v>
+      </c>
+      <c r="M23" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K23</f>
+        <v>21.37704761904762</v>
+      </c>
+    </row>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K24" s="14">
+        <v>16</v>
+      </c>
+      <c r="L24" s="15">
+        <f t="shared" si="0"/>
+        <v>21.477279666989325</v>
+      </c>
+      <c r="M24" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K24</f>
+        <v>21.343317460317458</v>
+      </c>
+    </row>
+    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K25" s="14">
+        <v>17</v>
+      </c>
+      <c r="L25" s="15">
+        <f t="shared" si="0"/>
+        <v>21.454406101662816</v>
+      </c>
+      <c r="M25" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K25</f>
+        <v>21.3095873015873</v>
+      </c>
+    </row>
+    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="G26" t="str">
+        <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
+        <v>Measured Propane Burn Rate = 0.55 lbs/day</v>
+      </c>
+      <c r="K26" s="14">
+        <v>18</v>
+      </c>
+      <c r="L26" s="15">
+        <f t="shared" si="0"/>
+        <v>21.431532536336306</v>
+      </c>
+      <c r="M26" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K26</f>
+        <v>21.275857142857141</v>
+      </c>
+    </row>
+    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K27" s="14">
+        <v>19</v>
+      </c>
+      <c r="L27" s="15">
+        <f t="shared" si="0"/>
+        <v>21.408658971009796</v>
+      </c>
+      <c r="M27" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K27</f>
+        <v>21.242126984126983</v>
+      </c>
+    </row>
+    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K28" s="14">
+        <v>20</v>
+      </c>
+      <c r="L28" s="15">
+        <f t="shared" si="0"/>
+        <v>21.385785405683286</v>
+      </c>
+      <c r="M28" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K28</f>
+        <v>21.208396825396825</v>
+      </c>
+    </row>
+    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="F29" s="20"/>
+      <c r="K29" s="14">
+        <v>21</v>
+      </c>
+      <c r="L29" s="15">
+        <f t="shared" si="0"/>
+        <v>21.362911840356777</v>
+      </c>
+      <c r="M29" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K29</f>
+        <v>21.174666666666667</v>
+      </c>
+    </row>
+    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+      <c r="K30" s="14">
+        <v>22</v>
+      </c>
+      <c r="L30" s="15">
+        <f t="shared" si="0"/>
+        <v>21.340038275030267</v>
+      </c>
+      <c r="M30" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K30</f>
+        <v>21.140936507936509</v>
+      </c>
+    </row>
+    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+      <c r="A31" s="3" t="s">
+        <v>15</v>
+      </c>
+      <c r="E31" s="3" t="s">
+        <v>18</v>
+      </c>
+      <c r="K31" s="14">
+        <v>23</v>
+      </c>
+      <c r="L31" s="15">
+        <f t="shared" si="0"/>
+        <v>21.317164709703757</v>
+      </c>
+      <c r="M31" s="15">
+        <f>INDEX(_tTankWeight24[Weight (lbs)],1,1)-$G$16/24*K31</f>
+        <v>21.107206349206347</v>
+      </c>
+    </row>
+    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B33" s="4" t="s">
+        <v>9</v>
+      </c>
+      <c r="C33" t="s">
+        <v>35</v>
+      </c>
+      <c r="E33" t="s">
+        <v>29</v>
+      </c>
+      <c r="H33" s="5">
+        <v>17</v>
+      </c>
+      <c r="I33" t="s">
+        <v>19</v>
+      </c>
+    </row>
+    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B34" s="4" t="s">
+        <v>10</v>
+      </c>
+      <c r="C34" t="s">
+        <v>6</v>
+      </c>
+      <c r="E34" t="s">
+        <v>20</v>
+      </c>
+      <c r="H34" s="6">
+        <f>H33/ABS(G12)</f>
+        <v>30.967333829343897</v>
+      </c>
+      <c r="I34" s="16" t="s">
+        <v>21</v>
+      </c>
+    </row>
+    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B35" s="4" t="s">
+        <v>11</v>
+      </c>
+      <c r="C35" t="s">
+        <v>25</v>
+      </c>
+    </row>
+    <row r="45" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="L45" t="s">
+        <v>41</v>
+      </c>
+      <c r="M45" t="s">
+        <v>40</v>
+      </c>
+    </row>
+    <row r="46" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K46">
+        <v>21.5</v>
+      </c>
+      <c r="L46">
+        <f>K46-17</f>
+        <v>4.5</v>
+      </c>
+      <c r="M46">
+        <v>0.55000000000000004</v>
+      </c>
+    </row>
+    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K47">
+        <v>24.55</v>
+      </c>
+      <c r="L47">
+        <f t="shared" ref="L47:L48" si="1">K47-17</f>
+        <v>7.5500000000000007</v>
+      </c>
+      <c r="M47">
+        <v>0.7</v>
+      </c>
+    </row>
+    <row r="48" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="K48">
+        <v>27.85</v>
+      </c>
+      <c r="L48">
+        <f t="shared" si="1"/>
+        <v>10.850000000000001</v>
+      </c>
+      <c r="M48">
+        <v>0.76</v>
+      </c>
+    </row>
+    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+      <c r="A56" s="3" t="s">
+        <v>36</v>
+      </c>
+    </row>
+    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A58" t="s">
+        <v>37</v>
+      </c>
+    </row>
+    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+      <c r="A59" t="s">
+        <v>38</v>
+      </c>
+    </row>
+  </sheetData>
+  <conditionalFormatting sqref="K8:M31">
+    <cfRule type="expression" dxfId="5" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Last data point for Day4
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="150" documentId="8_{1CE009F8-B825-4926-9E85-1E361AABE077}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{A51280DB-812D-441D-B141-EF4DFDF5ACB0}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{64C36F7D-AF83-42BC-8498-CFC4216E7E2D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day-1" sheetId="1" r:id="rId1"/>
@@ -352,10 +352,11 @@
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr9="http://schemas.microsoft.com/office/spreadsheetml/2016/revision9" mc:Ignorable="x14ac x16r2 xr xr9">
-  <numFmts count="3">
+  <numFmts count="4">
     <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
     <numFmt numFmtId="165" formatCode="0.0;\-0.0;0.0;@"/>
     <numFmt numFmtId="166" formatCode="0.000;\-0.000;0.000;@"/>
+    <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
   </numFmts>
   <fonts count="17" x14ac:knownFonts="1">
     <font>
@@ -486,7 +487,7 @@
       <family val="2"/>
     </font>
   </fonts>
-  <fills count="9">
+  <fills count="8">
     <fill>
       <patternFill patternType="none"/>
     </fill>
@@ -528,14 +529,8 @@
         <fgColor rgb="FFFFCC99"/>
       </patternFill>
     </fill>
-    <fill>
-      <patternFill patternType="solid">
-        <fgColor rgb="FFFDF5E9"/>
-        <bgColor theme="4" tint="0.79995117038483843"/>
-      </patternFill>
-    </fill>
   </fills>
-  <borders count="11">
+  <borders count="10">
     <border>
       <left/>
       <right/>
@@ -638,21 +633,6 @@
       <bottom/>
       <diagonal/>
     </border>
-    <border>
-      <left style="thin">
-        <color auto="1"/>
-      </left>
-      <right style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </right>
-      <top style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </top>
-      <bottom style="thin">
-        <color theme="0" tint="-0.14996795556505021"/>
-      </bottom>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="17">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
@@ -673,7 +653,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="28">
+  <cellXfs count="27">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -711,9 +691,8 @@
     <xf numFmtId="164" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="16"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="164" fontId="0" fillId="8" borderId="10" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="167" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -735,6 +714,34 @@
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -760,7 +767,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -800,13 +807,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -831,7 +831,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -871,13 +871,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -909,7 +902,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -949,13 +942,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -987,7 +973,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1025,13 +1011,6 @@
         </vertical>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -4094,10 +4073,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-4'!$C$8:$C$13</c:f>
+              <c:f>'Propane-Use-Day-4'!$C$8:$C$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -4115,16 +4094,19 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>7.9000000000814907</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>11.750000000058208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-4'!$D$8:$D$13</c:f>
+              <c:f>'Propane-Use-Day-4'!$D$8:$D$14</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="6"/>
+                <c:ptCount val="7"/>
                 <c:pt idx="0">
                   <c:v>21.13</c:v>
                 </c:pt>
@@ -4142,6 +4124,9 @@
                 </c:pt>
                 <c:pt idx="5">
                   <c:v>20.963333330000001</c:v>
+                </c:pt>
+                <c:pt idx="6">
+                  <c:v>20.83666667</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4259,76 +4244,76 @@
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="31"/>
                 <c:pt idx="0">
-                  <c:v>21.112539469868</c:v>
+                  <c:v>21.125609184642613</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>21.09334751129531</c:v>
+                  <c:v>21.102900152762675</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>21.074155552722615</c:v>
+                  <c:v>21.080191120882741</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>21.054963594149925</c:v>
+                  <c:v>21.057482089002804</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>21.03577163557723</c:v>
+                  <c:v>21.034773057122866</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>21.01657967700454</c:v>
+                  <c:v>21.012064025242932</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>20.997387718431845</c:v>
+                  <c:v>20.989354993362994</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>20.978195759859155</c:v>
+                  <c:v>20.966645961483056</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>20.959003801286464</c:v>
+                  <c:v>20.943936929603119</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>20.93981184271377</c:v>
+                  <c:v>20.921227897723185</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>20.920619884141079</c:v>
+                  <c:v>20.898518865843247</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>20.901427925568385</c:v>
+                  <c:v>20.875809833963309</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>20.882235966995694</c:v>
+                  <c:v>20.853100802083375</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>20.863044008423003</c:v>
+                  <c:v>20.830391770203438</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>20.843852049850309</c:v>
+                  <c:v>20.8076827383235</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>20.824660091277618</c:v>
+                  <c:v>20.784973706443566</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>20.805468132704924</c:v>
+                  <c:v>20.762264674563628</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>20.786276174132233</c:v>
+                  <c:v>20.73955564268369</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>20.767084215559539</c:v>
+                  <c:v>20.716846610803756</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>20.747892256986848</c:v>
+                  <c:v>20.694137578923819</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20.728700298414157</c:v>
+                  <c:v>20.671428547043881</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>20.709508339841463</c:v>
+                  <c:v>20.648719515163947</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>20.690316381268772</c:v>
+                  <c:v>20.626010483284009</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>20.671124422696078</c:v>
+                  <c:v>20.603301451404072</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -4967,8 +4952,8 @@
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="4"/>
-                <c:pt idx="0" formatCode="General">
-                  <c:v>0.46</c:v>
+                <c:pt idx="0">
+                  <c:v>0.54501676511847763</c:v>
                 </c:pt>
                 <c:pt idx="1">
                   <c:v>0.64</c:v>
@@ -5059,40 +5044,40 @@
                 <c:formatCode>0.000;\-0.000;0.000;@</c:formatCode>
                 <c:ptCount val="12"/>
                 <c:pt idx="0">
-                  <c:v>0.39733314704715617</c:v>
+                  <c:v>0.47394651974618668</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>0.43226180526275082</c:v>
+                  <c:v>0.50090696185247419</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>0.46719046347834547</c:v>
+                  <c:v>0.52786740395876175</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>0.50211912169394013</c:v>
+                  <c:v>0.55482784606504931</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>0.53704777990953478</c:v>
+                  <c:v>0.58178828817133688</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>0.57197643812512944</c:v>
+                  <c:v>0.60874873027762444</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>0.60690509634072409</c:v>
+                  <c:v>0.63570917238391189</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>0.64183375455631864</c:v>
+                  <c:v>0.66266961449019945</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>0.6767624127719134</c:v>
+                  <c:v>0.68963005659648702</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>0.71169107098750795</c:v>
+                  <c:v>0.71659049870277458</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>0.74661972920310271</c:v>
+                  <c:v>0.74355094080906214</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>0.78154838741869725</c:v>
+                  <c:v>0.7705113829153496</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5289,7 +5274,7 @@
             </a:p>
           </c:txPr>
         </c:title>
-        <c:numFmt formatCode="General" sourceLinked="1"/>
+        <c:numFmt formatCode="0.00;\-0.00;0.00;@" sourceLinked="1"/>
         <c:majorTickMark val="none"/>
         <c:minorTickMark val="none"/>
         <c:tickLblPos val="nextTo"/>
@@ -8783,8 +8768,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="5257800"/>
-          <a:ext cx="5419725" cy="2743200"/>
+          <a:off x="609600" y="5410200"/>
+          <a:ext cx="5566410" cy="2834640"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -8904,8 +8889,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="6067425"/>
-          <a:ext cx="5419725" cy="2743200"/>
+          <a:off x="609600" y="6248400"/>
+          <a:ext cx="5566410" cy="2834640"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -9061,8 +9046,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="6067425"/>
-          <a:ext cx="5505450" cy="2771775"/>
+          <a:off x="609600" y="6248400"/>
+          <a:ext cx="5650230" cy="2849880"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -9142,7 +9127,7 @@
                 <a:latin typeface="Consolas"/>
               </a:rPr>
               <a:pPr/>
-              <a:t>Measured Propane Burn Rate = 0.46 lbs/day</a:t>
+              <a:t>Measured Propane Burn Rate = 0.55 lbs/day</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="1100" b="1"/>
           </a:p>
@@ -9193,56 +9178,56 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="20">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="B7:D18" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="15">
       <calculatedColumnFormula>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day-2'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D15" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D15" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="B7:D15" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="10">
       <calculatedColumnFormula>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day-3'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F9E77B6-A77B-4862-A8B3-E12969205598}" name="_tTankWeight4" displayName="_tTankWeight4" ref="B7:D13" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B7:D13" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F9E77B6-A77B-4862-A8B3-E12969205598}" name="_tTankWeight4" displayName="_tTankWeight4" ref="B7:D14" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
+  <autoFilter ref="B7:D14" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B43DB70-94E1-459B-8FB3-761B425FC480}" name="X" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{182F14ED-38CE-440A-A952-5B718E8962E5}" name="Time (hours)" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{3B43DB70-94E1-459B-8FB3-761B425FC480}" name="X" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{182F14ED-38CE-440A-A952-5B718E8962E5}" name="Time (hours)" dataDxfId="5">
       <calculatedColumnFormula>(_tTankWeight4[[#This Row],[X]]-INDEX('Propane-Use-Day-4'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CAF6B0C6-7671-4815-AA0F-C7EC06E66BB3}" name="Weight (lbs)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{CAF6B0C6-7671-4815-AA0F-C7EC06E66BB3}" name="Weight (lbs)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9442,15 +9427,15 @@
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9468,7 +9453,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -9485,7 +9470,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -9503,7 +9488,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -9513,7 +9498,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -9521,7 +9506,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -9544,7 +9529,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45118.80972222222</v>
       </c>
@@ -9571,7 +9556,7 @@
         <v>28.209872610430022</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45118.810416666667</v>
       </c>
@@ -9598,7 +9583,7 @@
         <v>28.178040868395264</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45119.289583333331</v>
       </c>
@@ -9617,7 +9602,7 @@
         <v>28.146209126360503</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45119.354861111111</v>
       </c>
@@ -9639,7 +9624,7 @@
         <v>28.114377384325746</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45119.390277777777</v>
       </c>
@@ -9669,7 +9654,7 @@
         <v>28.082545642290984</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45119.415277777778</v>
       </c>
@@ -9688,7 +9673,7 @@
         <v>28.050713900256227</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45119.432638888888</v>
       </c>
@@ -9707,7 +9692,7 @@
         <v>28.018882158221469</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45119.465277777781</v>
       </c>
@@ -9727,7 +9712,7 @@
         <v>27.987050416186708</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>45119.48333333333</v>
       </c>
@@ -9746,7 +9731,7 @@
         <v>27.955218674151951</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>45119.513194444444</v>
       </c>
@@ -9765,7 +9750,7 @@
         <v>27.923386932117193</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>45119.53402777778</v>
       </c>
@@ -9784,7 +9769,7 @@
         <v>27.891555190082432</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>45119.561111111114</v>
       </c>
@@ -9803,7 +9788,7 @@
         <v>27.859723448047674</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>45119.582638888889</v>
       </c>
@@ -9822,7 +9807,7 @@
         <v>27.827891706012913</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>45119.633333333331</v>
       </c>
@@ -9841,7 +9826,7 @@
         <v>27.796059963978156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>45119.664583333331</v>
       </c>
@@ -9860,7 +9845,7 @@
         <v>27.764228221943398</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
       <c r="K23" s="14">
@@ -9871,7 +9856,7 @@
         <v>27.732396479908637</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -9880,7 +9865,7 @@
         <v>27.700564737873879</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -9889,7 +9874,7 @@
         <v>27.668732995839122</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -9910,7 +9895,7 @@
         <v>27.636901253804361</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -9925,7 +9910,7 @@
         <v>27.605069511769603</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
@@ -9949,7 +9934,7 @@
         <v>27.573237769734842</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -9968,7 +9953,7 @@
         <v>27.541406027700084</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -9977,7 +9962,7 @@
         <v>27.509574285665327</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -9986,7 +9971,7 @@
         <v>27.477742543630566</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -9997,7 +9982,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L32">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10019,15 +10004,15 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10036,7 +10021,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -10053,7 +10038,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -10071,7 +10056,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -10081,7 +10066,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -10089,7 +10074,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -10115,7 +10100,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45120.291666666664</v>
       </c>
@@ -10146,7 +10131,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45120.347916666666</v>
       </c>
@@ -10178,7 +10163,7 @@
         <v>24.636269841269844</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45120.377083333333</v>
       </c>
@@ -10201,7 +10186,7 @@
         <v>24.602539682539685</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45120.442361111112</v>
       </c>
@@ -10227,7 +10212,7 @@
         <v>24.568809523809527</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45120.518055555556</v>
       </c>
@@ -10261,7 +10246,7 @@
         <v>24.535079365079365</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45120.540972222225</v>
       </c>
@@ -10284,7 +10269,7 @@
         <v>24.501349206349207</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45120.615277777775</v>
       </c>
@@ -10307,7 +10292,7 @@
         <v>24.467619047619049</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45121.286111111112</v>
       </c>
@@ -10333,7 +10318,7 @@
         <v>24.433888888888891</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>45121.354861111111</v>
       </c>
@@ -10363,7 +10348,7 @@
         <v>24.400158730158733</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>45121.421527777777</v>
       </c>
@@ -10387,7 +10372,7 @@
         <v>24.366428571428575</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>45121.509027777778</v>
       </c>
@@ -10410,7 +10395,7 @@
         <v>24.332698412698413</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
       <c r="K19" s="14">
@@ -10425,7 +10410,7 @@
         <v>24.298968253968255</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="14">
         <v>12</v>
       </c>
@@ -10438,7 +10423,7 @@
         <v>24.265238095238097</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -10461,7 +10446,7 @@
         <v>24.231507936507938</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
@@ -10480,7 +10465,7 @@
         <v>24.19777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
@@ -10499,7 +10484,7 @@
         <v>24.164047619047622</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F24" s="20"/>
       <c r="K24" s="14">
         <v>16</v>
@@ -10513,7 +10498,7 @@
         <v>24.13031746031746</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -10526,7 +10511,7 @@
         <v>24.096587301587302</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K26" s="14">
         <v>18</v>
       </c>
@@ -10539,7 +10524,7 @@
         <v>24.062857142857144</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -10558,7 +10543,7 @@
         <v>24.029126984126986</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28" s="14">
         <v>20</v>
       </c>
@@ -10571,7 +10556,7 @@
         <v>23.995396825396828</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>29</v>
       </c>
@@ -10593,7 +10578,7 @@
         <v>23.96166666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>20</v>
       </c>
@@ -10616,7 +10601,7 @@
         <v>23.927936507936511</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -10629,7 +10614,7 @@
         <v>23.89420634920635</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -10642,7 +10627,7 @@
         <v>23.860476190476192</v>
       </c>
     </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K33" s="14">
         <v>25</v>
       </c>
@@ -10655,7 +10640,7 @@
         <v>23.826746031746033</v>
       </c>
     </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K34" s="14">
         <v>26</v>
       </c>
@@ -10668,7 +10653,7 @@
         <v>23.793015873015875</v>
       </c>
     </row>
-    <row r="35" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K35" s="14">
         <v>27</v>
       </c>
@@ -10681,7 +10666,7 @@
         <v>23.759285714285717</v>
       </c>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K36" s="14">
         <v>28</v>
       </c>
@@ -10694,7 +10679,7 @@
         <v>23.725555555555559</v>
       </c>
     </row>
-    <row r="37" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K37" s="14">
         <v>29</v>
       </c>
@@ -10707,7 +10692,7 @@
         <v>23.691825396825397</v>
       </c>
     </row>
-    <row r="38" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K38">
         <v>30</v>
       </c>
@@ -10720,24 +10705,24 @@
         <v>23.658095238095239</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M37 L38:M38">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10759,15 +10744,15 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10776,7 +10761,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -10793,7 +10778,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -10811,7 +10796,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -10821,7 +10806,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -10829,7 +10814,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -10855,7 +10840,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45124.356944444444</v>
       </c>
@@ -10886,7 +10871,7 @@
         <v>21.882999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45124.402083333334</v>
       </c>
@@ -10919,7 +10904,7 @@
         <v>21.849269841269841</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45124.440972222219</v>
       </c>
@@ -10942,7 +10927,7 @@
         <v>21.815539682539683</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45124.493750000001</v>
       </c>
@@ -10968,7 +10953,7 @@
         <v>21.781809523809525</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45124.536111111112</v>
       </c>
@@ -11002,7 +10987,7 @@
         <v>21.748079365079363</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45124.580555555556</v>
       </c>
@@ -11025,7 +11010,7 @@
         <v>21.714349206349205</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45124.622916666667</v>
       </c>
@@ -11048,8 +11033,8 @@
         <v>21.680619047619047</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="25">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
         <v>45124.800694444442</v>
       </c>
       <c r="C15" s="11">
@@ -11074,7 +11059,7 @@
         <v>21.646888888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G16" s="22">
         <f>H33/21</f>
         <v>0.80952380952380953</v>
@@ -11094,7 +11079,7 @@
         <v>21.61315873015873</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G17" s="22"/>
       <c r="K17" s="14">
         <v>9</v>
@@ -11108,7 +11093,7 @@
         <v>21.579428571428572</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K18" s="14">
         <v>10</v>
       </c>
@@ -11121,7 +11106,7 @@
         <v>21.54569841269841</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K19" s="14">
         <v>11</v>
       </c>
@@ -11134,7 +11119,7 @@
         <v>21.511968253968252</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="14">
         <v>12</v>
       </c>
@@ -11147,7 +11132,7 @@
         <v>21.478238095238094</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K21" s="14">
         <v>13</v>
       </c>
@@ -11160,7 +11145,7 @@
         <v>21.444507936507936</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K22" s="14">
         <v>14</v>
       </c>
@@ -11173,7 +11158,7 @@
         <v>21.410777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23" s="14">
         <v>15</v>
       </c>
@@ -11186,7 +11171,7 @@
         <v>21.37704761904762</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -11199,7 +11184,7 @@
         <v>21.343317460317458</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -11212,7 +11197,7 @@
         <v>21.3095873015873</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G26" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
         <v>Measured Propane Burn Rate = 0.64 lbs/day</v>
@@ -11229,7 +11214,7 @@
         <v>21.275857142857141</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27" s="14">
         <v>19</v>
       </c>
@@ -11242,7 +11227,7 @@
         <v>21.242126984126983</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28" s="14">
         <v>20</v>
       </c>
@@ -11255,7 +11240,7 @@
         <v>21.208396825396825</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F29" s="20"/>
       <c r="K29" s="14">
         <v>21</v>
@@ -11269,7 +11254,7 @@
         <v>21.174666666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -11282,7 +11267,7 @@
         <v>21.140936507936509</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -11301,7 +11286,7 @@
         <v>21.107206349206347</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -11318,7 +11303,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
@@ -11336,7 +11321,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
@@ -11344,7 +11329,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L40" t="s">
         <v>41</v>
       </c>
@@ -11352,7 +11337,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K41">
         <v>21.5</v>
       </c>
@@ -11364,7 +11349,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K42">
         <v>24.55</v>
       </c>
@@ -11376,7 +11361,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K43">
         <v>27.85</v>
       </c>
@@ -11388,24 +11373,24 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M31">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11423,19 +11408,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2660F757-7902-41C1-9127-0A0B0C181624}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B4" workbookViewId="0">
+      <selection activeCell="P18" sqref="P18:P19"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11444,7 +11429,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -11461,7 +11446,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -11479,7 +11464,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -11489,7 +11474,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -11497,7 +11482,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -11523,8 +11508,8 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
-      <c r="B8" s="25">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
+      <c r="B8" s="10">
         <v>45125.282638888886</v>
       </c>
       <c r="C8" s="11">
@@ -11536,10 +11521,10 @@
       </c>
       <c r="G8" s="17" cm="1">
         <f t="array" ref="G8:H8">LINEST(_tTankWeight4[Weight (lbs)],_tTankWeight4[Time (hours)])</f>
-        <v>-1.9191958572692229E-2</v>
+        <v>-2.2709031879936566E-2</v>
       </c>
       <c r="H8" s="17">
-        <v>21.112539469868</v>
+        <v>21.125609184642613</v>
       </c>
       <c r="K8" s="14" cm="1">
         <f t="array" ref="K8:K31">_xlfn.SEQUENCE(24,1,0,1)</f>
@@ -11547,15 +11532,15 @@
       </c>
       <c r="L8" s="15">
         <f>_nInt+_nSlope*K8</f>
-        <v>21.112539469868</v>
+        <v>21.125609184642613</v>
       </c>
       <c r="M8" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K8</f>
         <v>21.13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B9" s="25">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B9" s="10">
         <v>45125.387499999997</v>
       </c>
       <c r="C9" s="11">
@@ -11579,15 +11564,15 @@
       </c>
       <c r="L9" s="15">
         <f t="shared" ref="L9:L31" si="0">_nInt+_nSlope*K9</f>
-        <v>21.09334751129531</v>
+        <v>21.102900152762675</v>
       </c>
       <c r="M9" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K9</f>
         <v>21.096269841269841</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B10" s="25">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B10" s="10">
         <v>45125.504166666666</v>
       </c>
       <c r="C10" s="11">
@@ -11602,15 +11587,15 @@
       </c>
       <c r="L10" s="15">
         <f t="shared" si="0"/>
-        <v>21.074155552722615</v>
+        <v>21.080191120882741</v>
       </c>
       <c r="M10" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K10</f>
         <v>21.062539682539683</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B11" s="25">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B11" s="10">
         <v>45125.529166666667</v>
       </c>
       <c r="C11" s="11">
@@ -11628,15 +11613,15 @@
       </c>
       <c r="L11" s="15">
         <f t="shared" si="0"/>
-        <v>21.054963594149925</v>
+        <v>21.057482089002804</v>
       </c>
       <c r="M11" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K11</f>
         <v>21.028809523809525</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B12" s="25">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B12" s="10">
         <v>45125.571527777778</v>
       </c>
       <c r="C12" s="11">
@@ -11648,7 +11633,7 @@
       </c>
       <c r="G12" s="22">
         <f>ABS(24*_nSlope)</f>
-        <v>0.4606070057446135</v>
+        <v>0.54501676511847763</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -11662,15 +11647,15 @@
       </c>
       <c r="L12" s="15">
         <f t="shared" si="0"/>
-        <v>21.03577163557723</v>
+        <v>21.034773057122866</v>
       </c>
       <c r="M12" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K12</f>
         <v>20.995079365079363</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B13" s="25">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B13" s="10">
         <v>45125.611805555556</v>
       </c>
       <c r="C13" s="11">
@@ -11685,30 +11670,37 @@
       </c>
       <c r="L13" s="15">
         <f t="shared" si="0"/>
-        <v>21.01657967700454</v>
+        <v>21.012064025242932</v>
       </c>
       <c r="M13" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K13</f>
         <v>20.961349206349205</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="26">
+        <v>45125.772222222222</v>
+      </c>
+      <c r="C14" s="11">
+        <f>(_tTankWeight4[[#This Row],[X]]-INDEX('Propane-Use-Day-4'!$B$8,1,1))*24</f>
+        <v>11.750000000058208</v>
+      </c>
+      <c r="D14" s="19">
+        <v>20.83666667</v>
+      </c>
       <c r="K14" s="14">
         <v>6</v>
       </c>
       <c r="L14" s="15">
         <f t="shared" si="0"/>
-        <v>20.997387718431845</v>
+        <v>20.989354993362994</v>
       </c>
       <c r="M14" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K14</f>
         <v>20.927619047619046</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D15">
-        <v>21.05</v>
-      </c>
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G15" s="4" t="s">
         <v>34</v>
       </c>
@@ -11717,17 +11709,14 @@
       </c>
       <c r="L15" s="15">
         <f t="shared" si="0"/>
-        <v>20.978195759859155</v>
+        <v>20.966645961483056</v>
       </c>
       <c r="M15" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K15</f>
         <v>20.893888888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D16">
-        <v>21.37</v>
-      </c>
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G16" s="22">
         <f>H33/21</f>
         <v>0.80952380952380953</v>
@@ -11740,238 +11729,202 @@
       </c>
       <c r="L16" s="15">
         <f t="shared" si="0"/>
-        <v>20.959003801286464</v>
+        <v>20.943936929603119</v>
       </c>
       <c r="M16" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K16</f>
         <v>20.86015873015873</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D17">
-        <v>21.13</v>
-      </c>
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G17" s="22"/>
       <c r="K17" s="14">
         <v>9</v>
       </c>
       <c r="L17" s="15">
         <f t="shared" si="0"/>
-        <v>20.93981184271377</v>
+        <v>20.921227897723185</v>
       </c>
       <c r="M17" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K17</f>
         <v>20.826428571428572</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="C18" s="27">
-        <v>21.193333330000002</v>
-      </c>
-      <c r="D18">
-        <v>21.13</v>
-      </c>
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K18" s="14">
         <v>10</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="0"/>
-        <v>20.920619884141079</v>
+        <v>20.898518865843247</v>
       </c>
       <c r="M18" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K18</f>
         <v>20.79269841269841</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="D19">
-        <v>21.16</v>
-      </c>
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K19" s="14">
         <v>11</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>20.901427925568385</v>
+        <v>20.875809833963309</v>
       </c>
       <c r="M19" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K19</f>
         <v>20.758968253968252</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="14">
         <v>12</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>20.882235966995694</v>
+        <v>20.853100802083375</v>
       </c>
       <c r="M20" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K20</f>
         <v>20.725238095238094</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B21">
-        <v>20.96</v>
-      </c>
-      <c r="D21">
-        <v>21.04</v>
-      </c>
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K21" s="14">
         <v>13</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="0"/>
-        <v>20.863044008423003</v>
+        <v>20.830391770203438</v>
       </c>
       <c r="M21" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K21</f>
         <v>20.691507936507936</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B22">
-        <v>20.99</v>
-      </c>
-      <c r="D22">
-        <v>20.98</v>
-      </c>
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K22" s="14">
         <v>14</v>
       </c>
       <c r="L22" s="15">
         <f t="shared" si="0"/>
-        <v>20.843852049850309</v>
+        <v>20.8076827383235</v>
       </c>
       <c r="M22" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K22</f>
         <v>20.657777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B23">
-        <v>20.94</v>
-      </c>
-      <c r="D23">
-        <v>21.03</v>
-      </c>
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23" s="14">
         <v>15</v>
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>20.824660091277618</v>
+        <v>20.784973706443566</v>
       </c>
       <c r="M23" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K23</f>
         <v>20.624047619047619</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B24">
-        <v>20.963333330000001</v>
-      </c>
-      <c r="D24">
-        <v>21.016666669999999</v>
-      </c>
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>20.805468132704924</v>
+        <v>20.762264674563628</v>
       </c>
       <c r="M24" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K24</f>
         <v>20.590317460317458</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="0"/>
-        <v>20.786276174132233</v>
+        <v>20.73955564268369</v>
       </c>
       <c r="M25" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K25</f>
         <v>20.5565873015873</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G26" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
-        <v>Measured Propane Burn Rate = 0.46 lbs/day</v>
+        <v>Measured Propane Burn Rate = 0.55 lbs/day</v>
       </c>
       <c r="K26" s="14">
         <v>18</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="0"/>
-        <v>20.767084215559539</v>
+        <v>20.716846610803756</v>
       </c>
       <c r="M26" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K26</f>
         <v>20.522857142857141</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27" s="14">
         <v>19</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
-        <v>20.747892256986848</v>
+        <v>20.694137578923819</v>
       </c>
       <c r="M27" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K27</f>
         <v>20.489126984126983</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28" s="14">
         <v>20</v>
       </c>
       <c r="L28" s="15">
         <f t="shared" si="0"/>
-        <v>20.728700298414157</v>
+        <v>20.671428547043881</v>
       </c>
       <c r="M28" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K28</f>
         <v>20.455396825396825</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F29" s="20"/>
       <c r="K29" s="14">
         <v>21</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="0"/>
-        <v>20.709508339841463</v>
+        <v>20.648719515163947</v>
       </c>
       <c r="M29" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K29</f>
         <v>20.421666666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="0"/>
-        <v>20.690316381268772</v>
+        <v>20.626010483284009</v>
       </c>
       <c r="M30" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K30</f>
         <v>20.387936507936509</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -11983,14 +11936,14 @@
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
-        <v>20.671124422696078</v>
+        <v>20.603301451404072</v>
       </c>
       <c r="M31" s="15">
         <f>INDEX(_tTankWeight4[Weight (lbs)],1,1)-$G$16/24*K31</f>
         <v>20.354206349206347</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -12007,7 +11960,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
@@ -12019,13 +11972,13 @@
       </c>
       <c r="H34" s="6">
         <f>H33/ABS(G12)</f>
-        <v>36.907819004007415</v>
+        <v>31.191701041167939</v>
       </c>
       <c r="I34" s="16" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
@@ -12033,7 +11986,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L40" t="s">
         <v>41</v>
       </c>
@@ -12041,7 +11994,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K41">
         <v>21.13</v>
       </c>
@@ -12049,11 +12002,12 @@
         <f>K41-17</f>
         <v>4.129999999999999</v>
       </c>
-      <c r="M41">
-        <v>0.46</v>
-      </c>
-    </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="M41" s="22">
+        <f>ABS(24*_nSlope)</f>
+        <v>0.54501676511847763</v>
+      </c>
+    </row>
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K42">
         <v>21.88</v>
       </c>
@@ -12065,7 +12019,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K43">
         <v>24.67</v>
       </c>
@@ -12077,7 +12031,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K44">
         <v>28.11</v>
       </c>
@@ -12089,90 +12043,90 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="45" spans="2:13" ht="15" x14ac:dyDescent="0.25">
-      <c r="K45" s="3" t="s">
+    <row r="46" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
+      <c r="K46" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K47" cm="1">
         <f t="array" ref="K47:L47">LINEST(M41:M44,L41:L44)</f>
-        <v>3.4928658215594648E-2</v>
+        <v>2.6960442106287542E-2</v>
       </c>
       <c r="L47">
-        <v>0.39733314704715617</v>
-      </c>
-    </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.47394651974618668</v>
+      </c>
+    </row>
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K50" cm="1">
         <f t="array" ref="K50:K61">_xlfn.SEQUENCE(12,1,0,1)</f>
         <v>0</v>
       </c>
-      <c r="L50" s="26">
+      <c r="L50" s="25">
         <f>$L$47+K50*$K$47</f>
-        <v>0.39733314704715617</v>
-      </c>
-    </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.47394651974618668</v>
+      </c>
+    </row>
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K51">
         <v>1</v>
       </c>
-      <c r="L51" s="26">
+      <c r="L51" s="25">
         <f t="shared" ref="L51:L61" si="2">$L$47+K51*$K$47</f>
-        <v>0.43226180526275082</v>
-      </c>
-    </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.50090696185247419</v>
+      </c>
+    </row>
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K52">
         <v>2</v>
       </c>
-      <c r="L52" s="26">
+      <c r="L52" s="25">
         <f t="shared" si="2"/>
-        <v>0.46719046347834547</v>
-      </c>
-    </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.52786740395876175</v>
+      </c>
+    </row>
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K53">
         <v>3</v>
       </c>
-      <c r="L53" s="26">
+      <c r="L53" s="25">
         <f t="shared" si="2"/>
-        <v>0.50211912169394013</v>
-      </c>
-    </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.55482784606504931</v>
+      </c>
+    </row>
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K54">
         <v>4</v>
       </c>
-      <c r="L54" s="26">
+      <c r="L54" s="25">
         <f t="shared" si="2"/>
-        <v>0.53704777990953478</v>
-      </c>
-    </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.58178828817133688</v>
+      </c>
+    </row>
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K55">
         <v>5</v>
       </c>
-      <c r="L55" s="26">
+      <c r="L55" s="25">
         <f t="shared" si="2"/>
-        <v>0.57197643812512944</v>
-      </c>
-    </row>
-    <row r="56" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+        <v>0.60874873027762444</v>
+      </c>
+    </row>
+    <row r="56" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>36</v>
       </c>
       <c r="K56">
         <v>6</v>
       </c>
-      <c r="L56" s="26">
+      <c r="L56" s="25">
         <f t="shared" si="2"/>
-        <v>0.60690509634072409</v>
+        <v>0.63570917238391189</v>
       </c>
       <c r="O56" t="s">
         <v>9</v>
@@ -12181,13 +12135,13 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K57">
         <v>7</v>
       </c>
-      <c r="L57" s="26">
+      <c r="L57" s="25">
         <f t="shared" si="2"/>
-        <v>0.64183375455631864</v>
+        <v>0.66266961449019945</v>
       </c>
       <c r="O57" t="s">
         <v>10</v>
@@ -12196,16 +12150,16 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
       <c r="K58">
         <v>8</v>
       </c>
-      <c r="L58" s="26">
+      <c r="L58" s="25">
         <f t="shared" si="2"/>
-        <v>0.6767624127719134</v>
+        <v>0.68963005659648702</v>
       </c>
       <c r="O58" t="s">
         <v>11</v>
@@ -12214,39 +12168,39 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
       <c r="K59">
         <v>9</v>
       </c>
-      <c r="L59" s="26">
+      <c r="L59" s="25">
         <f t="shared" si="2"/>
-        <v>0.71169107098750795</v>
-      </c>
-    </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.71659049870277458</v>
+      </c>
+    </row>
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K60">
         <v>10</v>
       </c>
-      <c r="L60" s="26">
+      <c r="L60" s="25">
         <f t="shared" si="2"/>
-        <v>0.74661972920310271</v>
-      </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+        <v>0.74355094080906214</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K61">
         <v>11</v>
       </c>
-      <c r="L61" s="26">
+      <c r="L61" s="25">
         <f t="shared" si="2"/>
-        <v>0.78154838741869725</v>
+        <v>0.7705113829153496</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M31">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
Modifed rate per day change chart for Wikipedia
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="13" documentId="8_{230E8A76-DF52-4638-8471-66C904E26DEC}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{87D557A9-9814-4719-BB29-8770E8BBCFD7}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D939174-7BFA-4CA8-B8D3-6A5F92FF22D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day-1" sheetId="1" r:id="rId1"/>
@@ -183,7 +183,7 @@
 </file>
 
 <file path=xl/metadata.xml><?xml version="1.0" encoding="utf-8"?>
-<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xlrd="http://schemas.microsoft.com/office/spreadsheetml/2017/richdata" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
+<metadata xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:xda="http://schemas.microsoft.com/office/spreadsheetml/2017/dynamicarray">
   <metadataTypes count="1">
     <metadataType name="XLDAPR" minSupportedVersion="120000" copy="1" pasteAll="1" pasteValues="1" merge="1" splitFirst="1" rowColShift="1" clearFormats="1" clearComments="1" assign="1" coerce="1" cellMeta="1"/>
   </metadataTypes>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="168" uniqueCount="47">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="48">
   <si>
     <t>FROM:</t>
   </si>
@@ -346,6 +346,9 @@
   </si>
   <si>
     <t>Burn Rate (lbs/day)</t>
+  </si>
+  <si>
+    <t>The burn rate reduces by 0.02 lbs/day per lb of propane</t>
   </si>
 </sst>
 </file>
@@ -652,7 +655,7 @@
     <xf numFmtId="0" fontId="14" fillId="7" borderId="0" applyNumberFormat="0" applyAlignment="0" applyProtection="0"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" applyNumberFormat="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="27">
+  <cellXfs count="26">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="5" fillId="3" borderId="0" xfId="7"/>
     <xf numFmtId="0" fontId="6" fillId="4" borderId="0" xfId="8"/>
@@ -691,7 +694,6 @@
     <xf numFmtId="0" fontId="0" fillId="0" borderId="5" xfId="0" applyBorder="1"/>
     <xf numFmtId="0" fontId="13" fillId="0" borderId="0" xfId="16"/>
     <xf numFmtId="166" fontId="0" fillId="0" borderId="0" xfId="0" applyNumberFormat="1"/>
-    <xf numFmtId="22" fontId="0" fillId="0" borderId="3" xfId="0" applyNumberFormat="1" applyBorder="1"/>
   </cellXfs>
   <cellStyles count="17">
     <cellStyle name="Comment" xfId="9" xr:uid="{C4DDEBC2-DCD2-4316-AAE7-A5F6C47DBA99}"/>
@@ -713,6 +715,34 @@
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
   <dxfs count="31">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
+    </dxf>
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -738,7 +768,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -778,13 +808,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
         <left style="thin">
@@ -809,7 +832,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -849,13 +872,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -887,7 +903,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -927,13 +943,6 @@
       </border>
     </dxf>
     <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
-    </dxf>
-    <dxf>
       <border diagonalUp="0" diagonalDown="0">
         <left style="thin">
           <color auto="1"/>
@@ -965,7 +974,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="167" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1003,13 +1012,6 @@
         </vertical>
         <horizontal/>
       </border>
-    </dxf>
-    <dxf>
-      <fill>
-        <patternFill>
-          <bgColor rgb="FFFDF5E9"/>
-        </patternFill>
-      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -8809,8 +8811,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="5257800"/>
-          <a:ext cx="5419725" cy="2743200"/>
+          <a:off x="609600" y="5410200"/>
+          <a:ext cx="5566410" cy="2834640"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -8930,8 +8932,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="6067425"/>
-          <a:ext cx="5419725" cy="2743200"/>
+          <a:off x="609600" y="6248400"/>
+          <a:ext cx="5566410" cy="2834640"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -9087,8 +9089,8 @@
       </xdr:nvGrpSpPr>
       <xdr:grpSpPr>
         <a:xfrm>
-          <a:off x="609600" y="6067425"/>
-          <a:ext cx="5505450" cy="2771775"/>
+          <a:off x="609600" y="6248400"/>
+          <a:ext cx="5650230" cy="2849880"/>
           <a:chOff x="609600" y="5095875"/>
           <a:chExt cx="5419725" cy="2743200"/>
         </a:xfrm>
@@ -9215,60 +9217,132 @@
     </xdr:graphicFrame>
     <xdr:clientData/>
   </xdr:twoCellAnchor>
+  <xdr:twoCellAnchor>
+    <xdr:from>
+      <xdr:col>14</xdr:col>
+      <xdr:colOff>472440</xdr:colOff>
+      <xdr:row>39</xdr:row>
+      <xdr:rowOff>83820</xdr:rowOff>
+    </xdr:from>
+    <xdr:to>
+      <xdr:col>18</xdr:col>
+      <xdr:colOff>518160</xdr:colOff>
+      <xdr:row>42</xdr:row>
+      <xdr:rowOff>53340</xdr:rowOff>
+    </xdr:to>
+    <xdr:sp macro="" textlink="$O$60">
+      <xdr:nvSpPr>
+        <xdr:cNvPr id="6" name="TextBox 5">
+          <a:extLst>
+            <a:ext uri="{FF2B5EF4-FFF2-40B4-BE49-F238E27FC236}">
+              <a16:creationId xmlns:a16="http://schemas.microsoft.com/office/drawing/2014/main" id="{4743A20C-F5A4-7BFD-9CF2-55274D8F66BA}"/>
+            </a:ext>
+          </a:extLst>
+        </xdr:cNvPr>
+        <xdr:cNvSpPr txBox="1"/>
+      </xdr:nvSpPr>
+      <xdr:spPr>
+        <a:xfrm>
+          <a:off x="11323320" y="6667500"/>
+          <a:ext cx="2484120" cy="472440"/>
+        </a:xfrm>
+        <a:prstGeom prst="rect">
+          <a:avLst/>
+        </a:prstGeom>
+        <a:solidFill>
+          <a:schemeClr val="lt1"/>
+        </a:solidFill>
+        <a:ln w="9525" cmpd="sng">
+          <a:noFill/>
+        </a:ln>
+      </xdr:spPr>
+      <xdr:style>
+        <a:lnRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:lnRef>
+        <a:fillRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:fillRef>
+        <a:effectRef idx="0">
+          <a:scrgbClr r="0" g="0" b="0"/>
+        </a:effectRef>
+        <a:fontRef idx="minor">
+          <a:schemeClr val="dk1"/>
+        </a:fontRef>
+      </xdr:style>
+      <xdr:txBody>
+        <a:bodyPr vertOverflow="clip" horzOverflow="clip" wrap="square" rtlCol="0" anchor="t"/>
+        <a:lstStyle/>
+        <a:p>
+          <a:fld id="{7A5887D1-8904-4EA7-B61C-F0AB6002A20D}" type="TxLink">
+            <a:rPr lang="en-US" sz="1000" b="0" i="0" u="none" strike="noStrike">
+              <a:solidFill>
+                <a:srgbClr val="000000"/>
+              </a:solidFill>
+              <a:latin typeface="Consolas"/>
+            </a:rPr>
+            <a:t>The burn rate reduces by 0.02 lbs/day per lb of propane</a:t>
+          </a:fld>
+          <a:endParaRPr lang="en-US" sz="1100"/>
+        </a:p>
+      </xdr:txBody>
+    </xdr:sp>
+    <xdr:clientData/>
+  </xdr:twoCellAnchor>
 </xdr:wsDr>
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="20">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="18" tableBorderDxfId="17">
   <autoFilter ref="B7:D18" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="16"/>
+    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="15">
       <calculatedColumnFormula>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day-2'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="14"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D15" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D15" totalsRowShown="0" headerRowDxfId="13" tableBorderDxfId="12">
   <autoFilter ref="B7:D15" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="11"/>
+    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="10">
       <calculatedColumnFormula>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day-3'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="9"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F9E77B6-A77B-4862-A8B3-E12969205598}" name="_tTankWeight4" displayName="_tTankWeight4" ref="B7:D15" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F9E77B6-A77B-4862-A8B3-E12969205598}" name="_tTankWeight4" displayName="_tTankWeight4" ref="B7:D15" totalsRowShown="0" headerRowDxfId="8" tableBorderDxfId="7">
   <autoFilter ref="B7:D15" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B43DB70-94E1-459B-8FB3-761B425FC480}" name="X" dataDxfId="2"/>
-    <tableColumn id="2" xr3:uid="{182F14ED-38CE-440A-A952-5B718E8962E5}" name="Time (hours)" dataDxfId="1">
+    <tableColumn id="1" xr3:uid="{3B43DB70-94E1-459B-8FB3-761B425FC480}" name="X" dataDxfId="6"/>
+    <tableColumn id="2" xr3:uid="{182F14ED-38CE-440A-A952-5B718E8962E5}" name="Time (hours)" dataDxfId="5">
       <calculatedColumnFormula>(_tTankWeight4[[#This Row],[X]]-INDEX('Propane-Use-Day-4'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CAF6B0C6-7671-4815-AA0F-C7EC06E66BB3}" name="Weight (lbs)" dataDxfId="0"/>
+    <tableColumn id="3" xr3:uid="{CAF6B0C6-7671-4815-AA0F-C7EC06E66BB3}" name="Weight (lbs)" dataDxfId="4"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
@@ -9468,15 +9542,15 @@
       <selection activeCell="P18" sqref="P18"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -9494,7 +9568,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="2" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -9511,7 +9585,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:12" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -9529,7 +9603,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -9539,7 +9613,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -9547,7 +9621,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:12" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:12" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -9570,7 +9644,7 @@
         <v>5</v>
       </c>
     </row>
-    <row r="8" spans="1:12" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:12" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45118.80972222222</v>
       </c>
@@ -9597,7 +9671,7 @@
         <v>28.209872610430022</v>
       </c>
     </row>
-    <row r="9" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45118.810416666667</v>
       </c>
@@ -9624,7 +9698,7 @@
         <v>28.178040868395264</v>
       </c>
     </row>
-    <row r="10" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45119.289583333331</v>
       </c>
@@ -9643,7 +9717,7 @@
         <v>28.146209126360503</v>
       </c>
     </row>
-    <row r="11" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45119.354861111111</v>
       </c>
@@ -9665,7 +9739,7 @@
         <v>28.114377384325746</v>
       </c>
     </row>
-    <row r="12" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45119.390277777777</v>
       </c>
@@ -9695,7 +9769,7 @@
         <v>28.082545642290984</v>
       </c>
     </row>
-    <row r="13" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45119.415277777778</v>
       </c>
@@ -9714,7 +9788,7 @@
         <v>28.050713900256227</v>
       </c>
     </row>
-    <row r="14" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45119.432638888888</v>
       </c>
@@ -9733,7 +9807,7 @@
         <v>28.018882158221469</v>
       </c>
     </row>
-    <row r="15" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45119.465277777781</v>
       </c>
@@ -9753,7 +9827,7 @@
         <v>27.987050416186708</v>
       </c>
     </row>
-    <row r="16" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>45119.48333333333</v>
       </c>
@@ -9772,7 +9846,7 @@
         <v>27.955218674151951</v>
       </c>
     </row>
-    <row r="17" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>45119.513194444444</v>
       </c>
@@ -9791,7 +9865,7 @@
         <v>27.923386932117193</v>
       </c>
     </row>
-    <row r="18" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>45119.53402777778</v>
       </c>
@@ -9810,7 +9884,7 @@
         <v>27.891555190082432</v>
       </c>
     </row>
-    <row r="19" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B19" s="10">
         <v>45119.561111111114</v>
       </c>
@@ -9829,7 +9903,7 @@
         <v>27.859723448047674</v>
       </c>
     </row>
-    <row r="20" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B20" s="10">
         <v>45119.582638888889</v>
       </c>
@@ -9848,7 +9922,7 @@
         <v>27.827891706012913</v>
       </c>
     </row>
-    <row r="21" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B21" s="10">
         <v>45119.633333333331</v>
       </c>
@@ -9867,7 +9941,7 @@
         <v>27.796059963978156</v>
       </c>
     </row>
-    <row r="22" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B22" s="10">
         <v>45119.664583333331</v>
       </c>
@@ -9886,7 +9960,7 @@
         <v>27.764228221943398</v>
       </c>
     </row>
-    <row r="23" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B23" s="20"/>
       <c r="C23" s="21"/>
       <c r="K23" s="14">
@@ -9897,7 +9971,7 @@
         <v>27.732396479908637</v>
       </c>
     </row>
-    <row r="24" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -9906,7 +9980,7 @@
         <v>27.700564737873879</v>
       </c>
     </row>
-    <row r="25" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -9915,7 +9989,7 @@
         <v>27.668732995839122</v>
       </c>
     </row>
-    <row r="26" spans="1:12" ht="15" x14ac:dyDescent="0.25">
+    <row r="26" spans="1:12" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A26" s="3" t="s">
         <v>15</v>
       </c>
@@ -9936,7 +10010,7 @@
         <v>27.636901253804361</v>
       </c>
     </row>
-    <row r="27" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B27" s="4" t="s">
         <v>10</v>
       </c>
@@ -9951,7 +10025,7 @@
         <v>27.605069511769603</v>
       </c>
     </row>
-    <row r="28" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:12" x14ac:dyDescent="0.25">
       <c r="B28" s="4" t="s">
         <v>11</v>
       </c>
@@ -9975,7 +10049,7 @@
         <v>27.573237769734842</v>
       </c>
     </row>
-    <row r="29" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:12" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>20</v>
       </c>
@@ -9994,7 +10068,7 @@
         <v>27.541406027700084</v>
       </c>
     </row>
-    <row r="30" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -10003,7 +10077,7 @@
         <v>27.509574285665327</v>
       </c>
     </row>
-    <row r="31" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -10012,7 +10086,7 @@
         <v>27.477742543630566</v>
       </c>
     </row>
-    <row r="32" spans="1:12" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:12" x14ac:dyDescent="0.25">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -10023,7 +10097,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L32">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="3" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10045,15 +10119,15 @@
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10062,7 +10136,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -10079,7 +10153,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -10097,7 +10171,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -10107,7 +10181,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -10115,7 +10189,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -10141,7 +10215,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45120.291666666664</v>
       </c>
@@ -10172,7 +10246,7 @@
         <v>24.67</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45120.347916666666</v>
       </c>
@@ -10204,7 +10278,7 @@
         <v>24.636269841269844</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45120.377083333333</v>
       </c>
@@ -10227,7 +10301,7 @@
         <v>24.602539682539685</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45120.442361111112</v>
       </c>
@@ -10253,7 +10327,7 @@
         <v>24.568809523809527</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45120.518055555556</v>
       </c>
@@ -10287,7 +10361,7 @@
         <v>24.535079365079365</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45120.540972222225</v>
       </c>
@@ -10310,7 +10384,7 @@
         <v>24.501349206349207</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45120.615277777775</v>
       </c>
@@ -10333,7 +10407,7 @@
         <v>24.467619047619049</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45121.286111111112</v>
       </c>
@@ -10359,7 +10433,7 @@
         <v>24.433888888888891</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B16" s="10">
         <v>45121.354861111111</v>
       </c>
@@ -10389,7 +10463,7 @@
         <v>24.400158730158733</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B17" s="10">
         <v>45121.421527777777</v>
       </c>
@@ -10413,7 +10487,7 @@
         <v>24.366428571428575</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B18" s="10">
         <v>45121.509027777778</v>
       </c>
@@ -10436,7 +10510,7 @@
         <v>24.332698412698413</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B19" s="20"/>
       <c r="C19" s="21"/>
       <c r="K19" s="14">
@@ -10451,7 +10525,7 @@
         <v>24.298968253968255</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="14">
         <v>12</v>
       </c>
@@ -10464,7 +10538,7 @@
         <v>24.265238095238097</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B21" s="4" t="s">
         <v>9</v>
       </c>
@@ -10487,7 +10561,7 @@
         <v>24.231507936507938</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B22" s="4" t="s">
         <v>10</v>
       </c>
@@ -10506,7 +10580,7 @@
         <v>24.19777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B23" s="4" t="s">
         <v>11</v>
       </c>
@@ -10525,7 +10599,7 @@
         <v>24.164047619047622</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F24" s="20"/>
       <c r="K24" s="14">
         <v>16</v>
@@ -10539,7 +10613,7 @@
         <v>24.13031746031746</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -10552,7 +10626,7 @@
         <v>24.096587301587302</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K26" s="14">
         <v>18</v>
       </c>
@@ -10565,7 +10639,7 @@
         <v>24.062857142857144</v>
       </c>
     </row>
-    <row r="27" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="27" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A27" s="3" t="s">
         <v>15</v>
       </c>
@@ -10584,7 +10658,7 @@
         <v>24.029126984126986</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28" s="14">
         <v>20</v>
       </c>
@@ -10597,7 +10671,7 @@
         <v>23.995396825396828</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E29" t="s">
         <v>29</v>
       </c>
@@ -10619,7 +10693,7 @@
         <v>23.96166666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E30" t="s">
         <v>20</v>
       </c>
@@ -10642,7 +10716,7 @@
         <v>23.927936507936511</v>
       </c>
     </row>
-    <row r="31" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="31" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K31" s="14">
         <v>23</v>
       </c>
@@ -10655,7 +10729,7 @@
         <v>23.89420634920635</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K32" s="14">
         <v>24</v>
       </c>
@@ -10668,7 +10742,7 @@
         <v>23.860476190476192</v>
       </c>
     </row>
-    <row r="33" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K33" s="14">
         <v>25</v>
       </c>
@@ -10681,7 +10755,7 @@
         <v>23.826746031746033</v>
       </c>
     </row>
-    <row r="34" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K34" s="14">
         <v>26</v>
       </c>
@@ -10694,7 +10768,7 @@
         <v>23.793015873015875</v>
       </c>
     </row>
-    <row r="35" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K35" s="14">
         <v>27</v>
       </c>
@@ -10707,7 +10781,7 @@
         <v>23.759285714285717</v>
       </c>
     </row>
-    <row r="36" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="36" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K36" s="14">
         <v>28</v>
       </c>
@@ -10720,7 +10794,7 @@
         <v>23.725555555555559</v>
       </c>
     </row>
-    <row r="37" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="37" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K37" s="14">
         <v>29</v>
       </c>
@@ -10733,7 +10807,7 @@
         <v>23.691825396825397</v>
       </c>
     </row>
-    <row r="38" spans="11:13" x14ac:dyDescent="0.2">
+    <row r="38" spans="11:13" x14ac:dyDescent="0.25">
       <c r="K38">
         <v>30</v>
       </c>
@@ -10746,24 +10820,24 @@
         <v>23.658095238095239</v>
       </c>
     </row>
-    <row r="51" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="51" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A51" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="53" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A53" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="54" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A54" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M37 L38:M38">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="2" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -10785,15 +10859,15 @@
       <selection activeCell="D8" sqref="D8"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="15.85546875" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="15.88671875" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -10802,7 +10876,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -10819,7 +10893,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -10837,7 +10911,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -10847,7 +10921,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -10855,7 +10929,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -10881,7 +10955,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45124.356944444444</v>
       </c>
@@ -10912,7 +10986,7 @@
         <v>21.882999999999999</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45124.402083333334</v>
       </c>
@@ -10945,7 +11019,7 @@
         <v>21.849269841269841</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45124.440972222219</v>
       </c>
@@ -10968,7 +11042,7 @@
         <v>21.815539682539683</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45124.493750000001</v>
       </c>
@@ -10994,7 +11068,7 @@
         <v>21.781809523809525</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45124.536111111112</v>
       </c>
@@ -11028,7 +11102,7 @@
         <v>21.748079365079363</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45124.580555555556</v>
       </c>
@@ -11051,7 +11125,7 @@
         <v>21.714349206349205</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B14" s="10">
         <v>45124.622916666667</v>
       </c>
@@ -11074,7 +11148,7 @@
         <v>21.680619047619047</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B15" s="10">
         <v>45124.800694444442</v>
       </c>
@@ -11100,7 +11174,7 @@
         <v>21.646888888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G16" s="22">
         <f>H33/21</f>
         <v>0.80952380952380953</v>
@@ -11120,7 +11194,7 @@
         <v>21.61315873015873</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G17" s="22"/>
       <c r="K17" s="14">
         <v>9</v>
@@ -11134,7 +11208,7 @@
         <v>21.579428571428572</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K18" s="14">
         <v>10</v>
       </c>
@@ -11147,7 +11221,7 @@
         <v>21.54569841269841</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K19" s="14">
         <v>11</v>
       </c>
@@ -11160,7 +11234,7 @@
         <v>21.511968253968252</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K20" s="14">
         <v>12</v>
       </c>
@@ -11173,7 +11247,7 @@
         <v>21.478238095238094</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K21" s="14">
         <v>13</v>
       </c>
@@ -11186,7 +11260,7 @@
         <v>21.444507936507936</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K22" s="14">
         <v>14</v>
       </c>
@@ -11199,7 +11273,7 @@
         <v>21.410777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23" s="14">
         <v>15</v>
       </c>
@@ -11212,7 +11286,7 @@
         <v>21.37704761904762</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -11225,7 +11299,7 @@
         <v>21.343317460317458</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -11238,7 +11312,7 @@
         <v>21.3095873015873</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G26" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
         <v>Measured Propane Burn Rate = 0.64 lbs/day</v>
@@ -11255,7 +11329,7 @@
         <v>21.275857142857141</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27" s="14">
         <v>19</v>
       </c>
@@ -11268,7 +11342,7 @@
         <v>21.242126984126983</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28" s="14">
         <v>20</v>
       </c>
@@ -11281,7 +11355,7 @@
         <v>21.208396825396825</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F29" s="20"/>
       <c r="K29" s="14">
         <v>21</v>
@@ -11295,7 +11369,7 @@
         <v>21.174666666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -11308,7 +11382,7 @@
         <v>21.140936507936509</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -11327,7 +11401,7 @@
         <v>21.107206349206347</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -11344,7 +11418,7 @@
         <v>19</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
@@ -11362,7 +11436,7 @@
         <v>21</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
@@ -11370,7 +11444,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L40" t="s">
         <v>41</v>
       </c>
@@ -11378,7 +11452,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K41">
         <v>21.5</v>
       </c>
@@ -11390,7 +11464,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K42">
         <v>24.55</v>
       </c>
@@ -11402,7 +11476,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K43">
         <v>27.85</v>
       </c>
@@ -11414,24 +11488,24 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="56" spans="1:1" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:1" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>36</v>
       </c>
     </row>
-    <row r="58" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
     </row>
-    <row r="59" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:1" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M31">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="1" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -11449,19 +11523,19 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2660F757-7902-41C1-9127-0A0B0C181624}">
   <dimension ref="A1:P61"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="B13" workbookViewId="0">
-      <selection activeCell="F23" sqref="F23"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="D36" workbookViewId="0">
+      <selection activeCell="J41" sqref="J41"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
+  <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
   <cols>
-    <col min="2" max="2" width="17.140625" customWidth="1"/>
-    <col min="3" max="3" width="15.140625" bestFit="1" customWidth="1"/>
-    <col min="4" max="5" width="15.42578125" bestFit="1" customWidth="1"/>
-    <col min="6" max="6" width="15.140625" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="17.109375" customWidth="1"/>
+    <col min="3" max="3" width="15.109375" bestFit="1" customWidth="1"/>
+    <col min="4" max="5" width="15.44140625" bestFit="1" customWidth="1"/>
+    <col min="6" max="6" width="15.109375" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="1" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -11470,7 +11544,7 @@
       </c>
       <c r="C1" s="2"/>
     </row>
-    <row r="2" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="2" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A2" s="1" t="s">
         <v>2</v>
       </c>
@@ -11487,7 +11561,7 @@
       <c r="I2" s="24"/>
       <c r="J2" s="24"/>
     </row>
-    <row r="3" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="3" spans="1:13" x14ac:dyDescent="0.25">
       <c r="A3" s="1" t="s">
         <v>3</v>
       </c>
@@ -11505,7 +11579,7 @@
       <c r="I3" s="24"/>
       <c r="J3" s="24"/>
     </row>
-    <row r="4" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="4" spans="1:13" x14ac:dyDescent="0.25">
       <c r="E4" s="24" t="s">
         <v>28</v>
       </c>
@@ -11515,7 +11589,7 @@
       <c r="I4" s="24"/>
       <c r="J4" s="24"/>
     </row>
-    <row r="5" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="5" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A5" s="3" t="s">
         <v>14</v>
       </c>
@@ -11523,7 +11597,7 @@
         <v>23</v>
       </c>
     </row>
-    <row r="7" spans="1:13" ht="13.5" thickBot="1" x14ac:dyDescent="0.25">
+    <row r="7" spans="1:13" ht="13.8" thickBot="1" x14ac:dyDescent="0.3">
       <c r="B7" s="7" t="s">
         <v>4</v>
       </c>
@@ -11549,7 +11623,7 @@
         <v>33</v>
       </c>
     </row>
-    <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
+    <row r="8" spans="1:13" ht="13.8" thickTop="1" x14ac:dyDescent="0.25">
       <c r="B8" s="10">
         <v>45125.282638888886</v>
       </c>
@@ -11580,7 +11654,7 @@
         <v>21.13</v>
       </c>
     </row>
-    <row r="9" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="9" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B9" s="10">
         <v>45125.387499999997</v>
       </c>
@@ -11612,7 +11686,7 @@
         <v>21.096269841269841</v>
       </c>
     </row>
-    <row r="10" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="10" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B10" s="10">
         <v>45125.504166666666</v>
       </c>
@@ -11635,7 +11709,7 @@
         <v>21.062539682539683</v>
       </c>
     </row>
-    <row r="11" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="11" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B11" s="10">
         <v>45125.529166666667</v>
       </c>
@@ -11661,7 +11735,7 @@
         <v>21.028809523809525</v>
       </c>
     </row>
-    <row r="12" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="12" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B12" s="10">
         <v>45125.571527777778</v>
       </c>
@@ -11695,7 +11769,7 @@
         <v>20.995079365079363</v>
       </c>
     </row>
-    <row r="13" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="13" spans="1:13" x14ac:dyDescent="0.25">
       <c r="B13" s="10">
         <v>45125.611805555556</v>
       </c>
@@ -11718,8 +11792,8 @@
         <v>20.961349206349205</v>
       </c>
     </row>
-    <row r="14" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B14" s="26">
+    <row r="14" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B14" s="10">
         <v>45125.772222222222</v>
       </c>
       <c r="C14" s="11">
@@ -11741,8 +11815,8 @@
         <v>20.927619047619046</v>
       </c>
     </row>
-    <row r="15" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="B15" s="26">
+    <row r="15" spans="1:13" x14ac:dyDescent="0.25">
+      <c r="B15" s="10">
         <v>45126.34652777778</v>
       </c>
       <c r="C15" s="11">
@@ -11767,7 +11841,7 @@
         <v>20.893888888888888</v>
       </c>
     </row>
-    <row r="16" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="16" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G16" s="22">
         <f>H33/21</f>
         <v>0.80952380952380953</v>
@@ -11787,7 +11861,7 @@
         <v>20.86015873015873</v>
       </c>
     </row>
-    <row r="17" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="17" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G17" s="22"/>
       <c r="K17" s="14">
         <v>9</v>
@@ -11801,7 +11875,7 @@
         <v>20.826428571428572</v>
       </c>
     </row>
-    <row r="18" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="18" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K18" s="14">
         <v>10</v>
       </c>
@@ -11814,7 +11888,7 @@
         <v>20.79269841269841</v>
       </c>
     </row>
-    <row r="19" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="19" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D19">
         <v>20.49</v>
       </c>
@@ -11830,7 +11904,7 @@
         <v>20.758968253968252</v>
       </c>
     </row>
-    <row r="20" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="20" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D20">
         <v>20.48</v>
       </c>
@@ -11846,7 +11920,7 @@
         <v>20.725238095238094</v>
       </c>
     </row>
-    <row r="21" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="21" spans="1:13" x14ac:dyDescent="0.25">
       <c r="D21">
         <v>20.47</v>
       </c>
@@ -11862,7 +11936,7 @@
         <v>20.691507936507936</v>
       </c>
     </row>
-    <row r="22" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="22" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K22" s="14">
         <v>14</v>
       </c>
@@ -11875,7 +11949,7 @@
         <v>20.657777777777778</v>
       </c>
     </row>
-    <row r="23" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="23" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K23" s="14">
         <v>15</v>
       </c>
@@ -11888,7 +11962,7 @@
         <v>20.624047619047619</v>
       </c>
     </row>
-    <row r="24" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="24" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K24" s="14">
         <v>16</v>
       </c>
@@ -11901,7 +11975,7 @@
         <v>20.590317460317458</v>
       </c>
     </row>
-    <row r="25" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="25" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K25" s="14">
         <v>17</v>
       </c>
@@ -11914,7 +11988,7 @@
         <v>20.5565873015873</v>
       </c>
     </row>
-    <row r="26" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="26" spans="1:13" x14ac:dyDescent="0.25">
       <c r="G26" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
         <v>Measured Propane Burn Rate = 0.61 lbs/day</v>
@@ -11931,7 +12005,7 @@
         <v>20.522857142857141</v>
       </c>
     </row>
-    <row r="27" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="27" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K27" s="14">
         <v>19</v>
       </c>
@@ -11944,7 +12018,7 @@
         <v>20.489126984126983</v>
       </c>
     </row>
-    <row r="28" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="28" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K28" s="14">
         <v>20</v>
       </c>
@@ -11957,7 +12031,7 @@
         <v>20.455396825396825</v>
       </c>
     </row>
-    <row r="29" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="29" spans="1:13" x14ac:dyDescent="0.25">
       <c r="F29" s="20"/>
       <c r="K29" s="14">
         <v>21</v>
@@ -11971,7 +12045,7 @@
         <v>20.421666666666667</v>
       </c>
     </row>
-    <row r="30" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="30" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K30" s="14">
         <v>22</v>
       </c>
@@ -11984,7 +12058,7 @@
         <v>20.387936507936509</v>
       </c>
     </row>
-    <row r="31" spans="1:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="31" spans="1:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A31" s="3" t="s">
         <v>15</v>
       </c>
@@ -12003,7 +12077,7 @@
         <v>20.354206349206347</v>
       </c>
     </row>
-    <row r="32" spans="1:13" x14ac:dyDescent="0.2">
+    <row r="32" spans="1:13" x14ac:dyDescent="0.25">
       <c r="K32">
         <v>24</v>
       </c>
@@ -12016,7 +12090,7 @@
         <v>20.320476190476189</v>
       </c>
     </row>
-    <row r="33" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="33" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B33" s="4" t="s">
         <v>9</v>
       </c>
@@ -12044,7 +12118,7 @@
         <v>20.286746031746031</v>
       </c>
     </row>
-    <row r="34" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="34" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B34" s="4" t="s">
         <v>10</v>
       </c>
@@ -12073,7 +12147,7 @@
         <v>20.253015873015872</v>
       </c>
     </row>
-    <row r="35" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="35" spans="2:13" x14ac:dyDescent="0.25">
       <c r="B35" s="4" t="s">
         <v>11</v>
       </c>
@@ -12081,7 +12155,7 @@
         <v>25</v>
       </c>
     </row>
-    <row r="40" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="40" spans="2:13" x14ac:dyDescent="0.25">
       <c r="L40" t="s">
         <v>41</v>
       </c>
@@ -12089,7 +12163,7 @@
         <v>40</v>
       </c>
     </row>
-    <row r="41" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="41" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K41">
         <v>21.13</v>
       </c>
@@ -12102,7 +12176,7 @@
         <v>0.60885148818818891</v>
       </c>
     </row>
-    <row r="42" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="42" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K42">
         <v>21.88</v>
       </c>
@@ -12114,7 +12188,7 @@
         <v>0.64</v>
       </c>
     </row>
-    <row r="43" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="43" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K43">
         <v>24.67</v>
       </c>
@@ -12126,7 +12200,7 @@
         <v>0.7</v>
       </c>
     </row>
-    <row r="44" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="44" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K44">
         <v>28.11</v>
       </c>
@@ -12138,12 +12212,12 @@
         <v>0.76</v>
       </c>
     </row>
-    <row r="46" spans="2:13" ht="15" x14ac:dyDescent="0.25">
+    <row r="46" spans="2:13" ht="14.4" x14ac:dyDescent="0.3">
       <c r="K46" s="3" t="s">
         <v>43</v>
       </c>
     </row>
-    <row r="47" spans="2:13" x14ac:dyDescent="0.2">
+    <row r="47" spans="2:13" x14ac:dyDescent="0.25">
       <c r="K47" cm="1">
         <f t="array" ref="K47:L47">LINEST(M41:M44,L41:L44)</f>
         <v>2.0977517820843509E-2</v>
@@ -12152,12 +12226,12 @@
         <v>0.53147156698673692</v>
       </c>
     </row>
-    <row r="49" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="49" spans="1:16" x14ac:dyDescent="0.25">
       <c r="L49" t="s">
         <v>5</v>
       </c>
     </row>
-    <row r="50" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="50" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K50" cm="1">
         <f t="array" ref="K50:K61">_xlfn.SEQUENCE(12,1,0,1)</f>
         <v>0</v>
@@ -12167,7 +12241,7 @@
         <v>0.53147156698673692</v>
       </c>
     </row>
-    <row r="51" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="51" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K51">
         <v>1</v>
       </c>
@@ -12176,7 +12250,7 @@
         <v>0.55244908480758048</v>
       </c>
     </row>
-    <row r="52" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="52" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K52">
         <v>2</v>
       </c>
@@ -12185,7 +12259,7 @@
         <v>0.57342660262842393</v>
       </c>
     </row>
-    <row r="53" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="53" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K53">
         <v>3</v>
       </c>
@@ -12194,7 +12268,7 @@
         <v>0.59440412044926749</v>
       </c>
     </row>
-    <row r="54" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="54" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K54">
         <v>4</v>
       </c>
@@ -12203,7 +12277,7 @@
         <v>0.61538163827011094</v>
       </c>
     </row>
-    <row r="55" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="55" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K55">
         <v>5</v>
       </c>
@@ -12212,7 +12286,7 @@
         <v>0.6363591560909545</v>
       </c>
     </row>
-    <row r="56" spans="1:16" ht="15" x14ac:dyDescent="0.25">
+    <row r="56" spans="1:16" ht="14.4" x14ac:dyDescent="0.3">
       <c r="A56" s="3" t="s">
         <v>36</v>
       </c>
@@ -12230,7 +12304,7 @@
         <v>44</v>
       </c>
     </row>
-    <row r="57" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="57" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K57">
         <v>7</v>
       </c>
@@ -12245,7 +12319,7 @@
         <v>45</v>
       </c>
     </row>
-    <row r="58" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="58" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A58" t="s">
         <v>37</v>
       </c>
@@ -12263,7 +12337,7 @@
         <v>46</v>
       </c>
     </row>
-    <row r="59" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="59" spans="1:16" x14ac:dyDescent="0.25">
       <c r="A59" t="s">
         <v>38</v>
       </c>
@@ -12275,7 +12349,7 @@
         <v>0.72026922737432852</v>
       </c>
     </row>
-    <row r="60" spans="1:16" x14ac:dyDescent="0.2">
+    <row r="60" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K60">
         <v>10</v>
       </c>
@@ -12283,8 +12357,11 @@
         <f t="shared" si="5"/>
         <v>0.74124674519517197</v>
       </c>
-    </row>
-    <row r="61" spans="1:16" x14ac:dyDescent="0.2">
+      <c r="O60" t="s">
+        <v>47</v>
+      </c>
+    </row>
+    <row r="61" spans="1:16" x14ac:dyDescent="0.25">
       <c r="K61">
         <v>11</v>
       </c>
@@ -12295,7 +12372,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M31 L32:M34">
-    <cfRule type="expression" dxfId="5" priority="1">
+    <cfRule type="expression" dxfId="0" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>

</xml_diff>

<commit_message>
I noticed that all my data is for low tank levels
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{4D939174-7BFA-4CA8-B8D3-6A5F92FF22D9}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B22B34-7534-4FE8-8A0E-6D6DCBDBA67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -205,7 +205,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="169" uniqueCount="48">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="170" uniqueCount="49">
   <si>
     <t>FROM:</t>
   </si>
@@ -349,6 +349,9 @@
   </si>
   <si>
     <t>The burn rate reduces by 0.02 lbs/day per lb of propane</t>
+  </si>
+  <si>
+    <t>I believe the mean burn rate will end up somewhere around the vendor spec of 0.81 lb/day.</t>
   </si>
 </sst>
 </file>
@@ -9281,6 +9284,7 @@
               </a:solidFill>
               <a:latin typeface="Consolas"/>
             </a:rPr>
+            <a:pPr/>
             <a:t>The burn rate reduces by 0.02 lbs/day per lb of propane</a:t>
           </a:fld>
           <a:endParaRPr lang="en-US" sz="1100"/>
@@ -11521,10 +11525,10 @@
 
 <file path=xl/worksheets/sheet4.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{2660F757-7902-41C1-9127-0A0B0C181624}">
-  <dimension ref="A1:P61"/>
+  <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="J41" sqref="J41"/>
+      <selection activeCell="V53" sqref="V53"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>
@@ -12368,6 +12372,11 @@
       <c r="L61" s="25">
         <f t="shared" si="5"/>
         <v>0.76222426301601554</v>
+      </c>
+    </row>
+    <row r="62" spans="1:16" x14ac:dyDescent="0.25">
+      <c r="O62" t="s">
+        <v>48</v>
       </c>
     </row>
   </sheetData>

</xml_diff>

<commit_message>
More changes related to Wikipedia release
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{76B22B34-7534-4FE8-8A0E-6D6DCBDBA67D}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2C3E1D1C-DBA8-4AC3-93E4-3DD9BAF87196}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" activeTab="3" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
@@ -11528,7 +11528,7 @@
   <dimension ref="A1:P62"/>
   <sheetViews>
     <sheetView showGridLines="0" tabSelected="1" topLeftCell="D36" workbookViewId="0">
-      <selection activeCell="V53" sqref="V53"/>
+      <selection activeCell="K38" sqref="K38"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="13.2" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
Added another data point. Really, I should have started a new tab. At least I recorded the data.
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="25601"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="7" rupBuild="26626"/>
   <workbookPr codeName="ThisWorkbook"/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="155" documentId="8_{E52E9538-16AC-4C83-9985-386637D8DDE3}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2ECCBFE6-5F36-4EA7-A423-06C26C9E69F8}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{52081596-3D92-467C-ABA0-8565FC5BBA9A}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day-1" sheetId="1" r:id="rId1"/>
@@ -886,7 +886,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="168" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -950,7 +950,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="168" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1021,7 +1021,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="168" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -1092,7 +1092,7 @@
       </border>
     </dxf>
     <dxf>
-      <numFmt numFmtId="27" formatCode="dd/mm/yy\ h:mm"/>
+      <numFmt numFmtId="168" formatCode="dd/mm/yy\ h:mm"/>
       <border diagonalUp="0" diagonalDown="0">
         <left/>
         <right style="thin">
@@ -5628,10 +5628,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-5'!$C$10:$C$16</c:f>
+              <c:f>'Propane-Use-Day-5'!$C$10:$C$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5652,16 +5652,19 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>23.25</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>42.616666666755918</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-5'!$D$10:$D$16</c:f>
+              <c:f>'Propane-Use-Day-5'!$D$10:$D$17</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="7"/>
+                <c:ptCount val="8"/>
                 <c:pt idx="0">
                   <c:v>36.9</c:v>
                 </c:pt>
@@ -5682,6 +5685,9 @@
                 </c:pt>
                 <c:pt idx="6">
                   <c:v>36.159999999999997</c:v>
+                </c:pt>
+                <c:pt idx="7">
+                  <c:v>35.646666670000002</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5721,82 +5727,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5811,82 +5817,82 @@
                   <c:v>37.418489282725538</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>37.363365286694354</c:v>
+                  <c:v>37.308241290663169</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>37.308241290663169</c:v>
+                  <c:v>37.1979932986008</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>37.253117294631984</c:v>
+                  <c:v>37.08774530653843</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>37.1979932986008</c:v>
+                  <c:v>36.977497314476054</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>37.142869302569615</c:v>
+                  <c:v>36.867249322413684</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>37.08774530653843</c:v>
+                  <c:v>36.757001330351315</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>37.032621310507245</c:v>
+                  <c:v>36.646753338288946</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.977497314476054</c:v>
+                  <c:v>36.536505346226576</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.922373318444869</c:v>
+                  <c:v>36.426257354164207</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.867249322413684</c:v>
+                  <c:v>36.316009362101838</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.8121253263825</c:v>
+                  <c:v>36.205761370039468</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.757001330351315</c:v>
+                  <c:v>36.095513377977092</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.70187733432013</c:v>
+                  <c:v>35.985265385914722</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.646753338288946</c:v>
+                  <c:v>35.875017393852353</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36.591629342257761</c:v>
+                  <c:v>35.764769401789984</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36.536505346226576</c:v>
+                  <c:v>35.654521409727614</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36.481381350195392</c:v>
+                  <c:v>35.544273417665245</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.426257354164207</c:v>
+                  <c:v>35.434025425602876</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.371133358133022</c:v>
+                  <c:v>35.323777433540499</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.316009362101838</c:v>
+                  <c:v>35.21352944147813</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.260885366070653</c:v>
+                  <c:v>35.103281449415761</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.205761370039468</c:v>
+                  <c:v>34.993033457353391</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.150637374008276</c:v>
+                  <c:v>34.882785465291022</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36.095513377977092</c:v>
+                  <c:v>34.772537473228653</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.040389381945907</c:v>
+                  <c:v>34.662289481166283</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35.985265385914722</c:v>
+                  <c:v>34.552041489103914</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5926,82 +5932,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>1</c:v>
+                  <c:v>2</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>2</c:v>
+                  <c:v>4</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>3</c:v>
+                  <c:v>6</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>4</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>5</c:v>
+                  <c:v>10</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>6</c:v>
+                  <c:v>12</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>7</c:v>
+                  <c:v>14</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>8</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>9</c:v>
+                  <c:v>18</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>10</c:v>
+                  <c:v>20</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>11</c:v>
+                  <c:v>22</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>12</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>13</c:v>
+                  <c:v>26</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>14</c:v>
+                  <c:v>28</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>15</c:v>
+                  <c:v>30</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>16</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>17</c:v>
+                  <c:v>34</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>18</c:v>
+                  <c:v>36</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>19</c:v>
+                  <c:v>38</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>20</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>21</c:v>
+                  <c:v>42</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>22</c:v>
+                  <c:v>44</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>23</c:v>
+                  <c:v>46</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>24</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>25</c:v>
+                  <c:v>50</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>26</c:v>
+                  <c:v>52</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6016,82 +6022,82 @@
                   <c:v>36.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.86626984126984</c:v>
+                  <c:v>36.832539682539682</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.832539682539682</c:v>
+                  <c:v>36.765079365079366</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.798809523809524</c:v>
+                  <c:v>36.69761904761905</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.765079365079366</c:v>
+                  <c:v>36.630158730158726</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.731349206349208</c:v>
+                  <c:v>36.56269841269841</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.69761904761905</c:v>
+                  <c:v>36.495238095238093</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.663888888888884</c:v>
+                  <c:v>36.427777777777777</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.630158730158726</c:v>
+                  <c:v>36.360317460317461</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.596428571428568</c:v>
+                  <c:v>36.292857142857144</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.56269841269841</c:v>
+                  <c:v>36.225396825396821</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.528968253968252</c:v>
+                  <c:v>36.157936507936505</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.495238095238093</c:v>
+                  <c:v>36.090476190476188</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.461507936507935</c:v>
+                  <c:v>36.023015873015872</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.427777777777777</c:v>
+                  <c:v>35.955555555555556</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36.394047619047619</c:v>
+                  <c:v>35.888095238095239</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>36.360317460317461</c:v>
+                  <c:v>35.820634920634916</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>36.326587301587303</c:v>
+                  <c:v>35.7531746031746</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>36.292857142857144</c:v>
+                  <c:v>35.685714285714283</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>36.259126984126979</c:v>
+                  <c:v>35.618253968253967</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>36.225396825396821</c:v>
+                  <c:v>35.550793650793651</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>36.191666666666663</c:v>
+                  <c:v>35.483333333333334</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>36.157936507936505</c:v>
+                  <c:v>35.415873015873018</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>36.124206349206347</c:v>
+                  <c:v>35.348412698412695</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>36.090476190476188</c:v>
+                  <c:v>35.280952380952378</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>36.05674603174603</c:v>
+                  <c:v>35.213492063492062</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>36.023015873015872</c:v>
+                  <c:v>35.146031746031746</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12299,8 +12305,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C2640CD-FE65-4A9C-96E2-4EB4B7A88B35}" name="_tTankWeight46" displayName="_tTankWeight46" ref="B9:D16" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="B9:D16" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C2640CD-FE65-4A9C-96E2-4EB4B7A88B35}" name="_tTankWeight46" displayName="_tTankWeight46" ref="B9:D17" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B9:D17" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5E8842F1-EA49-43DF-A3E1-1B5CC76346AB}" name="X" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{36D8FF9C-5836-47BE-A23B-22C78B1E531D}" name="Time (hours)" dataDxfId="6">
@@ -15359,8 +15365,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1512FE03-6F96-4002-83C1-8201B1986D54}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A37" workbookViewId="0">
-      <selection activeCell="I46" sqref="I46"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A13" workbookViewId="0">
+      <selection activeCell="E27" sqref="E27"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15456,14 +15462,14 @@
     </row>
     <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="G8" s="17" cm="1">
-        <f t="array" ref="G8:H8">LINEST(_xlfn.DROP(_tTankWeight46[Weight (lbs)],2),_xlfn.DROP(_tTankWeight46[Time (hours)],2))</f>
+        <f t="array" ref="G8:H8">LINEST(_xlfn.DROP(_xlfn.DROP(_tTankWeight46[Weight (lbs)],2),-1),_xlfn.DROP(_xlfn.DROP(_tTankWeight46[Time (hours)],2),-1))</f>
         <v>-5.5123996031185153E-2</v>
       </c>
       <c r="H8" s="17">
         <v>37.418489282725538</v>
       </c>
       <c r="K8" s="14" cm="1">
-        <f t="array" ref="K8:K34">_xlfn.SEQUENCE(27,1,0,1)</f>
+        <f t="array" ref="K8:K34">_xlfn.SEQUENCE(27,1,0,2)</f>
         <v>0</v>
       </c>
       <c r="L8" s="15">
@@ -15495,15 +15501,15 @@
         <v>19</v>
       </c>
       <c r="K9" s="14">
-        <v>1</v>
+        <v>2</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" ref="L9:L31" si="0">_nInt+_nSlope*K9</f>
-        <v>37.363365286694354</v>
+        <v>37.308241290663169</v>
       </c>
       <c r="M9" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K9</f>
-        <v>36.86626984126984</v>
+        <v>36.832539682539682</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -15518,15 +15524,15 @@
         <v>36.9</v>
       </c>
       <c r="K10" s="14">
-        <v>2</v>
+        <v>4</v>
       </c>
       <c r="L10" s="15">
         <f t="shared" si="0"/>
-        <v>37.308241290663169</v>
+        <v>37.1979932986008</v>
       </c>
       <c r="M10" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K10</f>
-        <v>36.832539682539682</v>
+        <v>36.765079365079366</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -15544,15 +15550,15 @@
         <v>17</v>
       </c>
       <c r="K11" s="14">
-        <v>3</v>
+        <v>6</v>
       </c>
       <c r="L11" s="15">
         <f t="shared" si="0"/>
-        <v>37.253117294631984</v>
+        <v>37.08774530653843</v>
       </c>
       <c r="M11" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K11</f>
-        <v>36.798809523809524</v>
+        <v>36.69761904761905</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -15578,15 +15584,15 @@
         <v>=ABS(24*_nSlope)</v>
       </c>
       <c r="K12" s="14">
-        <v>4</v>
+        <v>8</v>
       </c>
       <c r="L12" s="15">
         <f t="shared" si="0"/>
-        <v>37.1979932986008</v>
+        <v>36.977497314476054</v>
       </c>
       <c r="M12" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K12</f>
-        <v>36.765079365079366</v>
+        <v>36.630158730158726</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -15601,15 +15607,15 @@
         <v>36.416666669999998</v>
       </c>
       <c r="K13" s="14">
-        <v>5</v>
+        <v>10</v>
       </c>
       <c r="L13" s="15">
         <f t="shared" si="0"/>
-        <v>37.142869302569615</v>
+        <v>36.867249322413684</v>
       </c>
       <c r="M13" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K13</f>
-        <v>36.731349206349208</v>
+        <v>36.56269841269841</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -15624,15 +15630,15 @@
         <v>36.31</v>
       </c>
       <c r="K14" s="14">
-        <v>6</v>
+        <v>12</v>
       </c>
       <c r="L14" s="15">
         <f t="shared" si="0"/>
-        <v>37.08774530653843</v>
+        <v>36.757001330351315</v>
       </c>
       <c r="M14" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K14</f>
-        <v>36.69761904761905</v>
+        <v>36.495238095238093</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -15650,15 +15656,15 @@
         <v>34</v>
       </c>
       <c r="K15" s="14">
-        <v>7</v>
+        <v>14</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" si="0"/>
-        <v>37.032621310507245</v>
+        <v>36.646753338288946</v>
       </c>
       <c r="M15" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K15</f>
-        <v>36.663888888888884</v>
+        <v>36.427777777777777</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -15680,263 +15686,273 @@
         <v>22</v>
       </c>
       <c r="K16" s="14">
-        <v>8</v>
+        <v>16</v>
       </c>
       <c r="L16" s="15">
         <f t="shared" si="0"/>
-        <v>36.977497314476054</v>
+        <v>36.536505346226576</v>
       </c>
       <c r="M16" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K16</f>
-        <v>36.630158730158726</v>
-      </c>
-    </row>
-    <row r="17" spans="3:13" x14ac:dyDescent="0.2">
+        <v>36.360317460317461</v>
+      </c>
+    </row>
+    <row r="17" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B17" s="26">
+        <v>45143.379861111112</v>
+      </c>
+      <c r="C17" s="11">
+        <f>(_tTankWeight46[[#This Row],[X]]-INDEX('Propane-Use-Day-5'!$B$10,1,1))*24</f>
+        <v>42.616666666755918</v>
+      </c>
+      <c r="D17" s="19">
+        <v>35.646666670000002</v>
+      </c>
       <c r="G17" s="22"/>
       <c r="K17" s="14">
-        <v>9</v>
+        <v>18</v>
       </c>
       <c r="L17" s="15">
         <f t="shared" si="0"/>
-        <v>36.922373318444869</v>
+        <v>36.426257354164207</v>
       </c>
       <c r="M17" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K17</f>
-        <v>36.596428571428568</v>
-      </c>
-    </row>
-    <row r="18" spans="3:13" x14ac:dyDescent="0.2">
+        <v>36.292857142857144</v>
+      </c>
+    </row>
+    <row r="18" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K18" s="14">
-        <v>10</v>
+        <v>20</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="0"/>
-        <v>36.867249322413684</v>
+        <v>36.316009362101838</v>
       </c>
       <c r="M18" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K18</f>
-        <v>36.56269841269841</v>
-      </c>
-    </row>
-    <row r="19" spans="3:13" x14ac:dyDescent="0.2">
+        <v>36.225396825396821</v>
+      </c>
+    </row>
+    <row r="19" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K19" s="14">
-        <v>11</v>
+        <v>22</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>36.8121253263825</v>
+        <v>36.205761370039468</v>
       </c>
       <c r="M19" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K19</f>
-        <v>36.528968253968252</v>
-      </c>
-    </row>
-    <row r="20" spans="3:13" x14ac:dyDescent="0.2">
+        <v>36.157936507936505</v>
+      </c>
+    </row>
+    <row r="20" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K20" s="14">
-        <v>12</v>
+        <v>24</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>36.757001330351315</v>
+        <v>36.095513377977092</v>
       </c>
       <c r="M20" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K20</f>
-        <v>36.495238095238093</v>
-      </c>
-    </row>
-    <row r="21" spans="3:13" x14ac:dyDescent="0.2">
+        <v>36.090476190476188</v>
+      </c>
+    </row>
+    <row r="21" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K21" s="14">
-        <v>13</v>
+        <v>26</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="0"/>
-        <v>36.70187733432013</v>
+        <v>35.985265385914722</v>
       </c>
       <c r="M21" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K21</f>
-        <v>36.461507936507935</v>
-      </c>
-    </row>
-    <row r="22" spans="3:13" x14ac:dyDescent="0.2">
+        <v>36.023015873015872</v>
+      </c>
+    </row>
+    <row r="22" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K22" s="14">
-        <v>14</v>
+        <v>28</v>
       </c>
       <c r="L22" s="15">
         <f t="shared" si="0"/>
-        <v>36.646753338288946</v>
+        <v>35.875017393852353</v>
       </c>
       <c r="M22" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K22</f>
-        <v>36.427777777777777</v>
-      </c>
-    </row>
-    <row r="23" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.955555555555556</v>
+      </c>
+    </row>
+    <row r="23" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K23" s="14">
-        <v>15</v>
+        <v>30</v>
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>36.591629342257761</v>
+        <v>35.764769401789984</v>
       </c>
       <c r="M23" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K23</f>
-        <v>36.394047619047619</v>
-      </c>
-    </row>
-    <row r="24" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.888095238095239</v>
+      </c>
+    </row>
+    <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K24" s="14">
-        <v>16</v>
+        <v>32</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>36.536505346226576</v>
+        <v>35.654521409727614</v>
       </c>
       <c r="M24" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K24</f>
-        <v>36.360317460317461</v>
-      </c>
-    </row>
-    <row r="25" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.820634920634916</v>
+      </c>
+    </row>
+    <row r="25" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K25" s="14">
-        <v>17</v>
+        <v>34</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="0"/>
-        <v>36.481381350195392</v>
+        <v>35.544273417665245</v>
       </c>
       <c r="M25" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K25</f>
-        <v>36.326587301587303</v>
-      </c>
-    </row>
-    <row r="26" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.7531746031746</v>
+      </c>
+    </row>
+    <row r="26" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K26" s="14">
-        <v>18</v>
+        <v>36</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="0"/>
-        <v>36.426257354164207</v>
+        <v>35.434025425602876</v>
       </c>
       <c r="M26" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K26</f>
-        <v>36.292857142857144</v>
-      </c>
-    </row>
-    <row r="27" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.685714285714283</v>
+      </c>
+    </row>
+    <row r="27" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K27" s="14">
-        <v>19</v>
+        <v>38</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
-        <v>36.371133358133022</v>
+        <v>35.323777433540499</v>
       </c>
       <c r="M27" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K27</f>
-        <v>36.259126984126979</v>
-      </c>
-    </row>
-    <row r="28" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.618253968253967</v>
+      </c>
+    </row>
+    <row r="28" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C28">
-        <v>36.159999999999997</v>
+        <v>35.69</v>
       </c>
       <c r="K28" s="14">
-        <v>20</v>
+        <v>40</v>
       </c>
       <c r="L28" s="15">
         <f t="shared" si="0"/>
-        <v>36.316009362101838</v>
+        <v>35.21352944147813</v>
       </c>
       <c r="M28" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K28</f>
-        <v>36.225396825396821</v>
-      </c>
-    </row>
-    <row r="29" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.550793650793651</v>
+      </c>
+    </row>
+    <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C29">
-        <v>36.19</v>
+        <v>35.65</v>
       </c>
       <c r="K29" s="14">
-        <v>21</v>
+        <v>42</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="0"/>
-        <v>36.260885366070653</v>
+        <v>35.103281449415761</v>
       </c>
       <c r="M29" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K29</f>
-        <v>36.191666666666663</v>
-      </c>
-    </row>
-    <row r="30" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.483333333333334</v>
+      </c>
+    </row>
+    <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="C30">
-        <v>36.130000000000003</v>
+        <v>35.6</v>
       </c>
       <c r="G30" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
         <v>Measured Propane Burn Rate = 1.32 lbs/day</v>
       </c>
       <c r="K30" s="14">
-        <v>22</v>
+        <v>44</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="0"/>
-        <v>36.205761370039468</v>
+        <v>34.993033457353391</v>
       </c>
       <c r="M30" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K30</f>
-        <v>36.157936507936505</v>
-      </c>
-    </row>
-    <row r="31" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.415873015873018</v>
+      </c>
+    </row>
+    <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K31" s="14">
-        <v>23</v>
+        <v>46</v>
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
-        <v>36.150637374008276</v>
+        <v>34.882785465291022</v>
       </c>
       <c r="M31" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K31</f>
-        <v>36.124206349206347</v>
-      </c>
-    </row>
-    <row r="32" spans="3:13" x14ac:dyDescent="0.2">
+        <v>35.348412698412695</v>
+      </c>
+    </row>
+    <row r="32" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K32">
-        <v>24</v>
+        <v>48</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" ref="L32" si="1">_nInt+_nSlope*K32</f>
-        <v>36.095513377977092</v>
+        <v>34.772537473228653</v>
       </c>
       <c r="M32" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K32</f>
-        <v>36.090476190476188</v>
+        <v>35.280952380952378</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K33">
-        <v>25</v>
+        <v>50</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" ref="L33" si="2">_nInt+_nSlope*K33</f>
-        <v>36.040389381945907</v>
+        <v>34.662289481166283</v>
       </c>
       <c r="M33" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K33</f>
-        <v>36.05674603174603</v>
+        <v>35.213492063492062</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
       <c r="K34">
-        <v>26</v>
+        <v>52</v>
       </c>
       <c r="L34" s="15">
         <f t="shared" ref="L34" si="3">_nInt+_nSlope*K34</f>
-        <v>35.985265385914722</v>
+        <v>34.552041489103914</v>
       </c>
       <c r="M34" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K34</f>
-        <v>36.023015873015872</v>
+        <v>35.146031746031746</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -16082,7 +16098,7 @@
         <v>0</v>
       </c>
       <c r="L51" s="25">
-        <f>$L$48+K51*$K$48</f>
+        <f t="shared" ref="L51:L71" si="5">$L$48+K51*$K$48</f>
         <v>0.53564610773587806</v>
       </c>
     </row>
@@ -16091,7 +16107,7 @@
         <v>1</v>
       </c>
       <c r="L52" s="25">
-        <f>$L$48+K52*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.55602290499569373</v>
       </c>
     </row>
@@ -16100,7 +16116,7 @@
         <v>2</v>
       </c>
       <c r="L53" s="25">
-        <f>$L$48+K53*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.57639970225550941</v>
       </c>
     </row>
@@ -16109,7 +16125,7 @@
         <v>3</v>
       </c>
       <c r="L54" s="25">
-        <f>$L$48+K54*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.59677649951532508</v>
       </c>
     </row>
@@ -16118,7 +16134,7 @@
         <v>4</v>
       </c>
       <c r="L55" s="25">
-        <f>$L$48+K55*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.61715329677514075</v>
       </c>
     </row>
@@ -16127,7 +16143,7 @@
         <v>5</v>
       </c>
       <c r="L56" s="25">
-        <f>$L$48+K56*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.63753009403495642</v>
       </c>
       <c r="O56" t="s">
@@ -16142,7 +16158,7 @@
         <v>6</v>
       </c>
       <c r="L57" s="25">
-        <f>$L$48+K57*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.65790689129477209</v>
       </c>
       <c r="O57" t="s">
@@ -16157,7 +16173,7 @@
         <v>7</v>
       </c>
       <c r="L58" s="25">
-        <f>$L$48+K58*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.67828368855458776</v>
       </c>
       <c r="O58" t="s">
@@ -16172,7 +16188,7 @@
         <v>8</v>
       </c>
       <c r="L59" s="25">
-        <f>$L$48+K59*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.69866048581440343</v>
       </c>
     </row>
@@ -16184,7 +16200,7 @@
         <v>9</v>
       </c>
       <c r="L60" s="25">
-        <f>$L$48+K60*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.7190372830742191</v>
       </c>
       <c r="O60" t="s">
@@ -16196,7 +16212,7 @@
         <v>10</v>
       </c>
       <c r="L61" s="25">
-        <f>$L$48+K61*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.73941408033403477</v>
       </c>
     </row>
@@ -16208,7 +16224,7 @@
         <v>11</v>
       </c>
       <c r="L62" s="25">
-        <f>$L$48+K62*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.75979087759385044</v>
       </c>
       <c r="O62" t="s">
@@ -16223,7 +16239,7 @@
         <v>12</v>
       </c>
       <c r="L63" s="25">
-        <f>$L$48+K63*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.78016767485366612</v>
       </c>
     </row>
@@ -16232,7 +16248,7 @@
         <v>13</v>
       </c>
       <c r="L64" s="25">
-        <f>$L$48+K64*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.80054447211348179</v>
       </c>
     </row>
@@ -16241,7 +16257,7 @@
         <v>14</v>
       </c>
       <c r="L65" s="25">
-        <f>$L$48+K65*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.82092126937329746</v>
       </c>
     </row>
@@ -16250,7 +16266,7 @@
         <v>15</v>
       </c>
       <c r="L66" s="25">
-        <f>$L$48+K66*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.84129806663311313</v>
       </c>
     </row>
@@ -16259,7 +16275,7 @@
         <v>16</v>
       </c>
       <c r="L67" s="25">
-        <f>$L$48+K67*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.8616748638929288</v>
       </c>
     </row>
@@ -16268,7 +16284,7 @@
         <v>17</v>
       </c>
       <c r="L68" s="25">
-        <f>$L$48+K68*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.88205166115274447</v>
       </c>
     </row>
@@ -16277,7 +16293,7 @@
         <v>18</v>
       </c>
       <c r="L69" s="25">
-        <f>$L$48+K69*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.90242845841256014</v>
       </c>
     </row>
@@ -16286,7 +16302,7 @@
         <v>19</v>
       </c>
       <c r="L70" s="25">
-        <f>$L$48+K70*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.92280525567237581</v>
       </c>
     </row>
@@ -16295,7 +16311,7 @@
         <v>20</v>
       </c>
       <c r="L71" s="25">
-        <f>$L$48+K71*$K$48</f>
+        <f t="shared" si="5"/>
         <v>0.94318205293219148</v>
       </c>
     </row>

</xml_diff>

<commit_message>
Last data for today
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\mbieg\Dropbox\GitHub\PowerQueryBitsAndPieces\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{020BA218-BFB3-4C51-BD66-44921A96E072}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5E246116-74BE-4AEF-AB9D-4F5B8C8D7C97}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15720" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="5115" yWindow="1755" windowWidth="17280" windowHeight="8880" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day-1" sheetId="1" r:id="rId1"/>
@@ -5628,10 +5628,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-5'!$C$10:$C$18</c:f>
+              <c:f>'Propane-Use-Day-5'!$C$10:$C$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5658,16 +5658,19 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>43.866666666639503</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>45.700000000011642</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-5'!$D$10:$D$18</c:f>
+              <c:f>'Propane-Use-Day-5'!$D$10:$D$19</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="9"/>
+                <c:ptCount val="10"/>
                 <c:pt idx="0">
                   <c:v>36.9</c:v>
                 </c:pt>
@@ -5694,6 +5697,9 @@
                 </c:pt>
                 <c:pt idx="8">
                   <c:v>35.576666670000002</c:v>
+                </c:pt>
+                <c:pt idx="9">
+                  <c:v>35.506666670000001</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5820,85 +5826,85 @@
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>36.956108529046318</c:v>
+                  <c:v>36.955809585575302</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.893183697923526</c:v>
+                  <c:v>36.892914962425309</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.830258866800733</c:v>
+                  <c:v>36.830020339275308</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.767334035677948</c:v>
+                  <c:v>36.767125716125314</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.704409204555155</c:v>
+                  <c:v>36.70423109297532</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.641484373432363</c:v>
+                  <c:v>36.641336469825319</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36.57855954230957</c:v>
+                  <c:v>36.578441846675325</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>36.515634711186785</c:v>
+                  <c:v>36.515547223525331</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>36.452709880063992</c:v>
+                  <c:v>36.45265260037533</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>36.389785048941199</c:v>
+                  <c:v>36.389757977225337</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>36.326860217818407</c:v>
+                  <c:v>36.326863354075343</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>36.263935386695621</c:v>
+                  <c:v>36.263968730925349</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>36.201010555572829</c:v>
+                  <c:v>36.201074107775348</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>36.138085724450036</c:v>
+                  <c:v>36.138179484625354</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>36.075160893327244</c:v>
+                  <c:v>36.07528486147536</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>36.012236062204451</c:v>
+                  <c:v>36.012390238325359</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>35.949311231081666</c:v>
+                  <c:v>35.949495615175366</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>35.886386399958873</c:v>
+                  <c:v>35.886600992025372</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>35.82346156883608</c:v>
+                  <c:v>35.823706368875371</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>35.760536737713288</c:v>
+                  <c:v>35.760811745725377</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>35.697611906590502</c:v>
+                  <c:v>35.697917122575383</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>35.63468707546771</c:v>
+                  <c:v>35.635022499425382</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>35.571762244344917</c:v>
+                  <c:v>35.572127876275388</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>35.508837413222125</c:v>
+                  <c:v>35.509233253125394</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>35.445912582099339</c:v>
+                  <c:v>35.446338629975394</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>35.382987750976547</c:v>
+                  <c:v>35.3834440068254</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>35.320062919853754</c:v>
+                  <c:v>35.320549383675406</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -12131,7 +12137,7 @@
                 <a:latin typeface="Consolas"/>
               </a:rPr>
               <a:pPr/>
-              <a:t>Measured Propane Burn Rate = 0.76 lbs/day</a:t>
+              <a:t>Measured Propane Burn Rate = 0.75 lbs/day</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="1100" b="1"/>
           </a:p>
@@ -12311,8 +12317,8 @@
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C2640CD-FE65-4A9C-96E2-4EB4B7A88B35}" name="_tTankWeight46" displayName="_tTankWeight46" ref="B9:D18" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
-  <autoFilter ref="B9:D18" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C2640CD-FE65-4A9C-96E2-4EB4B7A88B35}" name="_tTankWeight46" displayName="_tTankWeight46" ref="B9:D19" totalsRowShown="0" headerRowDxfId="9" tableBorderDxfId="8">
+  <autoFilter ref="B9:D19" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5E8842F1-EA49-43DF-A3E1-1B5CC76346AB}" name="X" dataDxfId="7"/>
     <tableColumn id="2" xr3:uid="{36D8FF9C-5836-47BE-A23B-22C78B1E531D}" name="Time (hours)" dataDxfId="6">
@@ -15371,8 +15377,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1512FE03-6F96-4002-83C1-8201B1986D54}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A16" workbookViewId="0">
-      <selection activeCell="D34" sqref="D34"/>
+    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
+      <selection activeCell="L3" sqref="L3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15469,10 +15475,10 @@
     <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="G8" s="17" cm="1">
         <f t="array" ref="G8:H8">LINEST(_xlfn.DROP(_xlfn.DROP(_tTankWeight46[Weight (lbs)],2),-1),_xlfn.DROP(_xlfn.DROP(_tTankWeight46[Time (hours)],2),-1))</f>
-        <v>-3.1462415561395465E-2</v>
+        <v>-3.1447311574998034E-2</v>
       </c>
       <c r="H8" s="17">
-        <v>36.956108529046318</v>
+        <v>36.955809585575302</v>
       </c>
       <c r="K8" s="14" cm="1">
         <f t="array" ref="K8:K34">_xlfn.SEQUENCE(27,1,0,2)</f>
@@ -15480,7 +15486,7 @@
       </c>
       <c r="L8" s="15">
         <f>_nInt+_nSlope*K8</f>
-        <v>36.956108529046318</v>
+        <v>36.955809585575302</v>
       </c>
       <c r="M8" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K8</f>
@@ -15511,7 +15517,7 @@
       </c>
       <c r="L9" s="15">
         <f t="shared" ref="L9:L31" si="0">_nInt+_nSlope*K9</f>
-        <v>36.893183697923526</v>
+        <v>36.892914962425309</v>
       </c>
       <c r="M9" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K9</f>
@@ -15534,7 +15540,7 @@
       </c>
       <c r="L10" s="15">
         <f t="shared" si="0"/>
-        <v>36.830258866800733</v>
+        <v>36.830020339275308</v>
       </c>
       <c r="M10" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K10</f>
@@ -15560,7 +15566,7 @@
       </c>
       <c r="L11" s="15">
         <f t="shared" si="0"/>
-        <v>36.767334035677948</v>
+        <v>36.767125716125314</v>
       </c>
       <c r="M11" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K11</f>
@@ -15580,7 +15586,7 @@
       </c>
       <c r="G12" s="22">
         <f>ABS(24*_nSlope)</f>
-        <v>0.75509797347349117</v>
+        <v>0.75473547779995287</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -15594,7 +15600,7 @@
       </c>
       <c r="L12" s="15">
         <f t="shared" si="0"/>
-        <v>36.704409204555155</v>
+        <v>36.70423109297532</v>
       </c>
       <c r="M12" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K12</f>
@@ -15617,7 +15623,7 @@
       </c>
       <c r="L13" s="15">
         <f t="shared" si="0"/>
-        <v>36.641484373432363</v>
+        <v>36.641336469825319</v>
       </c>
       <c r="M13" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K13</f>
@@ -15640,7 +15646,7 @@
       </c>
       <c r="L14" s="15">
         <f t="shared" si="0"/>
-        <v>36.57855954230957</v>
+        <v>36.578441846675325</v>
       </c>
       <c r="M14" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K14</f>
@@ -15666,7 +15672,7 @@
       </c>
       <c r="L15" s="15">
         <f t="shared" si="0"/>
-        <v>36.515634711186785</v>
+        <v>36.515547223525331</v>
       </c>
       <c r="M15" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K15</f>
@@ -15696,7 +15702,7 @@
       </c>
       <c r="L16" s="15">
         <f t="shared" si="0"/>
-        <v>36.452709880063992</v>
+        <v>36.45265260037533</v>
       </c>
       <c r="M16" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K16</f>
@@ -15720,7 +15726,7 @@
       </c>
       <c r="L17" s="15">
         <f t="shared" si="0"/>
-        <v>36.389785048941199</v>
+        <v>36.389757977225337</v>
       </c>
       <c r="M17" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K17</f>
@@ -15743,7 +15749,7 @@
       </c>
       <c r="L18" s="15">
         <f t="shared" si="0"/>
-        <v>36.326860217818407</v>
+        <v>36.326863354075343</v>
       </c>
       <c r="M18" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K18</f>
@@ -15751,12 +15757,22 @@
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B19" s="26">
+        <v>45143.508333333331</v>
+      </c>
+      <c r="C19" s="11">
+        <f>(_tTankWeight46[[#This Row],[X]]-INDEX('Propane-Use-Day-5'!$B$10,1,1))*24</f>
+        <v>45.700000000011642</v>
+      </c>
+      <c r="D19" s="19">
+        <v>35.506666670000001</v>
+      </c>
       <c r="K19" s="14">
         <v>22</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>36.263935386695621</v>
+        <v>36.263968730925349</v>
       </c>
       <c r="M19" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K19</f>
@@ -15769,7 +15785,7 @@
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>36.201010555572829</v>
+        <v>36.201074107775348</v>
       </c>
       <c r="M20" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K20</f>
@@ -15782,7 +15798,7 @@
       </c>
       <c r="L21" s="15">
         <f t="shared" si="0"/>
-        <v>36.138085724450036</v>
+        <v>36.138179484625354</v>
       </c>
       <c r="M21" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K21</f>
@@ -15795,7 +15811,7 @@
       </c>
       <c r="L22" s="15">
         <f t="shared" si="0"/>
-        <v>36.075160893327244</v>
+        <v>36.07528486147536</v>
       </c>
       <c r="M22" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K22</f>
@@ -15808,7 +15824,7 @@
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>36.012236062204451</v>
+        <v>36.012390238325359</v>
       </c>
       <c r="M23" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K23</f>
@@ -15816,15 +15832,12 @@
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="E24">
-        <v>35.54</v>
-      </c>
       <c r="K24" s="14">
         <v>32</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>35.949311231081666</v>
+        <v>35.949495615175366</v>
       </c>
       <c r="M24" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K24</f>
@@ -15832,15 +15845,12 @@
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="E25">
-        <v>35.590000000000003</v>
-      </c>
       <c r="K25" s="14">
         <v>34</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="0"/>
-        <v>35.886386399958873</v>
+        <v>35.886600992025372</v>
       </c>
       <c r="M25" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K25</f>
@@ -15848,15 +15858,12 @@
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="E26">
-        <v>35.6</v>
-      </c>
       <c r="K26" s="14">
         <v>36</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="0"/>
-        <v>35.82346156883608</v>
+        <v>35.823706368875371</v>
       </c>
       <c r="M26" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K26</f>
@@ -15869,7 +15876,7 @@
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
-        <v>35.760536737713288</v>
+        <v>35.760811745725377</v>
       </c>
       <c r="M27" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K27</f>
@@ -15882,7 +15889,7 @@
       </c>
       <c r="L28" s="15">
         <f t="shared" si="0"/>
-        <v>35.697611906590502</v>
+        <v>35.697917122575383</v>
       </c>
       <c r="M28" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K28</f>
@@ -15895,7 +15902,7 @@
       </c>
       <c r="L29" s="15">
         <f t="shared" si="0"/>
-        <v>35.63468707546771</v>
+        <v>35.635022499425382</v>
       </c>
       <c r="M29" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K29</f>
@@ -15905,14 +15912,14 @@
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G30" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
-        <v>Measured Propane Burn Rate = 0.76 lbs/day</v>
+        <v>Measured Propane Burn Rate = 0.75 lbs/day</v>
       </c>
       <c r="K30" s="14">
         <v>44</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="0"/>
-        <v>35.571762244344917</v>
+        <v>35.572127876275388</v>
       </c>
       <c r="M30" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K30</f>
@@ -15925,7 +15932,7 @@
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
-        <v>35.508837413222125</v>
+        <v>35.509233253125394</v>
       </c>
       <c r="M31" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K31</f>
@@ -15938,7 +15945,7 @@
       </c>
       <c r="L32" s="15">
         <f t="shared" ref="L32" si="1">_nInt+_nSlope*K32</f>
-        <v>35.445912582099339</v>
+        <v>35.446338629975394</v>
       </c>
       <c r="M32" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K32</f>
@@ -15951,7 +15958,7 @@
       </c>
       <c r="L33" s="15">
         <f t="shared" ref="L33" si="2">_nInt+_nSlope*K33</f>
-        <v>35.382987750976547</v>
+        <v>35.3834440068254</v>
       </c>
       <c r="M33" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K33</f>
@@ -15964,7 +15971,7 @@
       </c>
       <c r="L34" s="15">
         <f t="shared" ref="L34" si="3">_nInt+_nSlope*K34</f>
-        <v>35.320062919853754</v>
+        <v>35.320549383675406</v>
       </c>
       <c r="M34" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K34</f>
@@ -16011,7 +16018,7 @@
       </c>
       <c r="H40" s="6">
         <f>H39/ABS(G12)</f>
-        <v>22.513634782780688</v>
+        <v>22.524447968916007</v>
       </c>
       <c r="I40" s="16" t="s">
         <v>21</v>

</xml_diff>

<commit_message>
Added another day of data.
I clearly need to break the data down by day. The slope is varying too much every day to make a decent line.
</commit_message>
<xml_diff>
--- a/MosquitoMagnetFuelFlow.xlsx
+++ b/MosquitoMagnetFuelFlow.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://starkeyhearingtechnologies-my.sharepoint.com/personal/mark_biegert_starkey_com/Documents/Desktop/Toss/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="8_{3CC4EE32-2340-4791-9D05-F9275162F980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="24" documentId="8_{3CC4EE32-2340-4791-9D05-F9275162F980}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{3D214733-F16B-42B2-BBAF-7096CAF8786D}"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="360" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="4" xr2:uid="{AD5FE48E-9CE6-4EDE-8F69-E8FD3B4EAF42}"/>
   </bookViews>
   <sheets>
     <sheet name="Propane-Use-Day-1" sheetId="1" r:id="rId1"/>
@@ -761,7 +761,7 @@
     <cellStyle name="Title" xfId="1" builtinId="15" hidden="1"/>
     <cellStyle name="Total" xfId="6" builtinId="25" customBuiltin="1"/>
   </cellStyles>
-  <dxfs count="37">
+  <dxfs count="38">
     <dxf>
       <numFmt numFmtId="164" formatCode="0.00;\-0.00;0.00;@"/>
       <border diagonalUp="0" diagonalDown="0" outline="0">
@@ -825,6 +825,13 @@
         </vertical>
         <horizontal/>
       </border>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFDF5E9"/>
+        </patternFill>
+      </fill>
     </dxf>
     <dxf>
       <fill>
@@ -1224,13 +1231,13 @@
   </dxfs>
   <tableStyles count="1" defaultTableStyle="Biegert Table Standard" defaultPivotStyle="PivotStyleLight16">
     <tableStyle name="Biegert Table Standard" pivot="0" count="7" xr9:uid="{95B43237-2845-4068-A415-A5A3E7804959}">
-      <tableStyleElement type="wholeTable" dxfId="36"/>
-      <tableStyleElement type="headerRow" dxfId="35"/>
-      <tableStyleElement type="totalRow" dxfId="34"/>
-      <tableStyleElement type="firstColumn" dxfId="33"/>
-      <tableStyleElement type="lastColumn" dxfId="32"/>
-      <tableStyleElement type="firstRowStripe" dxfId="31"/>
-      <tableStyleElement type="firstColumnStripe" dxfId="30"/>
+      <tableStyleElement type="wholeTable" dxfId="37"/>
+      <tableStyleElement type="headerRow" dxfId="36"/>
+      <tableStyleElement type="totalRow" dxfId="35"/>
+      <tableStyleElement type="firstColumn" dxfId="34"/>
+      <tableStyleElement type="lastColumn" dxfId="33"/>
+      <tableStyleElement type="firstRowStripe" dxfId="32"/>
+      <tableStyleElement type="firstColumnStripe" dxfId="31"/>
     </tableStyle>
   </tableStyles>
   <colors>
@@ -5628,10 +5635,10 @@
           </c:marker>
           <c:xVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-5'!$C$10:$C$20</c:f>
+              <c:f>'Propane-Use-Day-5'!$C$10:$C$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>0</c:v>
                 </c:pt>
@@ -5664,16 +5671,25 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>137.56666666665114</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>138.21666666667443</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>143.93333333346527</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>161.08333333331393</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
           </c:xVal>
           <c:yVal>
             <c:numRef>
-              <c:f>'Propane-Use-Day-5'!$D$10:$D$20</c:f>
+              <c:f>'Propane-Use-Day-5'!$D$10:$D$23</c:f>
               <c:numCache>
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
-                <c:ptCount val="11"/>
+                <c:ptCount val="14"/>
                 <c:pt idx="0">
                   <c:v>36.9</c:v>
                 </c:pt>
@@ -5706,6 +5722,15 @@
                 </c:pt>
                 <c:pt idx="10">
                   <c:v>32.9</c:v>
+                </c:pt>
+                <c:pt idx="11">
+                  <c:v>32.92</c:v>
+                </c:pt>
+                <c:pt idx="12">
+                  <c:v>32.733333330000001</c:v>
+                </c:pt>
+                <c:pt idx="13">
+                  <c:v>32.24</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5745,82 +5770,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>66</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>72</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>78</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>96</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>102</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>108</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>114</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>120</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>126</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>132</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>138</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>144</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>156</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5832,85 +5857,85 @@
                 <c:formatCode>0.00;\-0.00;0.00;@</c:formatCode>
                 <c:ptCount val="27"/>
                 <c:pt idx="0">
-                  <c:v>36.959428896778562</c:v>
+                  <c:v>36.883956817376706</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.76968225101195</c:v>
+                  <c:v>36.652819681230028</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.579935605245339</c:v>
+                  <c:v>36.421682545083343</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.390188959478735</c:v>
+                  <c:v>36.190545408936664</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.200442313712124</c:v>
+                  <c:v>35.959408272789979</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>36.010695667945512</c:v>
+                  <c:v>35.728271136643301</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.820949022178901</c:v>
+                  <c:v>35.497134000496622</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.631202376412297</c:v>
+                  <c:v>35.265996864349937</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.441455730645686</c:v>
+                  <c:v>35.034859728203259</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.251709084879074</c:v>
+                  <c:v>34.80372259205658</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>35.061962439112463</c:v>
+                  <c:v>34.572585455909895</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.872215793345859</c:v>
+                  <c:v>34.341448319763217</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.682469147579248</c:v>
+                  <c:v>34.110311183616531</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.492722501812636</c:v>
+                  <c:v>33.879174047469853</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.302975856046025</c:v>
+                  <c:v>33.648036911323175</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>34.113229210279414</c:v>
+                  <c:v>33.416899775176489</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.92348256451281</c:v>
+                  <c:v>33.185762639029811</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33.733735918746198</c:v>
+                  <c:v>32.954625502883133</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33.543989272979587</c:v>
+                  <c:v>32.723488366736447</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33.354242627212976</c:v>
+                  <c:v>32.492351230589769</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>33.164495981446365</c:v>
+                  <c:v>32.261214094443083</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>32.974749335679761</c:v>
+                  <c:v>32.030076958296405</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.785002689913149</c:v>
+                  <c:v>31.798939822149723</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>32.595256044146538</c:v>
+                  <c:v>31.567802686003041</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>32.405509398379927</c:v>
+                  <c:v>31.336665549856363</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>32.215762752613323</c:v>
+                  <c:v>31.105528413709681</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>32.026016106846711</c:v>
+                  <c:v>30.874391277562999</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -5950,82 +5975,82 @@
                   <c:v>0</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>6</c:v>
+                  <c:v>8</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>12</c:v>
+                  <c:v>16</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>18</c:v>
+                  <c:v>24</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>24</c:v>
+                  <c:v>32</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>30</c:v>
+                  <c:v>40</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>36</c:v>
+                  <c:v>48</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>42</c:v>
+                  <c:v>56</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>48</c:v>
+                  <c:v>64</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>54</c:v>
+                  <c:v>72</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>60</c:v>
+                  <c:v>80</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>66</c:v>
+                  <c:v>88</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>72</c:v>
+                  <c:v>96</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>78</c:v>
+                  <c:v>104</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>84</c:v>
+                  <c:v>112</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>90</c:v>
+                  <c:v>120</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>96</c:v>
+                  <c:v>128</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>102</c:v>
+                  <c:v>136</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>108</c:v>
+                  <c:v>144</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>114</c:v>
+                  <c:v>152</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>120</c:v>
+                  <c:v>160</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>126</c:v>
+                  <c:v>168</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>132</c:v>
+                  <c:v>176</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>138</c:v>
+                  <c:v>184</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>144</c:v>
+                  <c:v>192</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>150</c:v>
+                  <c:v>200</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>156</c:v>
+                  <c:v>208</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6040,82 +6065,82 @@
                   <c:v>36.9</c:v>
                 </c:pt>
                 <c:pt idx="1">
-                  <c:v>36.69761904761905</c:v>
+                  <c:v>36.630158730158726</c:v>
                 </c:pt>
                 <c:pt idx="2">
-                  <c:v>36.495238095238093</c:v>
+                  <c:v>36.360317460317461</c:v>
                 </c:pt>
                 <c:pt idx="3">
-                  <c:v>36.292857142857144</c:v>
+                  <c:v>36.090476190476188</c:v>
                 </c:pt>
                 <c:pt idx="4">
-                  <c:v>36.090476190476188</c:v>
+                  <c:v>35.820634920634916</c:v>
                 </c:pt>
                 <c:pt idx="5">
-                  <c:v>35.888095238095239</c:v>
+                  <c:v>35.550793650793651</c:v>
                 </c:pt>
                 <c:pt idx="6">
-                  <c:v>35.685714285714283</c:v>
+                  <c:v>35.280952380952378</c:v>
                 </c:pt>
                 <c:pt idx="7">
-                  <c:v>35.483333333333334</c:v>
+                  <c:v>35.011111111111113</c:v>
                 </c:pt>
                 <c:pt idx="8">
-                  <c:v>35.280952380952378</c:v>
+                  <c:v>34.74126984126984</c:v>
                 </c:pt>
                 <c:pt idx="9">
-                  <c:v>35.078571428571429</c:v>
+                  <c:v>34.471428571428568</c:v>
                 </c:pt>
                 <c:pt idx="10">
-                  <c:v>34.876190476190473</c:v>
+                  <c:v>34.201587301587303</c:v>
                 </c:pt>
                 <c:pt idx="11">
-                  <c:v>34.673809523809524</c:v>
+                  <c:v>33.93174603174603</c:v>
                 </c:pt>
                 <c:pt idx="12">
-                  <c:v>34.471428571428568</c:v>
+                  <c:v>33.661904761904758</c:v>
                 </c:pt>
                 <c:pt idx="13">
-                  <c:v>34.269047619047619</c:v>
+                  <c:v>33.392063492063492</c:v>
                 </c:pt>
                 <c:pt idx="14">
-                  <c:v>34.066666666666663</c:v>
+                  <c:v>33.12222222222222</c:v>
                 </c:pt>
                 <c:pt idx="15">
-                  <c:v>33.864285714285714</c:v>
+                  <c:v>32.852380952380955</c:v>
                 </c:pt>
                 <c:pt idx="16">
-                  <c:v>33.661904761904758</c:v>
+                  <c:v>32.582539682539682</c:v>
                 </c:pt>
                 <c:pt idx="17">
-                  <c:v>33.459523809523809</c:v>
+                  <c:v>32.31269841269841</c:v>
                 </c:pt>
                 <c:pt idx="18">
-                  <c:v>33.257142857142853</c:v>
+                  <c:v>32.042857142857144</c:v>
                 </c:pt>
                 <c:pt idx="19">
-                  <c:v>33.054761904761904</c:v>
+                  <c:v>31.773015873015872</c:v>
                 </c:pt>
                 <c:pt idx="20">
-                  <c:v>32.852380952380955</c:v>
+                  <c:v>31.503174603174603</c:v>
                 </c:pt>
                 <c:pt idx="21">
-                  <c:v>32.65</c:v>
+                  <c:v>31.233333333333334</c:v>
                 </c:pt>
                 <c:pt idx="22">
-                  <c:v>32.447619047619042</c:v>
+                  <c:v>30.963492063492062</c:v>
                 </c:pt>
                 <c:pt idx="23">
-                  <c:v>32.245238095238093</c:v>
+                  <c:v>30.693650793650793</c:v>
                 </c:pt>
                 <c:pt idx="24">
-                  <c:v>32.042857142857144</c:v>
+                  <c:v>30.423809523809524</c:v>
                 </c:pt>
                 <c:pt idx="25">
-                  <c:v>31.840476190476188</c:v>
+                  <c:v>30.153968253968252</c:v>
                 </c:pt>
                 <c:pt idx="26">
-                  <c:v>31.638095238095236</c:v>
+                  <c:v>29.884126984126983</c:v>
                 </c:pt>
               </c:numCache>
             </c:numRef>
@@ -6142,7 +6167,7 @@
         <c:axId val="1689859120"/>
         <c:scaling>
           <c:orientation val="minMax"/>
-          <c:max val="150"/>
+          <c:max val="170"/>
           <c:min val="0"/>
         </c:scaling>
         <c:delete val="0"/>
@@ -12143,7 +12168,7 @@
                 <a:latin typeface="Consolas"/>
               </a:rPr>
               <a:pPr/>
-              <a:t>Measured Propane Burn Rate = 0.76 lbs/day</a:t>
+              <a:t>Measured Propane Burn Rate = 0.69 lbs/day</a:t>
             </a:fld>
             <a:endParaRPr lang="en-US" sz="1100" b="1"/>
           </a:p>
@@ -12267,64 +12292,64 @@
 </file>
 
 <file path=xl/tables/table1.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="28" tableBorderDxfId="27">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="2" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}" name="_tTankWeight" displayName="_tTankWeight" ref="B7:D22" totalsRowShown="0" headerRowDxfId="29" tableBorderDxfId="28">
   <autoFilter ref="B7:D22" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="26"/>
-    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="25">
+    <tableColumn id="1" xr3:uid="{50A0F3A2-E162-46C4-837A-DC05922AAF3E}" name="X" dataDxfId="27"/>
+    <tableColumn id="2" xr3:uid="{B53705B3-471E-46FE-A5FC-E295D297C414}" name="Time (hours)" dataDxfId="26">
       <calculatedColumnFormula>(_tTankWeight[[#This Row],[X]]-INDEX($B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="24"/>
+    <tableColumn id="3" xr3:uid="{B3B5534E-647A-4915-9C71-7D67E3F5C2DA}" name="Weight (lbs)" dataDxfId="25"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table2.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="22" tableBorderDxfId="21">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="1" xr:uid="{09DD156C-AFEA-438B-95DD-0AB1A1F1719C}" name="_tTankWeight2" displayName="_tTankWeight2" ref="B7:D18" totalsRowShown="0" headerRowDxfId="23" tableBorderDxfId="22">
   <autoFilter ref="B7:D18" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="20"/>
-    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="19">
+    <tableColumn id="1" xr3:uid="{9E925115-B54F-4B4C-AF74-BCDF7C7A568F}" name="X" dataDxfId="21"/>
+    <tableColumn id="2" xr3:uid="{496E99EF-94CF-4D0A-B048-1B2C0AE9F694}" name="Time (hours)" dataDxfId="20">
       <calculatedColumnFormula>(_tTankWeight2[[#This Row],[X]]-INDEX('Propane-Use-Day-2'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="18"/>
+    <tableColumn id="3" xr3:uid="{ECD2A7D4-374E-475D-AFEC-98EEA0B9C174}" name="Weight (lbs)" dataDxfId="19"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table3.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D15" totalsRowShown="0" headerRowDxfId="16" tableBorderDxfId="15">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="3" xr:uid="{DA0C3822-A090-49DA-BB24-C1136312D490}" name="_tTankWeight24" displayName="_tTankWeight24" ref="B7:D15" totalsRowShown="0" headerRowDxfId="17" tableBorderDxfId="16">
   <autoFilter ref="B7:D15" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="14"/>
-    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="13">
+    <tableColumn id="1" xr3:uid="{97B1BA55-1722-4D93-BB88-758CE5343A2A}" name="X" dataDxfId="15"/>
+    <tableColumn id="2" xr3:uid="{4D171C35-268F-4B9D-80C9-888D0938537F}" name="Time (hours)" dataDxfId="14">
       <calculatedColumnFormula>(_tTankWeight24[[#This Row],[X]]-INDEX('Propane-Use-Day-3'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="12"/>
+    <tableColumn id="3" xr3:uid="{4D7DC68D-F1A9-4E70-A339-66AB49B8ACA6}" name="Weight (lbs)" dataDxfId="13"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table4.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F9E77B6-A77B-4862-A8B3-E12969205598}" name="_tTankWeight4" displayName="_tTankWeight4" ref="B7:D15" totalsRowShown="0" headerRowDxfId="10" tableBorderDxfId="9">
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="4" xr:uid="{6F9E77B6-A77B-4862-A8B3-E12969205598}" name="_tTankWeight4" displayName="_tTankWeight4" ref="B7:D15" totalsRowShown="0" headerRowDxfId="11" tableBorderDxfId="10">
   <autoFilter ref="B7:D15" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
-    <tableColumn id="1" xr3:uid="{3B43DB70-94E1-459B-8FB3-761B425FC480}" name="X" dataDxfId="8"/>
-    <tableColumn id="2" xr3:uid="{182F14ED-38CE-440A-A952-5B718E8962E5}" name="Time (hours)" dataDxfId="7">
+    <tableColumn id="1" xr3:uid="{3B43DB70-94E1-459B-8FB3-761B425FC480}" name="X" dataDxfId="9"/>
+    <tableColumn id="2" xr3:uid="{182F14ED-38CE-440A-A952-5B718E8962E5}" name="Time (hours)" dataDxfId="8">
       <calculatedColumnFormula>(_tTankWeight4[[#This Row],[X]]-INDEX('Propane-Use-Day-4'!$B$8,1,1))*24</calculatedColumnFormula>
     </tableColumn>
-    <tableColumn id="3" xr3:uid="{CAF6B0C6-7671-4815-AA0F-C7EC06E66BB3}" name="Weight (lbs)" dataDxfId="6"/>
+    <tableColumn id="3" xr3:uid="{CAF6B0C6-7671-4815-AA0F-C7EC06E66BB3}" name="Weight (lbs)" dataDxfId="7"/>
   </tableColumns>
   <tableStyleInfo name="Biegert Table Standard" showFirstColumn="0" showLastColumn="0" showRowStripes="1" showColumnStripes="0"/>
 </table>
 </file>
 
 <file path=xl/tables/table5.xml><?xml version="1.0" encoding="utf-8"?>
-<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C2640CD-FE65-4A9C-96E2-4EB4B7A88B35}" name="_tTankWeight46" displayName="_tTankWeight46" ref="B9:D20" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
-  <autoFilter ref="B9:D20" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
+<table xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="xr xr3" id="5" xr:uid="{5C2640CD-FE65-4A9C-96E2-4EB4B7A88B35}" name="_tTankWeight46" displayName="_tTankWeight46" ref="B9:D23" totalsRowShown="0" headerRowDxfId="4" tableBorderDxfId="3">
+  <autoFilter ref="B9:D23" xr:uid="{54D38F27-53A3-4E24-9E84-90EF95A9A65D}"/>
   <tableColumns count="3">
     <tableColumn id="1" xr3:uid="{5E8842F1-EA49-43DF-A3E1-1B5CC76346AB}" name="X" dataDxfId="2"/>
     <tableColumn id="2" xr3:uid="{36D8FF9C-5836-47BE-A23B-22C78B1E531D}" name="Time (hours)" dataDxfId="1">
@@ -13085,7 +13110,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:L32">
-    <cfRule type="expression" dxfId="29" priority="1">
+    <cfRule type="expression" dxfId="30" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -13825,7 +13850,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M37 L38:M38">
-    <cfRule type="expression" dxfId="23" priority="1">
+    <cfRule type="expression" dxfId="24" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -14493,7 +14518,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M31">
-    <cfRule type="expression" dxfId="17" priority="1">
+    <cfRule type="expression" dxfId="18" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15365,7 +15390,7 @@
     </row>
   </sheetData>
   <conditionalFormatting sqref="K8:M31 L32:M34">
-    <cfRule type="expression" dxfId="11" priority="1">
+    <cfRule type="expression" dxfId="12" priority="1">
       <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
@@ -15383,8 +15408,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:xdr="http://schemas.openxmlformats.org/drawingml/2006/spreadsheetDrawing" xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{1512FE03-6F96-4002-83C1-8201B1986D54}">
   <dimension ref="A1:P71"/>
   <sheetViews>
-    <sheetView showGridLines="0" tabSelected="1" workbookViewId="0">
-      <selection activeCell="R4" sqref="R4"/>
+    <sheetView showGridLines="0" tabSelected="1" topLeftCell="A25" workbookViewId="0">
+      <selection activeCell="B31" sqref="B31"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="12.75" x14ac:dyDescent="0.2"/>
@@ -15481,18 +15506,18 @@
     <row r="8" spans="1:13" ht="13.5" thickTop="1" x14ac:dyDescent="0.2">
       <c r="G8" s="17" cm="1">
         <f t="array" ref="G8:H8">LINEST(_xlfn.DROP(_xlfn.DROP(_tTankWeight46[Weight (lbs)],2),-1),_xlfn.DROP(_xlfn.DROP(_tTankWeight46[Time (hours)],2),-1))</f>
-        <v>-3.1624440961101612E-2</v>
+        <v>-2.8892142018335128E-2</v>
       </c>
       <c r="H8" s="17">
-        <v>36.959428896778562</v>
+        <v>36.883956817376706</v>
       </c>
       <c r="K8" s="14" cm="1">
-        <f t="array" ref="K8:K34">_xlfn.SEQUENCE(27,1,0,6)</f>
+        <f t="array" ref="K8:K34">_xlfn.SEQUENCE(27,1,0,8)</f>
         <v>0</v>
       </c>
       <c r="L8" s="15">
         <f>_nInt+_nSlope*K8</f>
-        <v>36.959428896778562</v>
+        <v>36.883956817376706</v>
       </c>
       <c r="M8" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K8</f>
@@ -15519,15 +15544,15 @@
         <v>19</v>
       </c>
       <c r="K9" s="14">
-        <v>6</v>
+        <v>8</v>
       </c>
       <c r="L9" s="15">
         <f t="shared" ref="L9:L31" si="0">_nInt+_nSlope*K9</f>
-        <v>36.76968225101195</v>
+        <v>36.652819681230028</v>
       </c>
       <c r="M9" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K9</f>
-        <v>36.69761904761905</v>
+        <v>36.630158730158726</v>
       </c>
     </row>
     <row r="10" spans="1:13" x14ac:dyDescent="0.2">
@@ -15542,15 +15567,15 @@
         <v>36.9</v>
       </c>
       <c r="K10" s="14">
-        <v>12</v>
+        <v>16</v>
       </c>
       <c r="L10" s="15">
         <f t="shared" si="0"/>
-        <v>36.579935605245339</v>
+        <v>36.421682545083343</v>
       </c>
       <c r="M10" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K10</f>
-        <v>36.495238095238093</v>
+        <v>36.360317460317461</v>
       </c>
     </row>
     <row r="11" spans="1:13" x14ac:dyDescent="0.2">
@@ -15568,15 +15593,15 @@
         <v>17</v>
       </c>
       <c r="K11" s="14">
-        <v>18</v>
+        <v>24</v>
       </c>
       <c r="L11" s="15">
         <f t="shared" si="0"/>
-        <v>36.390188959478735</v>
+        <v>36.190545408936664</v>
       </c>
       <c r="M11" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K11</f>
-        <v>36.292857142857144</v>
+        <v>36.090476190476188</v>
       </c>
     </row>
     <row r="12" spans="1:13" x14ac:dyDescent="0.2">
@@ -15592,7 +15617,7 @@
       </c>
       <c r="G12" s="22">
         <f>ABS(24*_nSlope)</f>
-        <v>0.75898658306643862</v>
+        <v>0.69341140844004312</v>
       </c>
       <c r="H12" t="s">
         <v>22</v>
@@ -15602,15 +15627,15 @@
         <v>=ABS(24*_nSlope)</v>
       </c>
       <c r="K12" s="14">
-        <v>24</v>
+        <v>32</v>
       </c>
       <c r="L12" s="15">
         <f t="shared" si="0"/>
-        <v>36.200442313712124</v>
+        <v>35.959408272789979</v>
       </c>
       <c r="M12" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K12</f>
-        <v>36.090476190476188</v>
+        <v>35.820634920634916</v>
       </c>
     </row>
     <row r="13" spans="1:13" x14ac:dyDescent="0.2">
@@ -15625,15 +15650,15 @@
         <v>36.416666669999998</v>
       </c>
       <c r="K13" s="14">
-        <v>30</v>
+        <v>40</v>
       </c>
       <c r="L13" s="15">
         <f t="shared" si="0"/>
-        <v>36.010695667945512</v>
+        <v>35.728271136643301</v>
       </c>
       <c r="M13" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K13</f>
-        <v>35.888095238095239</v>
+        <v>35.550793650793651</v>
       </c>
     </row>
     <row r="14" spans="1:13" x14ac:dyDescent="0.2">
@@ -15648,15 +15673,15 @@
         <v>36.31</v>
       </c>
       <c r="K14" s="14">
-        <v>36</v>
+        <v>48</v>
       </c>
       <c r="L14" s="15">
         <f t="shared" si="0"/>
-        <v>35.820949022178901</v>
+        <v>35.497134000496622</v>
       </c>
       <c r="M14" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K14</f>
-        <v>35.685714285714283</v>
+        <v>35.280952380952378</v>
       </c>
     </row>
     <row r="15" spans="1:13" x14ac:dyDescent="0.2">
@@ -15674,15 +15699,15 @@
         <v>34</v>
       </c>
       <c r="K15" s="14">
-        <v>42</v>
+        <v>56</v>
       </c>
       <c r="L15" s="15">
         <f t="shared" si="0"/>
-        <v>35.631202376412297</v>
+        <v>35.265996864349937</v>
       </c>
       <c r="M15" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K15</f>
-        <v>35.483333333333334</v>
+        <v>35.011111111111113</v>
       </c>
     </row>
     <row r="16" spans="1:13" x14ac:dyDescent="0.2">
@@ -15704,15 +15729,15 @@
         <v>22</v>
       </c>
       <c r="K16" s="14">
-        <v>48</v>
+        <v>64</v>
       </c>
       <c r="L16" s="15">
         <f t="shared" si="0"/>
-        <v>35.441455730645686</v>
+        <v>35.034859728203259</v>
       </c>
       <c r="M16" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K16</f>
-        <v>35.280952380952378</v>
+        <v>34.74126984126984</v>
       </c>
     </row>
     <row r="17" spans="2:13" x14ac:dyDescent="0.2">
@@ -15728,15 +15753,15 @@
       </c>
       <c r="G17" s="22"/>
       <c r="K17" s="14">
-        <v>54</v>
+        <v>72</v>
       </c>
       <c r="L17" s="15">
         <f t="shared" si="0"/>
-        <v>35.251709084879074</v>
+        <v>34.80372259205658</v>
       </c>
       <c r="M17" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K17</f>
-        <v>35.078571428571429</v>
+        <v>34.471428571428568</v>
       </c>
     </row>
     <row r="18" spans="2:13" x14ac:dyDescent="0.2">
@@ -15751,15 +15776,15 @@
         <v>35.576666670000002</v>
       </c>
       <c r="K18" s="14">
-        <v>60</v>
+        <v>80</v>
       </c>
       <c r="L18" s="15">
         <f t="shared" si="0"/>
-        <v>35.061962439112463</v>
+        <v>34.572585455909895</v>
       </c>
       <c r="M18" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K18</f>
-        <v>34.876190476190473</v>
+        <v>34.201587301587303</v>
       </c>
     </row>
     <row r="19" spans="2:13" x14ac:dyDescent="0.2">
@@ -15774,15 +15799,15 @@
         <v>35.506666670000001</v>
       </c>
       <c r="K19" s="14">
-        <v>66</v>
+        <v>88</v>
       </c>
       <c r="L19" s="15">
         <f t="shared" si="0"/>
-        <v>34.872215793345859</v>
+        <v>34.341448319763217</v>
       </c>
       <c r="M19" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K19</f>
-        <v>34.673809523809524</v>
+        <v>33.93174603174603</v>
       </c>
     </row>
     <row r="20" spans="2:13" x14ac:dyDescent="0.2">
@@ -15797,214 +15822,231 @@
         <v>32.9</v>
       </c>
       <c r="K20" s="14">
-        <v>72</v>
+        <v>96</v>
       </c>
       <c r="L20" s="15">
         <f t="shared" si="0"/>
-        <v>34.682469147579248</v>
+        <v>34.110311183616531</v>
       </c>
       <c r="M20" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K20</f>
-        <v>34.471428571428568</v>
+        <v>33.661904761904758</v>
       </c>
     </row>
     <row r="21" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B21" s="26">
+        <v>45147.363194444442</v>
+      </c>
+      <c r="C21" s="11">
+        <f>(_tTankWeight46[[#This Row],[X]]-INDEX('Propane-Use-Day-5'!$B$10,1,1))*24</f>
+        <v>138.21666666667443</v>
+      </c>
+      <c r="D21" s="19">
+        <v>32.92</v>
+      </c>
       <c r="K21" s="14">
-        <v>78</v>
+        <v>104</v>
       </c>
       <c r="L21" s="15">
         <f t="shared" si="0"/>
-        <v>34.492722501812636</v>
+        <v>33.879174047469853</v>
       </c>
       <c r="M21" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K21</f>
-        <v>34.269047619047619</v>
+        <v>33.392063492063492</v>
       </c>
     </row>
     <row r="22" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B22" s="26">
+        <v>45147.601388888892</v>
+      </c>
+      <c r="C22" s="11">
+        <f>(_tTankWeight46[[#This Row],[X]]-INDEX('Propane-Use-Day-5'!$B$10,1,1))*24</f>
+        <v>143.93333333346527</v>
+      </c>
+      <c r="D22" s="19">
+        <v>32.733333330000001</v>
+      </c>
       <c r="K22" s="14">
-        <v>84</v>
+        <v>112</v>
       </c>
       <c r="L22" s="15">
         <f t="shared" si="0"/>
-        <v>34.302975856046025</v>
+        <v>33.648036911323175</v>
       </c>
       <c r="M22" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K22</f>
-        <v>34.066666666666663</v>
+        <v>33.12222222222222</v>
       </c>
     </row>
     <row r="23" spans="2:13" x14ac:dyDescent="0.2">
+      <c r="B23" s="26">
+        <v>45148.315972222219</v>
+      </c>
+      <c r="C23" s="11">
+        <f>(_tTankWeight46[[#This Row],[X]]-INDEX('Propane-Use-Day-5'!$B$10,1,1))*24</f>
+        <v>161.08333333331393</v>
+      </c>
+      <c r="D23" s="19">
+        <v>32.24</v>
+      </c>
       <c r="K23" s="14">
-        <v>90</v>
+        <v>120</v>
       </c>
       <c r="L23" s="15">
         <f t="shared" si="0"/>
-        <v>34.113229210279414</v>
+        <v>33.416899775176489</v>
       </c>
       <c r="M23" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K23</f>
-        <v>33.864285714285714</v>
+        <v>32.852380952380955</v>
       </c>
     </row>
     <row r="24" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K24" s="14">
-        <v>96</v>
+        <v>128</v>
       </c>
       <c r="L24" s="15">
         <f t="shared" si="0"/>
-        <v>33.92348256451281</v>
+        <v>33.185762639029811</v>
       </c>
       <c r="M24" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K24</f>
-        <v>33.661904761904758</v>
+        <v>32.582539682539682</v>
       </c>
     </row>
     <row r="25" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C25">
-        <v>32.86</v>
-      </c>
       <c r="K25" s="14">
-        <v>102</v>
+        <v>136</v>
       </c>
       <c r="L25" s="15">
         <f t="shared" si="0"/>
-        <v>33.733735918746198</v>
+        <v>32.954625502883133</v>
       </c>
       <c r="M25" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K25</f>
-        <v>33.459523809523809</v>
+        <v>32.31269841269841</v>
       </c>
     </row>
     <row r="26" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C26">
-        <v>32.94</v>
-      </c>
       <c r="K26" s="14">
-        <v>108</v>
+        <v>144</v>
       </c>
       <c r="L26" s="15">
         <f t="shared" si="0"/>
-        <v>33.543989272979587</v>
+        <v>32.723488366736447</v>
       </c>
       <c r="M26" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K26</f>
-        <v>33.257142857142853</v>
+        <v>32.042857142857144</v>
       </c>
     </row>
     <row r="27" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C27">
-        <v>32.89</v>
-      </c>
       <c r="K27" s="14">
-        <v>114</v>
+        <v>152</v>
       </c>
       <c r="L27" s="15">
         <f t="shared" si="0"/>
-        <v>33.354242627212976</v>
+        <v>32.492351230589769</v>
       </c>
       <c r="M27" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K27</f>
-        <v>33.054761904761904</v>
+        <v>31.773015873015872</v>
       </c>
     </row>
     <row r="28" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="C28">
-        <f>AVERAGE(C25:C27)</f>
-        <v>32.896666666666668</v>
-      </c>
       <c r="K28" s="14">
-        <v>120</v>
+        <v>160</v>
       </c>
       <c r="L28" s="15">
         <f t="shared" si="0"/>
-        <v>33.164495981446365</v>
+        <v>32.261214094443083</v>
       </c>
       <c r="M28" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K28</f>
-        <v>32.852380952380955</v>
+        <v>31.503174603174603</v>
       </c>
     </row>
     <row r="29" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K29" s="14">
-        <v>126</v>
+        <v>168</v>
       </c>
       <c r="L29" s="15">
         <f t="shared" si="0"/>
-        <v>32.974749335679761</v>
+        <v>32.030076958296405</v>
       </c>
       <c r="M29" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K29</f>
-        <v>32.65</v>
+        <v>31.233333333333334</v>
       </c>
     </row>
     <row r="30" spans="2:13" x14ac:dyDescent="0.2">
       <c r="G30" t="str">
         <f>"Measured Propane Burn Rate = "&amp;TEXT($G$12,"0.00")&amp;" lbs/day"</f>
-        <v>Measured Propane Burn Rate = 0.76 lbs/day</v>
+        <v>Measured Propane Burn Rate = 0.69 lbs/day</v>
       </c>
       <c r="K30" s="14">
-        <v>132</v>
+        <v>176</v>
       </c>
       <c r="L30" s="15">
         <f t="shared" si="0"/>
-        <v>32.785002689913149</v>
+        <v>31.798939822149723</v>
       </c>
       <c r="M30" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K30</f>
-        <v>32.447619047619042</v>
+        <v>30.963492063492062</v>
       </c>
     </row>
     <row r="31" spans="2:13" x14ac:dyDescent="0.2">
       <c r="K31" s="14">
-        <v>138</v>
+        <v>184</v>
       </c>
       <c r="L31" s="15">
         <f t="shared" si="0"/>
-        <v>32.595256044146538</v>
+        <v>31.567802686003041</v>
       </c>
       <c r="M31" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K31</f>
-        <v>32.245238095238093</v>
+        <v>30.693650793650793</v>
       </c>
     </row>
     <row r="32" spans="2:13" x14ac:dyDescent="0.2">
-      <c r="K32">
-        <v>144</v>
+      <c r="K32" s="14">
+        <v>192</v>
       </c>
       <c r="L32" s="15">
         <f t="shared" ref="L32" si="1">_nInt+_nSlope*K32</f>
-        <v>32.405509398379927</v>
+        <v>31.336665549856363</v>
       </c>
       <c r="M32" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K32</f>
-        <v>32.042857142857144</v>
+        <v>30.423809523809524</v>
       </c>
     </row>
     <row r="33" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K33">
-        <v>150</v>
+      <c r="K33" s="14">
+        <v>200</v>
       </c>
       <c r="L33" s="15">
         <f t="shared" ref="L33" si="2">_nInt+_nSlope*K33</f>
-        <v>32.215762752613323</v>
+        <v>31.105528413709681</v>
       </c>
       <c r="M33" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K33</f>
-        <v>31.840476190476188</v>
+        <v>30.153968253968252</v>
       </c>
     </row>
     <row r="34" spans="1:13" x14ac:dyDescent="0.2">
-      <c r="K34">
-        <v>156</v>
+      <c r="K34" s="14">
+        <v>208</v>
       </c>
       <c r="L34" s="15">
         <f t="shared" ref="L34" si="3">_nInt+_nSlope*K34</f>
-        <v>32.026016106846711</v>
+        <v>30.874391277562999</v>
       </c>
       <c r="M34" s="15">
         <f>INDEX(_tTankWeight46[Weight (lbs)],1,1)-$G$16/24*K34</f>
-        <v>31.638095238095236</v>
+        <v>29.884126984126983</v>
       </c>
     </row>
     <row r="35" spans="1:13" x14ac:dyDescent="0.2">
@@ -16047,7 +16089,7 @@
       </c>
       <c r="H40" s="6">
         <f>H39/ABS(G12)</f>
-        <v>22.398287900317058</v>
+        <v>24.516470010559296</v>
       </c>
       <c r="I40" s="16" t="s">
         <v>21</v>
@@ -16368,9 +16410,14 @@
       </c>
     </row>
   </sheetData>
-  <conditionalFormatting sqref="K8:M31 L32:M34">
+  <conditionalFormatting sqref="K8:M30 L31:M34">
+    <cfRule type="expression" dxfId="6" priority="2">
+      <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="K31:K34">
     <cfRule type="expression" dxfId="5" priority="1">
-      <formula>MOD(ROW(K8)-ROW($K$7),2)</formula>
+      <formula>MOD(ROW(K31)-ROW($K$7),2)</formula>
     </cfRule>
   </conditionalFormatting>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>

</xml_diff>